<commit_message>
update concepts for DPV, AI, EU AIAct, Risk
- AI: remove prefix AI from concepts e.g. ai:Model
- DPV Recipient: increase scope to include data and technologies
- DPV ThirdParty: broaden scope by removing personal data from definition
- DPV remove Entity Controls
- EU AIAct: parents from AI, add Market Availability and Placement statuses
- Risk: add incident concepts for Reports, Impact Assessment, Register
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ai.xlsx
+++ b/code/vocab_csv/ai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="39">
   <si>
     <t>Term</t>
   </si>
@@ -68,7 +68,7 @@
     <t>Artificial Intelligence (AI)</t>
   </si>
   <si>
-    <t>a technical and scientific field devoted to the engineered system that generates outputs such as content, forecasts, recommendations or decisions for a given set of human-defined objectives</t>
+    <t>A technical and scientific field devoted to the engineered system that generates outputs such as content, forecasts, recommendations or decisions for a given set of human-defined objectives</t>
   </si>
   <si>
     <t>dpv:Technology</t>
@@ -86,31 +86,37 @@
     <t>accepted</t>
   </si>
   <si>
-    <t>AITechnique</t>
-  </si>
-  <si>
-    <t>AI Technique</t>
+    <t>System</t>
+  </si>
+  <si>
+    <t>OECD 2024 definition: An AI system is a machine-based system that, for explicit or implicit objectives, infers, from the input it receives, how to generate outputs such as predictions, content, recommendations, or decisions that can influence physical or virtual environments. Different AI systems vary in their levels of autonomy and adaptiveness after deployment. ISO/IEC 22989:2023 definition: engineered system that generates outputs such as content, forecasts, recommendations or decisions for a given set of human-defined objectives</t>
+  </si>
+  <si>
+    <t>ai:AI</t>
+  </si>
+  <si>
+    <t>OECD, ISO/IEC 22989:2023</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Physical, mathematical or otherwise logical representation of a system, entity, phenomenon, process or data</t>
+  </si>
+  <si>
+    <t>Technique</t>
   </si>
   <si>
     <t>Techniques for using or applying AI</t>
   </si>
   <si>
-    <t>ai:AI</t>
-  </si>
-  <si>
-    <t>AICapability</t>
-  </si>
-  <si>
-    <t>AI Capability</t>
+    <t>Capability</t>
   </si>
   <si>
     <t>Capability or use of AI to achieve a technical goal or objective</t>
   </si>
   <si>
-    <t>AIRisk</t>
-  </si>
-  <si>
-    <t>AI Risk</t>
+    <t>Risk</t>
   </si>
   <si>
     <t>Risk associated with development, use, or operation of AI systems</t>
@@ -119,10 +125,7 @@
     <t>dpv:Risk</t>
   </si>
   <si>
-    <t>AIMeasure</t>
-  </si>
-  <si>
-    <t>AI Measure</t>
+    <t>Measure</t>
   </si>
   <si>
     <t>Measure to address risk associated with AI Systems</t>
@@ -167,21 +170,27 @@
       <name val="&quot;Arial&quot;"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -190,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -219,19 +228,28 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -627,6 +645,102 @@
       <c r="AC2" s="7"/>
       <c r="AD2" s="7"/>
     </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="12">
+        <v>45429.0</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="M3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="12">
+        <v>45429.0</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+    </row>
     <row r="6">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
@@ -764,16 +878,16 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
@@ -855,36 +969,36 @@
       <c r="K13" s="9"/>
     </row>
     <row r="14">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13"/>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="13"/>
-      <c r="AD14" s="13"/>
-      <c r="AE14" s="13"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="16"/>
+      <c r="AC14" s="16"/>
+      <c r="AD14" s="16"/>
+      <c r="AE14" s="16"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:AE150">
@@ -981,16 +1095,16 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
@@ -1002,7 +1116,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="K2" s="15">
+      <c r="K2" s="18">
         <v>45410.0</v>
       </c>
       <c r="L2" s="7"/>
@@ -1138,51 +1252,51 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="15">
+      <c r="J2" s="19"/>
+      <c r="K2" s="18">
         <v>45410.0</v>
       </c>
-      <c r="L2" s="16"/>
+      <c r="L2" s="19"/>
       <c r="M2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
     </row>
     <row r="3">
       <c r="K3" s="9"/>
@@ -1297,16 +1411,16 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
@@ -1318,7 +1432,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="K2" s="15">
+      <c r="K2" s="18">
         <v>45410.0</v>
       </c>
       <c r="L2" s="7"/>

</xml_diff>

<commit_message>
fixes AI, EU-AIAct, other documentation features
- fixes in AI: see #162
- fixes in EU-AIAct: see #163
- closes #161 skos:related has concepts correctly linked to their
  vocabularies while showing a prefixed version in HTML and IRI in RDF
  webpage and urls information
- fixes #159 purposes module link is broken in DPV spec
- fixes dct:source not providing a IRI object in RDF - now uses
  schema.org to indicate source
- adds examples for purposes
- adds purpose module documentation
- examples are now associated with concepts using `vann:example` and are
  specified in the HTML page in concept term table under 'examples'
- examples are indexed and listed in the `/example` page and their IRIs
  now resolve correctly from other pages (e.g. clicking link in a
  concept term table navigates to the example contents)
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ai.xlsx
+++ b/code/vocab_csv/ai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="40">
   <si>
     <t>Term</t>
   </si>
@@ -86,7 +86,10 @@
     <t>accepted</t>
   </si>
   <si>
-    <t>System</t>
+    <t>AISystem</t>
+  </si>
+  <si>
+    <t>AI System</t>
   </si>
   <si>
     <t>OECD 2024 definition: An AI system is a machine-based system that, for explicit or implicit objectives, infers, from the input it receives, how to generate outputs such as predictions, content, recommendations, or decisions that can influence physical or virtual environments. Different AI systems vary in their levels of autonomy and adaptiveness after deployment. ISO/IEC 22989:2023 definition: engineered system that generates outputs such as content, forecasts, recommendations or decisions for a given set of human-defined objectives</t>
@@ -95,7 +98,34 @@
     <t>ai:AI</t>
   </si>
   <si>
-    <t>OECD, ISO/IEC 22989:2023</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>OECD,</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://oecd.ai/en/wonk/ai-system-definition-update</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>,ISO/IEC 22989:2023,</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://www.iso.org/standard/74296.html</t>
+    </r>
   </si>
   <si>
     <t>Model</t>
@@ -141,7 +171,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -174,6 +204,11 @@
       <name val="Arial"/>
     </font>
     <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -199,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -234,16 +269,19 @@
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -650,13 +688,13 @@
         <v>23</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>19</v>
@@ -665,10 +703,10 @@
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="12">
+      <c r="J3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="13">
         <v>45429.0</v>
       </c>
       <c r="L3" s="7"/>
@@ -695,16 +733,16 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>19</v>
@@ -716,7 +754,7 @@
       <c r="J4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="13">
         <v>45429.0</v>
       </c>
       <c r="L4" s="7"/>
@@ -804,7 +842,10 @@
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="J3"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -878,16 +919,16 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
@@ -969,36 +1010,36 @@
       <c r="K13" s="9"/>
     </row>
     <row r="14">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="16"/>
-      <c r="V14" s="16"/>
-      <c r="W14" s="16"/>
-      <c r="X14" s="16"/>
-      <c r="Y14" s="16"/>
-      <c r="Z14" s="16"/>
-      <c r="AA14" s="16"/>
-      <c r="AB14" s="16"/>
-      <c r="AC14" s="16"/>
-      <c r="AD14" s="16"/>
-      <c r="AE14" s="16"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:AE150">
@@ -1095,16 +1136,16 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
@@ -1116,7 +1157,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="K2" s="18">
+      <c r="K2" s="19">
         <v>45410.0</v>
       </c>
       <c r="L2" s="7"/>
@@ -1252,51 +1293,51 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="18">
+      <c r="J2" s="20"/>
+      <c r="K2" s="19">
         <v>45410.0</v>
       </c>
-      <c r="L2" s="19"/>
+      <c r="L2" s="20"/>
       <c r="M2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
     </row>
     <row r="3">
       <c r="K3" s="9"/>
@@ -1411,16 +1452,16 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
@@ -1432,7 +1473,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="K2" s="18">
+      <c r="K2" s="19">
         <v>45410.0</v>
       </c>
       <c r="L2" s="7"/>

</xml_diff>

<commit_message>
adds Bias concepts to RISK and AI - see #182
- adds bias taxnomy to RISK
- adds bias taxonomy (specific to AI) to AI
- contains RDF and HTML outputs

Co-authored-by: Daniel Doherty <dohertd3@tcd.ie>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ai.xlsx
+++ b/code/vocab_csv/ai.xlsx
@@ -8,6 +8,7 @@
     <sheet state="visible" name="ai-capabilities" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="ai-risks" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="ai-measures" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="ai-bias" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="101">
   <si>
     <t>Term</t>
   </si>
@@ -163,6 +164,189 @@
   <si>
     <t>dpv:RiskMitigationMeasure</t>
   </si>
+  <si>
+    <t>AI specific Biases</t>
+  </si>
+  <si>
+    <t>AIBias</t>
+  </si>
+  <si>
+    <t>AI Bias</t>
+  </si>
+  <si>
+    <t>Bias associated with development, use, or other activities involving an AI technology or system</t>
+  </si>
+  <si>
+    <t>risk:Bias</t>
+  </si>
+  <si>
+    <t>risk:RiskConcept</t>
+  </si>
+  <si>
+    <t>Daniel Doherty</t>
+  </si>
+  <si>
+    <t>AutomationBias</t>
+  </si>
+  <si>
+    <t>Automation Bias</t>
+  </si>
+  <si>
+    <t>Bias tha occurs due to propensity for humans to favour suggestions from automated decision-making systems and to ignore contradictory information made without automation, even if it is correct</t>
+  </si>
+  <si>
+    <t>risk:CognitiveBias</t>
+  </si>
+  <si>
+    <t>ISO/IEC 24027:2021</t>
+  </si>
+  <si>
+    <t>DataBias</t>
+  </si>
+  <si>
+    <t>Data Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs due to unaddressed data properties that lead to AI systems that perform better or worse for different groups</t>
+  </si>
+  <si>
+    <t>ai:AIBias</t>
+  </si>
+  <si>
+    <t>DataLabelsAndLabellingProcessBias</t>
+  </si>
+  <si>
+    <t>Data Labels And Labelling Process Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs due to the labelling process itself introducing societal or cognitive biases</t>
+  </si>
+  <si>
+    <t>ai:DataBias</t>
+  </si>
+  <si>
+    <t>NonRepresentativeSamplingBias</t>
+  </si>
+  <si>
+    <t>Non-Representative Sampling Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs if a dataset is not representative of the intended deployment environment, where the model learns biases based on the ways in which the data is non-representative</t>
+  </si>
+  <si>
+    <t>MissingFeaturesAndLabelsBias</t>
+  </si>
+  <si>
+    <t>Missing Features And Labels Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs when features are missing from individual training samples</t>
+  </si>
+  <si>
+    <t>If the frequency of missing features is higher for one group than another then this presents another vector for bias</t>
+  </si>
+  <si>
+    <t>DataAggregationBias</t>
+  </si>
+  <si>
+    <t>Data Aggregation Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs from aggregating data covering different groups of objects that might have different statistical distributions which introduce bias into the data used to train AI systems</t>
+  </si>
+  <si>
+    <t>DistributedTrainingBias</t>
+  </si>
+  <si>
+    <t>Distributed Training Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs due to distributed machine having different sources of data that do not have the same distribution of feature space</t>
+  </si>
+  <si>
+    <t>EngineeringDecisionBias</t>
+  </si>
+  <si>
+    <t>Engineering Decision Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs due to machine learning model architectures - encompassing all model specifications, parameters and manually designed features</t>
+  </si>
+  <si>
+    <t>Data bias and human cognitive bias can contribute to such bias</t>
+  </si>
+  <si>
+    <t>FeatureEngineeringBias</t>
+  </si>
+  <si>
+    <t>Feature Engineering Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs from steps such as encoding, data type conversion, dimensionality reduction and feature selection which are subject to choices made by the AI developer and introduce bias in the ML model</t>
+  </si>
+  <si>
+    <t>ai:EngineeringDecisionBias</t>
+  </si>
+  <si>
+    <t>AlgorithmSelectionBias</t>
+  </si>
+  <si>
+    <t>Algorithm Selection Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs from the selection of machine learning algorithms built into the AI system which introduce unwanted bias in predictions made by the system because the type of algorithm used introduces a variation in the performance of the ML model</t>
+  </si>
+  <si>
+    <t>HyperparameterTuningBias</t>
+  </si>
+  <si>
+    <t>Hyperparameter Tuning Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs from hyperparameters defining how the model is structured and which cannot be directly trained from the data like model parameters, where hyperparameters affect the model functioning and accuracy of the model</t>
+  </si>
+  <si>
+    <t>InformativenessBias</t>
+  </si>
+  <si>
+    <t>Informativeness Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs or some groups, the mapping between inputs present in the data and outputs are more difficult to learn and where a model that only has one feature set available, can be biased against the group whose relationships are difficult to learn from available data</t>
+  </si>
+  <si>
+    <t>This can happen when some features are highly informative about one group, while a different set of features is highly informative about another group. If this is the case, then a model that only has one feature set available, can be biased against the group whose relationships are difficult to learn from available data</t>
+  </si>
+  <si>
+    <t>ModelBias</t>
+  </si>
+  <si>
+    <t>Model Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs when ML uses functions like a maximum likelihood estimator to determine parameters, and there is data skew or under-representation present in the data, where the maximum likelihood estimation tends to amplify any underlying bias in the distribution</t>
+  </si>
+  <si>
+    <t>ModelInteractionBias</t>
+  </si>
+  <si>
+    <t>Model Interaction Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs from the structure of a model to create biased predictions</t>
+  </si>
+  <si>
+    <t>ModelExpressivenessBias</t>
+  </si>
+  <si>
+    <t>Model Expressiveness Bias</t>
+  </si>
+  <si>
+    <t>Bias that occurs from the number and nature of parameters in a model as well as the neural network topology which affect the expressiveness of the model and any feature that affects model expressiveness differently across groups</t>
+  </si>
+  <si>
+    <t>ai:ModelInteractionBias</t>
+  </si>
 </sst>
 </file>
 
@@ -171,7 +355,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -213,6 +397,16 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -234,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -294,6 +488,30 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -368,6 +586,10 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1527,4 +1749,969 @@
   </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="29.88"/>
+    <col customWidth="1" min="2" max="2" width="31.88"/>
+    <col customWidth="1" min="3" max="3" width="60.88"/>
+    <col customWidth="1" min="9" max="9" width="43.13"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="25">
+        <v>45553.0</v>
+      </c>
+      <c r="L3" s="26"/>
+      <c r="M3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="17"/>
+      <c r="AD3" s="17"/>
+      <c r="AE3" s="17"/>
+      <c r="AF3" s="17"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L4" s="26"/>
+      <c r="M4" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L5" s="26"/>
+      <c r="M5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L6" s="26"/>
+      <c r="M6" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="17"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L7" s="26"/>
+      <c r="M7" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="17"/>
+      <c r="AD7" s="17"/>
+      <c r="AE7" s="17"/>
+      <c r="AF7" s="17"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L8" s="26"/>
+      <c r="M8" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="17"/>
+      <c r="AF8" s="17"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L9" s="26"/>
+      <c r="M9" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="17"/>
+      <c r="AD9" s="17"/>
+      <c r="AE9" s="17"/>
+      <c r="AF9" s="17"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L10" s="26"/>
+      <c r="M10" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="17"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="17"/>
+      <c r="AF10" s="17"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L11" s="26"/>
+      <c r="M11" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L12" s="26"/>
+      <c r="M12" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="17"/>
+      <c r="AD12" s="17"/>
+      <c r="AE12" s="17"/>
+      <c r="AF12" s="17"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L13" s="26"/>
+      <c r="M13" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="17"/>
+      <c r="AD13" s="17"/>
+      <c r="AE13" s="17"/>
+      <c r="AF13" s="17"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L14" s="26"/>
+      <c r="M14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="17"/>
+      <c r="AF14" s="17"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L15" s="26"/>
+      <c r="M15" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="17"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L16" s="26"/>
+      <c r="M16" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
+      <c r="AF16" s="17"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L17" s="26"/>
+      <c r="M17" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
+      <c r="AE17" s="17"/>
+      <c r="AF17" s="17"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="27">
+        <v>45548.0</v>
+      </c>
+      <c r="L18" s="26"/>
+      <c r="M18" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="17"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:AF141">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$M2="accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AB117">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$M2="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AB117">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$M2="changed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:O141 A3:L141 P3:AF141">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$M2="deprecated"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update RDF for changes
- changes in dpv, tech, ai, eu-aiact, eu-gdpr, risk
- fixes incorrect IRI term in AI spreadsheets
- ai: core, capabilities, risks, techniques
- dpv: entities, entity legal roles, entity organisations, notices,
  organisational measures, processing, processing context and processing
  scale (syntactic change in references), purposes
- eu-aiact: capability, data, docs, misc concepts, sector, status
- eu-gdpr: data transfers (references), rights
- risk: core, incident status, risk controls, risk events taxonomy
- tech: core, io, provision, tools
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ai.xlsx
+++ b/code/vocab_csv/ai.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="737">
   <si>
     <t>Term</t>
   </si>
@@ -533,6 +533,9 @@
   </si>
   <si>
     <t>Encoding knowledge in a formal language</t>
+  </si>
+  <si>
+    <t>SymbolicReasoning</t>
   </si>
   <si>
     <t>Symbolic Reasoning</t>
@@ -3324,10 +3327,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -3359,23 +3362,23 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F2" s="40"/>
       <c r="G2" s="5" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H2" s="40"/>
       <c r="I2" s="8"/>
@@ -3414,23 +3417,23 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -3504,23 +3507,23 @@
     </row>
     <row r="6">
       <c r="A6" s="35" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -3558,23 +3561,23 @@
     </row>
     <row r="7">
       <c r="A7" s="26" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -3612,23 +3615,23 @@
     </row>
     <row r="8">
       <c r="A8" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>516</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>517</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>514</v>
-      </c>
       <c r="E8" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -3666,23 +3669,23 @@
     </row>
     <row r="9">
       <c r="A9" s="26" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
@@ -3720,23 +3723,23 @@
     </row>
     <row r="10">
       <c r="A10" s="26" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
@@ -3774,23 +3777,23 @@
     </row>
     <row r="11">
       <c r="A11" s="26" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
@@ -3828,23 +3831,23 @@
     </row>
     <row r="12">
       <c r="A12" s="26" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -3882,23 +3885,23 @@
     </row>
     <row r="13">
       <c r="A13" s="26" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
@@ -3936,23 +3939,23 @@
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
@@ -3990,23 +3993,23 @@
     </row>
     <row r="15">
       <c r="A15" s="26" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
@@ -4044,23 +4047,23 @@
     </row>
     <row r="16">
       <c r="A16" s="26" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
@@ -4098,23 +4101,23 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -4152,23 +4155,23 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -4206,23 +4209,23 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -4260,23 +4263,23 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -4318,23 +4321,23 @@
     </row>
     <row r="22">
       <c r="A22" s="35" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -4372,23 +4375,23 @@
     </row>
     <row r="23">
       <c r="A23" s="26" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
@@ -4426,23 +4429,23 @@
     </row>
     <row r="24">
       <c r="A24" s="26" t="s">
+        <v>562</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="B24" s="26" t="s">
-        <v>562</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>563</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>560</v>
-      </c>
       <c r="E24" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -4480,23 +4483,23 @@
     </row>
     <row r="25">
       <c r="A25" s="26" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -4534,23 +4537,23 @@
     </row>
     <row r="26">
       <c r="A26" s="26" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -4588,23 +4591,23 @@
     </row>
     <row r="27">
       <c r="A27" s="26" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -4642,23 +4645,23 @@
     </row>
     <row r="28">
       <c r="A28" s="26" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
@@ -4696,23 +4699,23 @@
     </row>
     <row r="29">
       <c r="A29" s="26" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -4750,23 +4753,23 @@
     </row>
     <row r="30">
       <c r="A30" s="26" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -4804,23 +4807,23 @@
     </row>
     <row r="31">
       <c r="A31" s="26" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
@@ -4858,23 +4861,23 @@
     </row>
     <row r="32">
       <c r="A32" s="26" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
@@ -4912,23 +4915,23 @@
     </row>
     <row r="33">
       <c r="A33" s="26" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -4966,23 +4969,23 @@
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
@@ -5020,23 +5023,23 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -5074,23 +5077,23 @@
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
@@ -5132,23 +5135,23 @@
     </row>
     <row r="38">
       <c r="A38" s="35" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
@@ -5186,23 +5189,23 @@
     </row>
     <row r="39">
       <c r="A39" s="26" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -5240,23 +5243,23 @@
     </row>
     <row r="40">
       <c r="A40" s="26" t="s">
+        <v>608</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>609</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>607</v>
       </c>
-      <c r="B40" s="26" t="s">
-        <v>608</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>609</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>606</v>
-      </c>
       <c r="E40" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -5294,23 +5297,23 @@
     </row>
     <row r="41">
       <c r="A41" s="26" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
@@ -5348,23 +5351,23 @@
     </row>
     <row r="42">
       <c r="A42" s="26" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
@@ -5402,23 +5405,23 @@
     </row>
     <row r="43">
       <c r="A43" s="26" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
@@ -5456,23 +5459,23 @@
     </row>
     <row r="44">
       <c r="A44" s="26" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
@@ -5510,23 +5513,23 @@
     </row>
     <row r="45">
       <c r="A45" s="26" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
@@ -5564,23 +5567,23 @@
     </row>
     <row r="46">
       <c r="A46" s="26" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
@@ -5618,23 +5621,23 @@
     </row>
     <row r="47">
       <c r="A47" s="26" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E47" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
@@ -5672,23 +5675,23 @@
     </row>
     <row r="48">
       <c r="A48" s="26" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
@@ -5726,23 +5729,23 @@
     </row>
     <row r="49">
       <c r="A49" s="26" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
@@ -5780,23 +5783,23 @@
     </row>
     <row r="50">
       <c r="A50" s="6" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
@@ -5834,23 +5837,23 @@
     </row>
     <row r="51">
       <c r="A51" s="6" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
@@ -5888,23 +5891,23 @@
     </row>
     <row r="52">
       <c r="A52" s="6" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
@@ -5945,23 +5948,23 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
@@ -5999,26 +6002,26 @@
     </row>
     <row r="55">
       <c r="A55" s="26" t="s">
+        <v>651</v>
+      </c>
+      <c r="B55" s="33" t="s">
+        <v>652</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>653</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>654</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>650</v>
-      </c>
-      <c r="B55" s="33" t="s">
-        <v>651</v>
-      </c>
-      <c r="C55" s="25" t="s">
-        <v>652</v>
-      </c>
-      <c r="D55" s="26" t="s">
-        <v>653</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>649</v>
       </c>
       <c r="F55" s="25"/>
       <c r="G55" s="26" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="I55" s="25"/>
       <c r="J55" s="25"/>
@@ -6055,26 +6058,26 @@
     </row>
     <row r="56">
       <c r="A56" s="26" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D56" s="26" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F56" s="25"/>
       <c r="G56" s="26" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="I56" s="25"/>
       <c r="J56" s="25"/>
@@ -6111,31 +6114,31 @@
     </row>
     <row r="57">
       <c r="A57" s="26" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D57" s="26" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F57" s="25"/>
       <c r="G57" s="26" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="I57" s="25"/>
       <c r="J57" s="25"/>
       <c r="K57" s="6" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="L57" s="25"/>
       <c r="M57" s="9">
@@ -6169,31 +6172,31 @@
     </row>
     <row r="58">
       <c r="A58" s="26" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F58" s="25"/>
       <c r="G58" s="26" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="I58" s="25"/>
       <c r="J58" s="25"/>
       <c r="K58" s="41" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="L58" s="25"/>
       <c r="M58" s="9">
@@ -6230,23 +6233,23 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
@@ -6287,23 +6290,23 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
@@ -6344,23 +6347,23 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
@@ -6398,19 +6401,19 @@
     </row>
     <row r="66">
       <c r="A66" s="14" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C66" s="42" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
@@ -6425,7 +6428,7 @@
         <v>21</v>
       </c>
       <c r="N66" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
@@ -6448,26 +6451,26 @@
     </row>
     <row r="67">
       <c r="A67" s="42" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B67" s="42" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C67" s="42" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="D67" s="43" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="E67" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
       <c r="I67" s="11"/>
       <c r="J67" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K67" s="44">
         <v>45548.0</v>
@@ -6477,7 +6480,7 @@
         <v>21</v>
       </c>
       <c r="N67" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
@@ -6500,26 +6503,26 @@
     </row>
     <row r="68">
       <c r="A68" s="42" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B68" s="42" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C68" s="42" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D68" s="43" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E68" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="11"/>
       <c r="J68" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K68" s="44">
         <v>45548.0</v>
@@ -6529,7 +6532,7 @@
         <v>21</v>
       </c>
       <c r="N68" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O68" s="11"/>
       <c r="P68" s="11"/>
@@ -6552,26 +6555,26 @@
     </row>
     <row r="69">
       <c r="A69" s="42" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B69" s="42" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C69" s="42" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D69" s="43" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E69" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
       <c r="H69" s="11"/>
       <c r="I69" s="11"/>
       <c r="J69" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K69" s="44">
         <v>45548.0</v>
@@ -6581,7 +6584,7 @@
         <v>21</v>
       </c>
       <c r="N69" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O69" s="11"/>
       <c r="P69" s="11"/>
@@ -6604,26 +6607,26 @@
     </row>
     <row r="70">
       <c r="A70" s="42" t="s">
+        <v>696</v>
+      </c>
+      <c r="B70" s="42" t="s">
+        <v>697</v>
+      </c>
+      <c r="C70" s="42" t="s">
+        <v>698</v>
+      </c>
+      <c r="D70" s="43" t="s">
         <v>695</v>
       </c>
-      <c r="B70" s="42" t="s">
-        <v>696</v>
-      </c>
-      <c r="C70" s="42" t="s">
-        <v>697</v>
-      </c>
-      <c r="D70" s="43" t="s">
-        <v>694</v>
-      </c>
       <c r="E70" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
       <c r="I70" s="11"/>
       <c r="J70" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K70" s="44">
         <v>45548.0</v>
@@ -6633,7 +6636,7 @@
         <v>21</v>
       </c>
       <c r="N70" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O70" s="11"/>
       <c r="P70" s="11"/>
@@ -6656,28 +6659,28 @@
     </row>
     <row r="71">
       <c r="A71" s="42" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B71" s="42" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D71" s="43" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E71" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F71" s="11"/>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="42" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="J71" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K71" s="44">
         <v>45548.0</v>
@@ -6687,7 +6690,7 @@
         <v>21</v>
       </c>
       <c r="N71" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O71" s="11"/>
       <c r="P71" s="11"/>
@@ -6710,26 +6713,26 @@
     </row>
     <row r="72">
       <c r="A72" s="42" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B72" s="42" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="D72" s="43" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E72" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
       <c r="J72" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K72" s="44">
         <v>45548.0</v>
@@ -6739,7 +6742,7 @@
         <v>21</v>
       </c>
       <c r="N72" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O72" s="11"/>
       <c r="P72" s="11"/>
@@ -6762,26 +6765,26 @@
     </row>
     <row r="73">
       <c r="A73" s="42" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B73" s="42" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="D73" s="43" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E73" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
       <c r="I73" s="11"/>
       <c r="J73" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K73" s="44">
         <v>45548.0</v>
@@ -6791,7 +6794,7 @@
         <v>21</v>
       </c>
       <c r="N73" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O73" s="11"/>
       <c r="P73" s="11"/>
@@ -6814,28 +6817,28 @@
     </row>
     <row r="74">
       <c r="A74" s="42" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B74" s="42" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C74" s="42" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D74" s="43" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E74" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F74" s="11"/>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="42" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="J74" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K74" s="44">
         <v>45548.0</v>
@@ -6845,7 +6848,7 @@
         <v>21</v>
       </c>
       <c r="N74" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O74" s="11"/>
       <c r="P74" s="11"/>
@@ -6868,26 +6871,26 @@
     </row>
     <row r="75">
       <c r="A75" s="42" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B75" s="42" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C75" s="42" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="D75" s="43" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="E75" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F75" s="11"/>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
       <c r="I75" s="11"/>
       <c r="J75" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K75" s="44">
         <v>45548.0</v>
@@ -6897,7 +6900,7 @@
         <v>21</v>
       </c>
       <c r="N75" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O75" s="11"/>
       <c r="P75" s="11"/>
@@ -6920,26 +6923,26 @@
     </row>
     <row r="76">
       <c r="A76" s="42" t="s">
+        <v>717</v>
+      </c>
+      <c r="B76" s="42" t="s">
+        <v>718</v>
+      </c>
+      <c r="C76" s="42" t="s">
+        <v>719</v>
+      </c>
+      <c r="D76" s="43" t="s">
         <v>716</v>
       </c>
-      <c r="B76" s="42" t="s">
-        <v>717</v>
-      </c>
-      <c r="C76" s="42" t="s">
-        <v>718</v>
-      </c>
-      <c r="D76" s="43" t="s">
-        <v>715</v>
-      </c>
       <c r="E76" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
       <c r="I76" s="11"/>
       <c r="J76" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K76" s="44">
         <v>45548.0</v>
@@ -6949,7 +6952,7 @@
         <v>21</v>
       </c>
       <c r="N76" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O76" s="11"/>
       <c r="P76" s="11"/>
@@ -6972,26 +6975,26 @@
     </row>
     <row r="77">
       <c r="A77" s="42" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B77" s="42" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C77" s="42" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="D77" s="43" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="E77" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F77" s="11"/>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
       <c r="I77" s="11"/>
       <c r="J77" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K77" s="44">
         <v>45548.0</v>
@@ -7001,7 +7004,7 @@
         <v>21</v>
       </c>
       <c r="N77" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O77" s="11"/>
       <c r="P77" s="11"/>
@@ -7024,28 +7027,28 @@
     </row>
     <row r="78">
       <c r="A78" s="42" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B78" s="42" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C78" s="42" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="D78" s="43" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="E78" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F78" s="11"/>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="42" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="J78" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K78" s="44">
         <v>45548.0</v>
@@ -7055,7 +7058,7 @@
         <v>21</v>
       </c>
       <c r="N78" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O78" s="11"/>
       <c r="P78" s="11"/>
@@ -7078,26 +7081,26 @@
     </row>
     <row r="79">
       <c r="A79" s="42" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B79" s="42" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C79" s="42" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="D79" s="43" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="E79" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F79" s="11"/>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="11"/>
       <c r="J79" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K79" s="44">
         <v>45548.0</v>
@@ -7107,7 +7110,7 @@
         <v>21</v>
       </c>
       <c r="N79" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O79" s="11"/>
       <c r="P79" s="11"/>
@@ -7130,26 +7133,26 @@
     </row>
     <row r="80">
       <c r="A80" s="42" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B80" s="42" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C80" s="42" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D80" s="43" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="E80" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F80" s="11"/>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
       <c r="I80" s="11"/>
       <c r="J80" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K80" s="44">
         <v>45548.0</v>
@@ -7159,7 +7162,7 @@
         <v>21</v>
       </c>
       <c r="N80" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O80" s="11"/>
       <c r="P80" s="11"/>
@@ -7182,26 +7185,26 @@
     </row>
     <row r="81">
       <c r="A81" s="42" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B81" s="42" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="C81" s="42" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="D81" s="43" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="E81" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F81" s="11"/>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="11"/>
       <c r="J81" s="42" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K81" s="44">
         <v>45548.0</v>
@@ -7211,7 +7214,7 @@
         <v>21</v>
       </c>
       <c r="N81" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="O81" s="11"/>
       <c r="P81" s="11"/>
@@ -9242,10 +9245,10 @@
         <v>162</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>158</v>
@@ -9289,13 +9292,13 @@
     </row>
     <row r="7">
       <c r="A7" s="35" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="25" t="s">
@@ -9337,13 +9340,13 @@
     </row>
     <row r="8">
       <c r="A8" s="35" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25" t="s">
@@ -9354,7 +9357,7 @@
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K8" s="15">
         <v>45627.0</v>
@@ -9387,16 +9390,16 @@
     </row>
     <row r="9">
       <c r="A9" s="26" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>68</v>
@@ -9406,7 +9409,7 @@
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
       <c r="J9" s="25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K9" s="15">
         <v>45627.0</v>
@@ -9439,16 +9442,16 @@
     </row>
     <row r="10">
       <c r="A10" s="26" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>68</v>
@@ -9458,7 +9461,7 @@
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
       <c r="J10" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K10" s="15">
         <v>45627.0</v>
@@ -9491,16 +9494,16 @@
     </row>
     <row r="11">
       <c r="A11" s="26" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>68</v>
@@ -9510,7 +9513,7 @@
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
       <c r="J11" s="25" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K11" s="15">
         <v>45627.0</v>
@@ -9543,16 +9546,16 @@
     </row>
     <row r="12">
       <c r="A12" s="26" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>68</v>
@@ -9562,7 +9565,7 @@
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="25" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K12" s="15">
         <v>45627.0</v>
@@ -9595,16 +9598,16 @@
     </row>
     <row r="13">
       <c r="A13" s="26" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>68</v>
@@ -9614,7 +9617,7 @@
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K13" s="15">
         <v>45627.0</v>
@@ -9647,13 +9650,13 @@
     </row>
     <row r="14">
       <c r="A14" s="35" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="25" t="s">
@@ -9695,13 +9698,13 @@
     </row>
     <row r="15">
       <c r="A15" s="35" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="25" t="s">
@@ -9743,16 +9746,16 @@
     </row>
     <row r="16">
       <c r="A16" s="26" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>68</v>
@@ -9793,16 +9796,16 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>201</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>200</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>68</v>
@@ -9843,16 +9846,16 @@
     </row>
     <row r="18">
       <c r="A18" s="26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>68</v>
@@ -9862,7 +9865,7 @@
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
       <c r="J18" s="25" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="K18" s="15">
         <v>45627.0</v>
@@ -9895,16 +9898,16 @@
     </row>
     <row r="19">
       <c r="A19" s="26" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>68</v>
@@ -9914,7 +9917,7 @@
       <c r="H19" s="25"/>
       <c r="I19" s="25"/>
       <c r="J19" s="25" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="K19" s="15">
         <v>45627.0</v>
@@ -9947,16 +9950,16 @@
     </row>
     <row r="20">
       <c r="A20" s="26" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>68</v>
@@ -9997,16 +10000,16 @@
     </row>
     <row r="21">
       <c r="A21" s="26" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>68</v>
@@ -10047,13 +10050,13 @@
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="25" t="s">
@@ -10064,7 +10067,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K22" s="15">
         <v>45627.0</v>
@@ -10097,16 +10100,16 @@
     </row>
     <row r="23">
       <c r="A23" s="26" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>68</v>
@@ -10116,7 +10119,7 @@
       <c r="H23" s="25"/>
       <c r="I23" s="25"/>
       <c r="J23" s="25" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="K23" s="15">
         <v>45627.0</v>
@@ -10149,16 +10152,16 @@
     </row>
     <row r="24">
       <c r="A24" s="26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>68</v>
@@ -10168,7 +10171,7 @@
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
       <c r="J24" s="25" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K24" s="15">
         <v>45627.0</v>
@@ -10201,16 +10204,16 @@
     </row>
     <row r="25">
       <c r="A25" s="26" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>68</v>
@@ -10220,7 +10223,7 @@
       <c r="H25" s="25"/>
       <c r="I25" s="25"/>
       <c r="J25" s="25" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="K25" s="15">
         <v>45627.0</v>
@@ -10253,16 +10256,16 @@
     </row>
     <row r="26">
       <c r="A26" s="26" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>68</v>
@@ -10272,7 +10275,7 @@
       <c r="H26" s="25"/>
       <c r="I26" s="25"/>
       <c r="J26" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="K26" s="15">
         <v>45627.0</v>
@@ -10305,16 +10308,16 @@
     </row>
     <row r="27">
       <c r="A27" s="26" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>68</v>
@@ -10324,7 +10327,7 @@
       <c r="H27" s="25"/>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K27" s="15">
         <v>45627.0</v>
@@ -10357,16 +10360,16 @@
     </row>
     <row r="28">
       <c r="A28" s="26" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E28" s="25" t="s">
         <v>68</v>
@@ -10376,7 +10379,7 @@
       <c r="H28" s="25"/>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="K28" s="15">
         <v>45627.0</v>
@@ -10409,13 +10412,13 @@
     </row>
     <row r="29">
       <c r="A29" s="26" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D29" s="33"/>
       <c r="E29" s="25" t="s">
@@ -10426,7 +10429,7 @@
       <c r="H29" s="25"/>
       <c r="I29" s="25"/>
       <c r="J29" s="36" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="K29" s="27">
         <v>45627.0</v>
@@ -10467,12 +10470,12 @@
     </row>
     <row r="32">
       <c r="A32" s="6" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -10602,13 +10605,13 @@
     </row>
     <row r="3">
       <c r="A3" s="35" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D3" s="33"/>
       <c r="E3" s="25" t="s">
@@ -10650,16 +10653,16 @@
     </row>
     <row r="4">
       <c r="A4" s="26" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>64</v>
@@ -10702,16 +10705,16 @@
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>64</v>
@@ -10754,16 +10757,16 @@
     </row>
     <row r="6">
       <c r="A6" s="26" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>64</v>
@@ -10806,16 +10809,16 @@
     </row>
     <row r="7">
       <c r="A7" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>268</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>269</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>270</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>267</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>64</v>
@@ -10825,7 +10828,7 @@
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="25" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="K7" s="27">
         <v>45627.0</v>
@@ -10858,16 +10861,16 @@
     </row>
     <row r="8">
       <c r="A8" s="26" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>64</v>
@@ -10877,7 +10880,7 @@
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K8" s="27">
         <v>45627.0</v>
@@ -10914,13 +10917,13 @@
     </row>
     <row r="10">
       <c r="A10" s="35" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25" t="s">
@@ -10962,16 +10965,16 @@
     </row>
     <row r="11">
       <c r="A11" s="26" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>64</v>
@@ -11012,16 +11015,16 @@
     </row>
     <row r="12">
       <c r="A12" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>283</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>282</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>64</v>
@@ -11062,16 +11065,16 @@
     </row>
     <row r="13">
       <c r="A13" s="26" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>64</v>
@@ -11112,16 +11115,16 @@
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>290</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>289</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>64</v>
@@ -11131,7 +11134,7 @@
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
       <c r="J14" s="36" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="K14" s="27">
         <v>45627.0</v>
@@ -11164,16 +11167,16 @@
     </row>
     <row r="15">
       <c r="A15" s="26" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>64</v>
@@ -11214,16 +11217,16 @@
     </row>
     <row r="16">
       <c r="A16" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>298</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>300</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>297</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>64</v>
@@ -11264,16 +11267,16 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>64</v>
@@ -11314,16 +11317,16 @@
     </row>
     <row r="18">
       <c r="A18" s="26" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>64</v>
@@ -11364,16 +11367,16 @@
     </row>
     <row r="19">
       <c r="A19" s="26" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>64</v>
@@ -11383,7 +11386,7 @@
       <c r="H19" s="25"/>
       <c r="I19" s="25"/>
       <c r="J19" s="25" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="K19" s="27">
         <v>45627.0</v>
@@ -11416,16 +11419,16 @@
     </row>
     <row r="20">
       <c r="A20" s="26" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>64</v>
@@ -11466,16 +11469,16 @@
     </row>
     <row r="21">
       <c r="A21" s="26" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>64</v>
@@ -11516,16 +11519,16 @@
     </row>
     <row r="22">
       <c r="A22" s="26" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>64</v>
@@ -11566,16 +11569,16 @@
     </row>
     <row r="23">
       <c r="A23" s="26" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>64</v>
@@ -11650,13 +11653,13 @@
     </row>
     <row r="25">
       <c r="A25" s="35" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D25" s="25"/>
       <c r="E25" s="25" t="s">
@@ -11667,7 +11670,7 @@
       <c r="H25" s="25"/>
       <c r="I25" s="25"/>
       <c r="J25" s="25" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="K25" s="27">
         <v>45627.0</v>
@@ -11700,16 +11703,16 @@
     </row>
     <row r="26">
       <c r="A26" s="26" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>64</v>
@@ -11752,16 +11755,16 @@
     </row>
     <row r="27">
       <c r="A27" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="D27" s="25" t="s">
         <v>332</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>333</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>331</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>64</v>
@@ -11771,7 +11774,7 @@
       <c r="H27" s="25"/>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K27" s="27">
         <v>45627.0</v>
@@ -11804,16 +11807,16 @@
     </row>
     <row r="28">
       <c r="A28" s="26" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E28" s="25" t="s">
         <v>64</v>
@@ -11856,16 +11859,16 @@
     </row>
     <row r="29">
       <c r="A29" s="26" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E29" s="25" t="s">
         <v>64</v>
@@ -11908,16 +11911,16 @@
     </row>
     <row r="30">
       <c r="A30" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="D30" s="25" t="s">
         <v>343</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>344</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>345</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>342</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>64</v>
@@ -11927,7 +11930,7 @@
       <c r="H30" s="25"/>
       <c r="I30" s="25"/>
       <c r="J30" s="25" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K30" s="27">
         <v>45627.0</v>
@@ -11994,13 +11997,13 @@
     </row>
     <row r="32">
       <c r="A32" s="35" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="25" t="s">
@@ -12011,7 +12014,7 @@
       <c r="H32" s="25"/>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="K32" s="27">
         <v>45627.0</v>
@@ -12044,16 +12047,16 @@
     </row>
     <row r="33">
       <c r="A33" s="26" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>64</v>
@@ -12096,16 +12099,16 @@
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="D34" s="25" t="s">
         <v>355</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>354</v>
       </c>
       <c r="E34" s="25" t="s">
         <v>64</v>
@@ -12146,16 +12149,16 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E35" s="25" t="s">
         <v>64</v>
@@ -12196,16 +12199,16 @@
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E36" s="25" t="s">
         <v>64</v>
@@ -12250,13 +12253,13 @@
     </row>
     <row r="38">
       <c r="A38" s="35" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="25" t="s">
@@ -12298,16 +12301,16 @@
     </row>
     <row r="39">
       <c r="A39" s="26" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>64</v>
@@ -12317,7 +12320,7 @@
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
       <c r="J39" s="25" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="K39" s="27">
         <v>45627.0</v>
@@ -12350,16 +12353,16 @@
     </row>
     <row r="40">
       <c r="A40" s="26" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E40" s="25" t="s">
         <v>64</v>
@@ -12369,7 +12372,7 @@
       <c r="H40" s="25"/>
       <c r="I40" s="25"/>
       <c r="J40" s="25" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="K40" s="27">
         <v>45627.0</v>
@@ -12402,16 +12405,16 @@
     </row>
     <row r="41">
       <c r="A41" s="26" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E41" s="25" t="s">
         <v>64</v>
@@ -12421,7 +12424,7 @@
       <c r="H41" s="25"/>
       <c r="I41" s="25"/>
       <c r="J41" s="25" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="K41" s="27">
         <v>45627.0</v>
@@ -12454,16 +12457,16 @@
     </row>
     <row r="42">
       <c r="A42" s="26" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E42" s="25" t="s">
         <v>64</v>
@@ -12473,7 +12476,7 @@
       <c r="H42" s="25"/>
       <c r="I42" s="25"/>
       <c r="J42" s="25" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K42" s="27">
         <v>45627.0</v>
@@ -12506,16 +12509,16 @@
     </row>
     <row r="43">
       <c r="A43" s="26" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E43" s="25" t="s">
         <v>64</v>
@@ -12525,7 +12528,7 @@
       <c r="H43" s="25"/>
       <c r="I43" s="25"/>
       <c r="J43" s="25" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="K43" s="27">
         <v>45627.0</v>
@@ -12558,16 +12561,16 @@
     </row>
     <row r="44">
       <c r="A44" s="26" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E44" s="25" t="s">
         <v>64</v>
@@ -12577,7 +12580,7 @@
       <c r="H44" s="25"/>
       <c r="I44" s="25"/>
       <c r="J44" s="25" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="K44" s="27">
         <v>45627.0</v>
@@ -12610,16 +12613,16 @@
     </row>
     <row r="45">
       <c r="A45" s="26" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E45" s="25" t="s">
         <v>64</v>
@@ -12629,7 +12632,7 @@
       <c r="H45" s="25"/>
       <c r="I45" s="25"/>
       <c r="J45" s="25" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="K45" s="27">
         <v>45627.0</v>
@@ -12662,16 +12665,16 @@
     </row>
     <row r="46">
       <c r="A46" s="26" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E46" s="25" t="s">
         <v>64</v>
@@ -12681,7 +12684,7 @@
       <c r="H46" s="25"/>
       <c r="I46" s="25"/>
       <c r="J46" s="25" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="K46" s="27">
         <v>45627.0</v>
@@ -12714,16 +12717,16 @@
     </row>
     <row r="47">
       <c r="A47" s="26" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E47" s="25" t="s">
         <v>64</v>
@@ -12733,7 +12736,7 @@
       <c r="H47" s="25"/>
       <c r="I47" s="25"/>
       <c r="J47" s="25" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="K47" s="27">
         <v>45627.0</v>
@@ -12770,13 +12773,13 @@
     </row>
     <row r="49">
       <c r="A49" s="35" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D49" s="25"/>
       <c r="E49" s="25" t="s">
@@ -12795,7 +12798,7 @@
         <v>21</v>
       </c>
       <c r="N49" s="25" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O49" s="25"/>
       <c r="P49" s="25"/>
@@ -12818,16 +12821,16 @@
     </row>
     <row r="50">
       <c r="A50" s="26" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E50" s="25" t="s">
         <v>64</v>
@@ -12845,7 +12848,7 @@
         <v>21</v>
       </c>
       <c r="N50" s="25" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O50" s="25"/>
       <c r="P50" s="25"/>
@@ -12868,16 +12871,16 @@
     </row>
     <row r="51">
       <c r="A51" s="26" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E51" s="25" t="s">
         <v>64</v>
@@ -12895,7 +12898,7 @@
         <v>21</v>
       </c>
       <c r="N51" s="25" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O51" s="25"/>
       <c r="P51" s="25"/>
@@ -12918,16 +12921,16 @@
     </row>
     <row r="52">
       <c r="A52" s="26" t="s">
+        <v>419</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>420</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>421</v>
+      </c>
+      <c r="D52" s="25" t="s">
         <v>418</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>419</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>420</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>417</v>
       </c>
       <c r="E52" s="25" t="s">
         <v>64</v>
@@ -12945,7 +12948,7 @@
         <v>21</v>
       </c>
       <c r="N52" s="25" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O52" s="25"/>
       <c r="P52" s="25"/>
@@ -13002,10 +13005,10 @@
     </row>
     <row r="54">
       <c r="A54" s="35" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C54" s="25"/>
       <c r="D54" s="25"/>
@@ -13040,13 +13043,13 @@
     </row>
     <row r="55">
       <c r="A55" s="26" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D55" s="25"/>
       <c r="E55" s="25" t="s">
@@ -13248,16 +13251,16 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
@@ -13266,7 +13269,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="6" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="37">
@@ -13395,12 +13398,12 @@
     </row>
     <row r="2">
       <c r="A2" s="35" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="25"/>
       <c r="D2" s="26" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
@@ -13441,17 +13444,17 @@
     </row>
     <row r="3">
       <c r="A3" s="25" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D3" s="33"/>
       <c r="E3" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
@@ -13491,24 +13494,24 @@
     </row>
     <row r="4">
       <c r="A4" s="25" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D4" s="33"/>
       <c r="E4" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
       <c r="J4" s="26" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="K4" s="27">
         <v>45627.0</v>
@@ -13541,24 +13544,24 @@
     </row>
     <row r="5">
       <c r="A5" s="25" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
       <c r="J5" s="26" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="K5" s="27">
         <v>45627.0</v>
@@ -13591,24 +13594,24 @@
     </row>
     <row r="6">
       <c r="A6" s="25" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D6" s="33"/>
       <c r="E6" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
       <c r="J6" s="26" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K6" s="27">
         <v>45627.0</v>
@@ -13641,24 +13644,24 @@
     </row>
     <row r="7">
       <c r="A7" s="25" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D7" s="33"/>
       <c r="E7" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="26" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="K7" s="27">
         <v>45627.0</v>
@@ -13691,24 +13694,24 @@
     </row>
     <row r="8">
       <c r="A8" s="25" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="26" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K8" s="27">
         <v>45627.0</v>
@@ -13741,24 +13744,24 @@
     </row>
     <row r="9">
       <c r="A9" s="25" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
       <c r="J9" s="26" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="K9" s="27">
         <v>45627.0</v>
@@ -13791,26 +13794,26 @@
     </row>
     <row r="10">
       <c r="A10" s="38" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
       <c r="J10" s="26" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="K10" s="27">
         <v>45627.0</v>
@@ -13843,26 +13846,26 @@
     </row>
     <row r="11">
       <c r="A11" s="38" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
       <c r="J11" s="26" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="K11" s="27">
         <v>45627.0</v>
@@ -13895,26 +13898,26 @@
     </row>
     <row r="12">
       <c r="A12" s="38" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="26" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="K12" s="27">
         <v>45627.0</v>
@@ -13947,24 +13950,24 @@
     </row>
     <row r="13">
       <c r="A13" s="25" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
       <c r="J13" s="26" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="K13" s="27">
         <v>45627.0</v>
@@ -13997,24 +14000,24 @@
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D14" s="33"/>
       <c r="E14" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
       <c r="J14" s="26" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="K14" s="27">
         <v>45627.0</v>
@@ -14047,24 +14050,24 @@
     </row>
     <row r="15">
       <c r="A15" s="25" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
       <c r="J15" s="26" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="K15" s="27">
         <v>45627.0</v>
@@ -14097,26 +14100,26 @@
     </row>
     <row r="16">
       <c r="A16" s="38" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
       <c r="J16" s="26" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="K16" s="27">
         <v>45627.0</v>
@@ -14149,26 +14152,26 @@
     </row>
     <row r="17">
       <c r="A17" s="38" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
       <c r="J17" s="26" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="K17" s="27">
         <v>45627.0</v>
@@ -14201,26 +14204,26 @@
     </row>
     <row r="18">
       <c r="A18" s="38" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
       <c r="J18" s="26" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="K18" s="27">
         <v>45627.0</v>
@@ -14253,7 +14256,7 @@
     </row>
     <row r="20">
       <c r="A20" s="39" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
closes #160 contributors metadata in RDF, HTML
- Contributors for concepts and creators for vocabs are now declared as
  instances of `dct:Agent` and `foaf:Person` in a blank node in vocab
- Affiliation is expressed using `org:memberOf` -> `foaf:name`
- ORCID, if provided, is expressed using `scoro:hasORCID`
- Website, if provided, is expressed using `foaf:homepage`
- In the HTML metadata, this is used to populate the ReSpec json and the
  contributors section. If website or ORCID are available, they are
  hyperlinked to the person's name.
- Fixes incorrect contributors list string in AI and EU-AIAct extensions
- The contributors metadata is in `code/contributors,json`
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ai.xlsx
+++ b/code/vocab_csv/ai.xlsx
@@ -1303,7 +1303,7 @@
     <t>Capability to generate new content that is distinct from merely deriving or transforming existing content</t>
   </si>
   <si>
-    <t xml:space="preserve">Delaram Golpayegani, Harshvardhan J. Pandit, </t>
+    <t>Delaram Golpayegani, Harshvardhan J. Pandit</t>
   </si>
   <si>
     <t>AudioGeneration</t>
@@ -12822,7 +12822,7 @@
       <c r="M49" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="N49" s="25" t="s">
+      <c r="N49" s="26" t="s">
         <v>410</v>
       </c>
       <c r="O49" s="25"/>
@@ -12872,7 +12872,7 @@
       <c r="M50" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="N50" s="25" t="s">
+      <c r="N50" s="26" t="s">
         <v>410</v>
       </c>
       <c r="O50" s="25"/>
@@ -12922,7 +12922,7 @@
       <c r="M51" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="N51" s="25" t="s">
+      <c r="N51" s="26" t="s">
         <v>410</v>
       </c>
       <c r="O51" s="25"/>
@@ -12972,7 +12972,7 @@
       <c r="M52" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="N52" s="25" t="s">
+      <c r="N52" s="26" t="s">
         <v>410</v>
       </c>
       <c r="O52" s="25"/>

</xml_diff>

<commit_message>
fixes broken source links in legal-kr, eu-gdpr, ai
- closes #280
- the links in legal-kr contains '(', ')', and ',' which caused the
  `vocab_func` function handling webpage links to malfunction as we use
  these for separating multiple links
- the solution was encoding these links in the spreadsheet so that the
  characters are not triggered during output generation but they are
  decoded by browsers when showing/using the link (the encoded url also
  resolves as expected)
- also fixes eu-gdpr A16, A17, A18 source - missing '(' at start
- AI extension - fixed `AudioProcessing` and `BiometricIdentification`
  source references which used a different format for references

Co-authored-by: Arthit Suriyawongkul <arthit@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ai.xlsx
+++ b/code/vocab_csv/ai.xlsx
@@ -788,159 +788,140 @@
     <t xml:space="preserve">Technique involving processing audio </t>
   </si>
   <si>
+    <t>(AI Watch,https://ai-watch.ec.europa.eu/);(Defining Artificial Intelligence 2.0,https://publications.jrc.ec.europa.eu/repository/handle/JRC126426)</t>
+  </si>
+  <si>
+    <t>Subsymbolic</t>
+  </si>
+  <si>
+    <t>Neurosymbolic</t>
+  </si>
+  <si>
+    <t>AudioCapability</t>
+  </si>
+  <si>
+    <t>Audio Capability</t>
+  </si>
+  <si>
+    <t>Capabilities related to the processing and generation of audio</t>
+  </si>
+  <si>
+    <t>SoundSourceSeparation</t>
+  </si>
+  <si>
+    <t>Sound Source Separation</t>
+  </si>
+  <si>
+    <t>Capability for extracting individual sound from audio recordings</t>
+  </si>
+  <si>
+    <t>ai:AudioCapability</t>
+  </si>
+  <si>
+    <t>SoundSynthesis</t>
+  </si>
+  <si>
+    <t>Sound Synthesis</t>
+  </si>
+  <si>
+    <t>Capability for generation of artificial sound</t>
+  </si>
+  <si>
+    <t>ai:AudioCapability,ai:ContentGeneration</t>
+  </si>
+  <si>
+    <t>SpeakerRecognition</t>
+  </si>
+  <si>
+    <t>Speaker Recognition</t>
+  </si>
+  <si>
+    <t>Capability of recognising speaker(s) in audio recordings</t>
+  </si>
+  <si>
+    <t>ai:AudioProcessing,ai:HumanOrientedCapability</t>
+  </si>
+  <si>
+    <t>SpeechRecognition</t>
+  </si>
+  <si>
+    <t>Speech Recognition</t>
+  </si>
+  <si>
+    <t>Capability of converting a speech signal to a representation of the content of the speech</t>
+  </si>
+  <si>
+    <t>ISO/IEC 22989:2022, 3.6.17</t>
+  </si>
+  <si>
+    <t>SpeechSynthesis</t>
+  </si>
+  <si>
+    <t>Speech Synthesis</t>
+  </si>
+  <si>
+    <t>Capability for generation of artificial speech</t>
+  </si>
+  <si>
+    <t>ISO/IEC 22989:2022, 3.6.18</t>
+  </si>
+  <si>
+    <t>HumanOrientedCapability</t>
+  </si>
+  <si>
+    <t>Human-Oriented Capability</t>
+  </si>
+  <si>
+    <t>Capabilities that are inherently about humans or oriented towards human characteristics and activities</t>
+  </si>
+  <si>
+    <t>BehaviourAnalysis</t>
+  </si>
+  <si>
+    <t>Behaviour Analysis</t>
+  </si>
+  <si>
+    <t>Capability of a system in analysing people's behaviour</t>
+  </si>
+  <si>
+    <t>ai:HumanOrientedCapability</t>
+  </si>
+  <si>
+    <t>BiometricCapability</t>
+  </si>
+  <si>
+    <t>Biometric Capability</t>
+  </si>
+  <si>
+    <t>Capability involving processing of biometric data or related to biometrics</t>
+  </si>
+  <si>
+    <t>BiometricCategorisation</t>
+  </si>
+  <si>
+    <t>Biometric Categorisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capability involving assigning natural persons to specific categories based on their biometric data </t>
+  </si>
+  <si>
+    <t>ai:BiometricCapability</t>
+  </si>
+  <si>
+    <t>BiometricIdentification</t>
+  </si>
+  <si>
+    <t>Biometric Identification</t>
+  </si>
+  <si>
+    <t>Capability involving automated recognition of physical, physiological and behavioural human features such as the face, eye movement, body shape, voice, prosody, gait, posture, heart rate, blood pressure, odour, keystrokes characteristics, for the purpose of establishing an individual’s identity by comparing biometric data of that individual to stored biometric data of individuals in a reference database, irrespective of whether the individual has given its consent or not</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
       </rPr>
-      <t>AI Watch, Defining Artificial Intelligence 2.0 [</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>https://publications.jrc.ec.europa.eu/repository/handle/JRC126426</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>]</t>
-    </r>
-  </si>
-  <si>
-    <t>Subsymbolic</t>
-  </si>
-  <si>
-    <t>Neurosymbolic</t>
-  </si>
-  <si>
-    <t>AudioCapability</t>
-  </si>
-  <si>
-    <t>Audio Capability</t>
-  </si>
-  <si>
-    <t>Capabilities related to the processing and generation of audio</t>
-  </si>
-  <si>
-    <t>SoundSourceSeparation</t>
-  </si>
-  <si>
-    <t>Sound Source Separation</t>
-  </si>
-  <si>
-    <t>Capability for extracting individual sound from audio recordings</t>
-  </si>
-  <si>
-    <t>ai:AudioCapability</t>
-  </si>
-  <si>
-    <t>SoundSynthesis</t>
-  </si>
-  <si>
-    <t>Sound Synthesis</t>
-  </si>
-  <si>
-    <t>Capability for generation of artificial sound</t>
-  </si>
-  <si>
-    <t>ai:AudioCapability,ai:ContentGeneration</t>
-  </si>
-  <si>
-    <t>SpeakerRecognition</t>
-  </si>
-  <si>
-    <t>Speaker Recognition</t>
-  </si>
-  <si>
-    <t>Capability of recognising speaker(s) in audio recordings</t>
-  </si>
-  <si>
-    <t>ai:AudioProcessing,ai:HumanOrientedCapability</t>
-  </si>
-  <si>
-    <t>SpeechRecognition</t>
-  </si>
-  <si>
-    <t>Speech Recognition</t>
-  </si>
-  <si>
-    <t>Capability of converting a speech signal to a representation of the content of the speech</t>
-  </si>
-  <si>
-    <t>ISO/IEC 22989:2022, 3.6.17</t>
-  </si>
-  <si>
-    <t>SpeechSynthesis</t>
-  </si>
-  <si>
-    <t>Speech Synthesis</t>
-  </si>
-  <si>
-    <t>Capability for generation of artificial speech</t>
-  </si>
-  <si>
-    <t>ISO/IEC 22989:2022, 3.6.18</t>
-  </si>
-  <si>
-    <t>HumanOrientedCapability</t>
-  </si>
-  <si>
-    <t>Human-Oriented Capability</t>
-  </si>
-  <si>
-    <t>Capabilities that are inherently about humans or oriented towards human characteristics and activities</t>
-  </si>
-  <si>
-    <t>BehaviourAnalysis</t>
-  </si>
-  <si>
-    <t>Behaviour Analysis</t>
-  </si>
-  <si>
-    <t>Capability of a system in analysing people's behaviour</t>
-  </si>
-  <si>
-    <t>ai:HumanOrientedCapability</t>
-  </si>
-  <si>
-    <t>BiometricCapability</t>
-  </si>
-  <si>
-    <t>Biometric Capability</t>
-  </si>
-  <si>
-    <t>Capability involving processing of biometric data or related to biometrics</t>
-  </si>
-  <si>
-    <t>BiometricCategorisation</t>
-  </si>
-  <si>
-    <t>Biometric Categorisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capability involving assigning natural persons to specific categories based on their biometric data </t>
-  </si>
-  <si>
-    <t>ai:BiometricCapability</t>
-  </si>
-  <si>
-    <t>BiometricIdentification</t>
-  </si>
-  <si>
-    <t>Biometric Identification</t>
-  </si>
-  <si>
-    <t>Capability involving automated recognition of physical, physiological and behavioural human features such as the face, eye movement, body shape, voice, prosody, gait, posture, heart rate, blood pressure, odour, keystrokes characteristics, for the purpose of establishing an individual’s identity by comparing biometric data of that individual to stored biometric data of individuals in a reference database, irrespective of whether the individual has given its consent or not</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>The AI Act, Recital 15 [</t>
+      <t>(The AI Act Recital 15,</t>
     </r>
     <r>
       <rPr>
@@ -954,7 +935,7 @@
       <rPr>
         <rFont val="Arial"/>
       </rPr>
-      <t>]</t>
+      <t>)</t>
     </r>
   </si>
   <si>
@@ -2310,7 +2291,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2367,11 +2348,6 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -2461,7 +2437,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2568,11 +2544,11 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -2581,16 +2557,13 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -3375,7 +3348,7 @@
       <c r="H2" s="40"/>
       <c r="I2" s="8"/>
       <c r="J2" s="40"/>
-      <c r="M2" s="37">
+      <c r="M2" s="36">
         <v>45410.0</v>
       </c>
       <c r="N2" s="40"/>
@@ -6185,7 +6158,7 @@
       </c>
       <c r="I58" s="25"/>
       <c r="J58" s="25"/>
-      <c r="K58" s="41" t="s">
+      <c r="K58" s="37" t="s">
         <v>670</v>
       </c>
       <c r="L58" s="25"/>
@@ -6396,7 +6369,7 @@
       <c r="B66" s="11" t="s">
         <v>681</v>
       </c>
-      <c r="C66" s="42" t="s">
+      <c r="C66" s="41" t="s">
         <v>682</v>
       </c>
       <c r="D66" s="10" t="s">
@@ -6442,16 +6415,16 @@
       <c r="AH66" s="7"/>
     </row>
     <row r="67">
-      <c r="A67" s="42" t="s">
+      <c r="A67" s="41" t="s">
         <v>685</v>
       </c>
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="41" t="s">
         <v>686</v>
       </c>
-      <c r="C67" s="42" t="s">
+      <c r="C67" s="41" t="s">
         <v>687</v>
       </c>
-      <c r="D67" s="43" t="s">
+      <c r="D67" s="42" t="s">
         <v>688</v>
       </c>
       <c r="E67" s="6" t="s">
@@ -6463,10 +6436,10 @@
       </c>
       <c r="H67" s="11"/>
       <c r="K67" s="11"/>
-      <c r="L67" s="42" t="s">
+      <c r="L67" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M67" s="44">
+      <c r="M67" s="43">
         <v>45548.0</v>
       </c>
       <c r="N67" s="16"/>
@@ -6496,16 +6469,16 @@
       <c r="AH67" s="7"/>
     </row>
     <row r="68">
-      <c r="A68" s="42" t="s">
+      <c r="A68" s="41" t="s">
         <v>690</v>
       </c>
-      <c r="B68" s="42" t="s">
+      <c r="B68" s="41" t="s">
         <v>691</v>
       </c>
-      <c r="C68" s="42" t="s">
+      <c r="C68" s="41" t="s">
         <v>692</v>
       </c>
-      <c r="D68" s="43" t="s">
+      <c r="D68" s="42" t="s">
         <v>693</v>
       </c>
       <c r="E68" s="6" t="s">
@@ -6517,10 +6490,10 @@
       </c>
       <c r="H68" s="11"/>
       <c r="K68" s="11"/>
-      <c r="L68" s="42" t="s">
+      <c r="L68" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M68" s="44">
+      <c r="M68" s="43">
         <v>45548.0</v>
       </c>
       <c r="N68" s="16"/>
@@ -6550,16 +6523,16 @@
       <c r="AH68" s="7"/>
     </row>
     <row r="69">
-      <c r="A69" s="42" t="s">
+      <c r="A69" s="41" t="s">
         <v>694</v>
       </c>
-      <c r="B69" s="42" t="s">
+      <c r="B69" s="41" t="s">
         <v>695</v>
       </c>
-      <c r="C69" s="42" t="s">
+      <c r="C69" s="41" t="s">
         <v>696</v>
       </c>
-      <c r="D69" s="43" t="s">
+      <c r="D69" s="42" t="s">
         <v>697</v>
       </c>
       <c r="E69" s="6" t="s">
@@ -6571,10 +6544,10 @@
       </c>
       <c r="H69" s="11"/>
       <c r="K69" s="11"/>
-      <c r="L69" s="42" t="s">
+      <c r="L69" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M69" s="44">
+      <c r="M69" s="43">
         <v>45548.0</v>
       </c>
       <c r="N69" s="16"/>
@@ -6604,16 +6577,16 @@
       <c r="AH69" s="7"/>
     </row>
     <row r="70">
-      <c r="A70" s="42" t="s">
+      <c r="A70" s="41" t="s">
         <v>698</v>
       </c>
-      <c r="B70" s="42" t="s">
+      <c r="B70" s="41" t="s">
         <v>699</v>
       </c>
-      <c r="C70" s="42" t="s">
+      <c r="C70" s="41" t="s">
         <v>700</v>
       </c>
-      <c r="D70" s="43" t="s">
+      <c r="D70" s="42" t="s">
         <v>697</v>
       </c>
       <c r="E70" s="6" t="s">
@@ -6625,10 +6598,10 @@
       </c>
       <c r="H70" s="11"/>
       <c r="K70" s="11"/>
-      <c r="L70" s="42" t="s">
+      <c r="L70" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M70" s="44">
+      <c r="M70" s="43">
         <v>45548.0</v>
       </c>
       <c r="N70" s="16"/>
@@ -6658,16 +6631,16 @@
       <c r="AH70" s="7"/>
     </row>
     <row r="71">
-      <c r="A71" s="42" t="s">
+      <c r="A71" s="41" t="s">
         <v>701</v>
       </c>
-      <c r="B71" s="42" t="s">
+      <c r="B71" s="41" t="s">
         <v>702</v>
       </c>
-      <c r="C71" s="42" t="s">
+      <c r="C71" s="41" t="s">
         <v>703</v>
       </c>
-      <c r="D71" s="43" t="s">
+      <c r="D71" s="42" t="s">
         <v>697</v>
       </c>
       <c r="E71" s="6" t="s">
@@ -6678,13 +6651,13 @@
         <v>506</v>
       </c>
       <c r="H71" s="11"/>
-      <c r="K71" s="42" t="s">
+      <c r="K71" s="41" t="s">
         <v>704</v>
       </c>
-      <c r="L71" s="42" t="s">
+      <c r="L71" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M71" s="44">
+      <c r="M71" s="43">
         <v>45548.0</v>
       </c>
       <c r="N71" s="16"/>
@@ -6714,16 +6687,16 @@
       <c r="AH71" s="7"/>
     </row>
     <row r="72">
-      <c r="A72" s="42" t="s">
+      <c r="A72" s="41" t="s">
         <v>705</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="41" t="s">
         <v>706</v>
       </c>
-      <c r="C72" s="42" t="s">
+      <c r="C72" s="41" t="s">
         <v>707</v>
       </c>
-      <c r="D72" s="43" t="s">
+      <c r="D72" s="42" t="s">
         <v>697</v>
       </c>
       <c r="E72" s="6" t="s">
@@ -6735,10 +6708,10 @@
       </c>
       <c r="H72" s="11"/>
       <c r="K72" s="11"/>
-      <c r="L72" s="42" t="s">
+      <c r="L72" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M72" s="44">
+      <c r="M72" s="43">
         <v>45548.0</v>
       </c>
       <c r="N72" s="16"/>
@@ -6768,16 +6741,16 @@
       <c r="AH72" s="7"/>
     </row>
     <row r="73">
-      <c r="A73" s="42" t="s">
+      <c r="A73" s="41" t="s">
         <v>708</v>
       </c>
-      <c r="B73" s="42" t="s">
+      <c r="B73" s="41" t="s">
         <v>709</v>
       </c>
-      <c r="C73" s="42" t="s">
+      <c r="C73" s="41" t="s">
         <v>710</v>
       </c>
-      <c r="D73" s="43" t="s">
+      <c r="D73" s="42" t="s">
         <v>697</v>
       </c>
       <c r="E73" s="6" t="s">
@@ -6789,10 +6762,10 @@
       </c>
       <c r="H73" s="11"/>
       <c r="K73" s="11"/>
-      <c r="L73" s="42" t="s">
+      <c r="L73" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M73" s="44">
+      <c r="M73" s="43">
         <v>45548.0</v>
       </c>
       <c r="N73" s="16"/>
@@ -6822,16 +6795,16 @@
       <c r="AH73" s="7"/>
     </row>
     <row r="74">
-      <c r="A74" s="42" t="s">
+      <c r="A74" s="41" t="s">
         <v>711</v>
       </c>
-      <c r="B74" s="42" t="s">
+      <c r="B74" s="41" t="s">
         <v>712</v>
       </c>
-      <c r="C74" s="42" t="s">
+      <c r="C74" s="41" t="s">
         <v>713</v>
       </c>
-      <c r="D74" s="43" t="s">
+      <c r="D74" s="42" t="s">
         <v>693</v>
       </c>
       <c r="E74" s="6" t="s">
@@ -6842,13 +6815,13 @@
         <v>506</v>
       </c>
       <c r="H74" s="11"/>
-      <c r="K74" s="42" t="s">
+      <c r="K74" s="41" t="s">
         <v>714</v>
       </c>
-      <c r="L74" s="42" t="s">
+      <c r="L74" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M74" s="44">
+      <c r="M74" s="43">
         <v>45548.0</v>
       </c>
       <c r="N74" s="16"/>
@@ -6878,16 +6851,16 @@
       <c r="AH74" s="7"/>
     </row>
     <row r="75">
-      <c r="A75" s="42" t="s">
+      <c r="A75" s="41" t="s">
         <v>715</v>
       </c>
-      <c r="B75" s="42" t="s">
+      <c r="B75" s="41" t="s">
         <v>716</v>
       </c>
-      <c r="C75" s="42" t="s">
+      <c r="C75" s="41" t="s">
         <v>717</v>
       </c>
-      <c r="D75" s="43" t="s">
+      <c r="D75" s="42" t="s">
         <v>718</v>
       </c>
       <c r="E75" s="6" t="s">
@@ -6899,10 +6872,10 @@
       </c>
       <c r="H75" s="11"/>
       <c r="K75" s="11"/>
-      <c r="L75" s="42" t="s">
+      <c r="L75" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M75" s="44">
+      <c r="M75" s="43">
         <v>45548.0</v>
       </c>
       <c r="N75" s="16"/>
@@ -6932,16 +6905,16 @@
       <c r="AH75" s="7"/>
     </row>
     <row r="76">
-      <c r="A76" s="42" t="s">
+      <c r="A76" s="41" t="s">
         <v>719</v>
       </c>
-      <c r="B76" s="42" t="s">
+      <c r="B76" s="41" t="s">
         <v>720</v>
       </c>
-      <c r="C76" s="42" t="s">
+      <c r="C76" s="41" t="s">
         <v>721</v>
       </c>
-      <c r="D76" s="43" t="s">
+      <c r="D76" s="42" t="s">
         <v>718</v>
       </c>
       <c r="E76" s="6" t="s">
@@ -6953,10 +6926,10 @@
       </c>
       <c r="H76" s="11"/>
       <c r="K76" s="11"/>
-      <c r="L76" s="42" t="s">
+      <c r="L76" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M76" s="44">
+      <c r="M76" s="43">
         <v>45548.0</v>
       </c>
       <c r="N76" s="16"/>
@@ -6986,16 +6959,16 @@
       <c r="AH76" s="7"/>
     </row>
     <row r="77">
-      <c r="A77" s="42" t="s">
+      <c r="A77" s="41" t="s">
         <v>722</v>
       </c>
-      <c r="B77" s="42" t="s">
+      <c r="B77" s="41" t="s">
         <v>723</v>
       </c>
-      <c r="C77" s="42" t="s">
+      <c r="C77" s="41" t="s">
         <v>724</v>
       </c>
-      <c r="D77" s="43" t="s">
+      <c r="D77" s="42" t="s">
         <v>718</v>
       </c>
       <c r="E77" s="6" t="s">
@@ -7007,10 +6980,10 @@
       </c>
       <c r="H77" s="11"/>
       <c r="K77" s="11"/>
-      <c r="L77" s="42" t="s">
+      <c r="L77" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M77" s="44">
+      <c r="M77" s="43">
         <v>45548.0</v>
       </c>
       <c r="N77" s="16"/>
@@ -7040,16 +7013,16 @@
       <c r="AH77" s="7"/>
     </row>
     <row r="78">
-      <c r="A78" s="42" t="s">
+      <c r="A78" s="41" t="s">
         <v>725</v>
       </c>
-      <c r="B78" s="42" t="s">
+      <c r="B78" s="41" t="s">
         <v>726</v>
       </c>
-      <c r="C78" s="42" t="s">
+      <c r="C78" s="41" t="s">
         <v>727</v>
       </c>
-      <c r="D78" s="43" t="s">
+      <c r="D78" s="42" t="s">
         <v>718</v>
       </c>
       <c r="E78" s="6" t="s">
@@ -7060,13 +7033,13 @@
         <v>506</v>
       </c>
       <c r="H78" s="11"/>
-      <c r="K78" s="42" t="s">
+      <c r="K78" s="41" t="s">
         <v>728</v>
       </c>
-      <c r="L78" s="42" t="s">
+      <c r="L78" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M78" s="44">
+      <c r="M78" s="43">
         <v>45548.0</v>
       </c>
       <c r="N78" s="16"/>
@@ -7096,16 +7069,16 @@
       <c r="AH78" s="7"/>
     </row>
     <row r="79">
-      <c r="A79" s="42" t="s">
+      <c r="A79" s="41" t="s">
         <v>729</v>
       </c>
-      <c r="B79" s="42" t="s">
+      <c r="B79" s="41" t="s">
         <v>730</v>
       </c>
-      <c r="C79" s="42" t="s">
+      <c r="C79" s="41" t="s">
         <v>731</v>
       </c>
-      <c r="D79" s="43" t="s">
+      <c r="D79" s="42" t="s">
         <v>718</v>
       </c>
       <c r="E79" s="6" t="s">
@@ -7117,10 +7090,10 @@
       </c>
       <c r="H79" s="11"/>
       <c r="K79" s="11"/>
-      <c r="L79" s="42" t="s">
+      <c r="L79" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M79" s="44">
+      <c r="M79" s="43">
         <v>45548.0</v>
       </c>
       <c r="N79" s="16"/>
@@ -7150,16 +7123,16 @@
       <c r="AH79" s="7"/>
     </row>
     <row r="80">
-      <c r="A80" s="42" t="s">
+      <c r="A80" s="41" t="s">
         <v>732</v>
       </c>
-      <c r="B80" s="42" t="s">
+      <c r="B80" s="41" t="s">
         <v>733</v>
       </c>
-      <c r="C80" s="42" t="s">
+      <c r="C80" s="41" t="s">
         <v>734</v>
       </c>
-      <c r="D80" s="43" t="s">
+      <c r="D80" s="42" t="s">
         <v>718</v>
       </c>
       <c r="E80" s="6" t="s">
@@ -7171,10 +7144,10 @@
       </c>
       <c r="H80" s="11"/>
       <c r="K80" s="11"/>
-      <c r="L80" s="42" t="s">
+      <c r="L80" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M80" s="44">
+      <c r="M80" s="43">
         <v>45548.0</v>
       </c>
       <c r="N80" s="16"/>
@@ -7204,16 +7177,16 @@
       <c r="AH80" s="7"/>
     </row>
     <row r="81">
-      <c r="A81" s="42" t="s">
+      <c r="A81" s="41" t="s">
         <v>735</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="B81" s="41" t="s">
         <v>736</v>
       </c>
-      <c r="C81" s="42" t="s">
+      <c r="C81" s="41" t="s">
         <v>737</v>
       </c>
-      <c r="D81" s="43" t="s">
+      <c r="D81" s="42" t="s">
         <v>738</v>
       </c>
       <c r="E81" s="6" t="s">
@@ -7225,10 +7198,10 @@
       </c>
       <c r="H81" s="11"/>
       <c r="K81" s="11"/>
-      <c r="L81" s="42" t="s">
+      <c r="L81" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="M81" s="44">
+      <c r="M81" s="43">
         <v>45548.0</v>
       </c>
       <c r="N81" s="16"/>
@@ -10452,7 +10425,7 @@
       <c r="G29" s="25"/>
       <c r="H29" s="25"/>
       <c r="I29" s="25"/>
-      <c r="J29" s="36" t="s">
+      <c r="J29" s="26" t="s">
         <v>251</v>
       </c>
       <c r="K29" s="27">
@@ -10543,10 +10516,7 @@
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="J29"/>
-  </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10625,7 +10595,7 @@
       <c r="B2" s="5"/>
       <c r="D2" s="8"/>
       <c r="I2" s="8"/>
-      <c r="K2" s="37"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3">
       <c r="A3" s="35" t="s">
@@ -11157,7 +11127,7 @@
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
-      <c r="J14" s="36" t="s">
+      <c r="J14" s="37" t="s">
         <v>294</v>
       </c>
       <c r="K14" s="27">
@@ -13296,7 +13266,7 @@
         <v>429</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="K2" s="37">
+      <c r="K2" s="36">
         <v>45410.0</v>
       </c>
       <c r="L2" s="7"/>

</xml_diff>

<commit_message>
fix definitions,typos, and links in AI, EU-AIAct
- typos in definition of concepts
- broken or missing links (fixed using anchor macro)
- updated definitions in EU-AIAct to published version

Co-authored-by: Delaram Golpayegani <sgolpays@tcd.ie>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ai.xlsx
+++ b/code/vocab_csv/ai.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="768">
   <si>
     <t>Term</t>
   </si>
@@ -1726,7 +1726,10 @@
     <t>Input Data Noise</t>
   </si>
   <si>
-    <t>Concept representing input data being noise</t>
+    <t>Concept representing input data being noisy</t>
+  </si>
+  <si>
+    <t>modified</t>
   </si>
   <si>
     <t>InputDataSparse</t>
@@ -1780,7 +1783,7 @@
     <t>Input Data Misinterpretation</t>
   </si>
   <si>
-    <t>Concept representing input data being misinterpretation</t>
+    <t>Concept representing input data being misinterpreted</t>
   </si>
   <si>
     <t>InputDataUnrepresentative</t>
@@ -1864,7 +1867,7 @@
     <t>Testing Data Noise</t>
   </si>
   <si>
-    <t>Concept representing testing data being noise</t>
+    <t>Concept representing testing data being noisy</t>
   </si>
   <si>
     <t>TestingDataSparse</t>
@@ -1918,7 +1921,7 @@
     <t>Testing Data Misinterpretation</t>
   </si>
   <si>
-    <t>Concept representing testing data being misinterpretation</t>
+    <t>Concept representing testing data being misinterpreted</t>
   </si>
   <si>
     <t>TestingDataUnrepresentative</t>
@@ -2002,7 +2005,7 @@
     <t>Validation Data Noise</t>
   </si>
   <si>
-    <t>Concept representing validation data being noise</t>
+    <t>Concept representing validation data being noisy</t>
   </si>
   <si>
     <t>ValidationDataSparse</t>
@@ -2056,7 +2059,7 @@
     <t>Validation Data Misinterpretation</t>
   </si>
   <si>
-    <t>Concept representing validation data being misinterpretation</t>
+    <t>Concept representing validation data being misinterpreted</t>
   </si>
   <si>
     <t>ValidationDataUnrepresentative</t>
@@ -2210,7 +2213,7 @@
     <t>Automation Bias</t>
   </si>
   <si>
-    <t>Bias tha occurs due to propensity for humans to favour suggestions from automated decision-making systems and to ignore contradictory information made without automation, even if it is correct</t>
+    <t>Bias that occurs due to propensity for humans to favour suggestions from automated decision-making systems and to ignore contradictory information made without automation, even if it is correct</t>
   </si>
   <si>
     <t>ai:AIBias,risk:CognitiveBias</t>
@@ -2529,7 +2532,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2682,6 +2685,9 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4667,7 +4673,6 @@
       <c r="E11" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="F11" s="7"/>
       <c r="G11" s="6" t="s">
         <v>534</v>
       </c>
@@ -4679,9 +4684,11 @@
       <c r="M11" s="9">
         <v>45627.0</v>
       </c>
-      <c r="N11" s="7"/>
+      <c r="N11" s="9">
+        <v>45868.0</v>
+      </c>
       <c r="O11" s="6" t="s">
-        <v>21</v>
+        <v>559</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>22</v>
@@ -4707,13 +4714,13 @@
     </row>
     <row r="12">
       <c r="A12" s="27" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>546</v>
@@ -4761,13 +4768,13 @@
     </row>
     <row r="13">
       <c r="A13" s="27" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>546</v>
@@ -4815,13 +4822,13 @@
     </row>
     <row r="14">
       <c r="A14" s="27" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>546</v>
@@ -4869,13 +4876,13 @@
     </row>
     <row r="15">
       <c r="A15" s="27" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>546</v>
@@ -4923,13 +4930,13 @@
     </row>
     <row r="16">
       <c r="A16" s="27" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>546</v>
@@ -4977,13 +4984,13 @@
     </row>
     <row r="17">
       <c r="A17" s="27" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>546</v>
@@ -4991,53 +4998,31 @@
       <c r="E17" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="F17" s="7"/>
       <c r="G17" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
       <c r="M17" s="9">
         <v>45627.0</v>
       </c>
-      <c r="N17" s="7"/>
+      <c r="N17" s="9">
+        <v>45868.0</v>
+      </c>
       <c r="O17" s="6" t="s">
-        <v>21</v>
+        <v>559</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="7"/>
-      <c r="AA17" s="7"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="7"/>
-      <c r="AE17" s="7"/>
-      <c r="AF17" s="7"/>
-      <c r="AG17" s="7"/>
-      <c r="AH17" s="7"/>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>546</v>
@@ -5085,13 +5070,13 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>546</v>
@@ -5139,13 +5124,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>546</v>
@@ -5196,13 +5181,13 @@
     </row>
     <row r="22">
       <c r="A22" s="36" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>542</v>
@@ -5250,16 +5235,16 @@
     </row>
     <row r="23">
       <c r="A23" s="27" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>533</v>
@@ -5304,16 +5289,16 @@
     </row>
     <row r="24">
       <c r="A24" s="27" t="s">
+        <v>594</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>595</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>593</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>594</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>595</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>592</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>533</v>
@@ -5358,16 +5343,16 @@
     </row>
     <row r="25">
       <c r="A25" s="27" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>533</v>
@@ -5412,16 +5397,16 @@
     </row>
     <row r="26">
       <c r="A26" s="27" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>533</v>
@@ -5466,70 +5451,48 @@
     </row>
     <row r="27">
       <c r="A27" s="27" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="F27" s="7"/>
       <c r="G27" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
       <c r="M27" s="9">
         <v>45627.0</v>
       </c>
-      <c r="N27" s="7"/>
+      <c r="N27" s="9">
+        <v>45868.0</v>
+      </c>
       <c r="O27" s="6" t="s">
-        <v>21</v>
+        <v>559</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="7"/>
-      <c r="Z27" s="7"/>
-      <c r="AA27" s="7"/>
-      <c r="AB27" s="7"/>
-      <c r="AC27" s="7"/>
-      <c r="AD27" s="7"/>
-      <c r="AE27" s="7"/>
-      <c r="AF27" s="7"/>
-      <c r="AG27" s="7"/>
-      <c r="AH27" s="7"/>
     </row>
     <row r="28">
       <c r="A28" s="27" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>533</v>
@@ -5574,16 +5537,16 @@
     </row>
     <row r="29">
       <c r="A29" s="27" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>533</v>
@@ -5628,16 +5591,16 @@
     </row>
     <row r="30">
       <c r="A30" s="27" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>533</v>
@@ -5682,16 +5645,16 @@
     </row>
     <row r="31">
       <c r="A31" s="27" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>533</v>
@@ -5736,16 +5699,16 @@
     </row>
     <row r="32">
       <c r="A32" s="27" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>533</v>
@@ -5790,70 +5753,48 @@
     </row>
     <row r="33">
       <c r="A33" s="27" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="F33" s="7"/>
       <c r="G33" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
       <c r="M33" s="9">
         <v>45627.0</v>
       </c>
-      <c r="N33" s="7"/>
+      <c r="N33" s="9">
+        <v>45868.0</v>
+      </c>
       <c r="O33" s="6" t="s">
-        <v>21</v>
+        <v>559</v>
       </c>
       <c r="P33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
-      <c r="V33" s="7"/>
-      <c r="W33" s="7"/>
-      <c r="X33" s="7"/>
-      <c r="Y33" s="7"/>
-      <c r="Z33" s="7"/>
-      <c r="AA33" s="7"/>
-      <c r="AB33" s="7"/>
-      <c r="AC33" s="7"/>
-      <c r="AD33" s="7"/>
-      <c r="AE33" s="7"/>
-      <c r="AF33" s="7"/>
-      <c r="AG33" s="7"/>
-      <c r="AH33" s="7"/>
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>533</v>
@@ -5898,16 +5839,16 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>533</v>
@@ -5952,16 +5893,16 @@
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>533</v>
@@ -6010,13 +5951,13 @@
     </row>
     <row r="38">
       <c r="A38" s="36" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>542</v>
@@ -6064,16 +6005,16 @@
     </row>
     <row r="39">
       <c r="A39" s="27" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>533</v>
@@ -6118,16 +6059,16 @@
     </row>
     <row r="40">
       <c r="A40" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>641</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>639</v>
-      </c>
-      <c r="B40" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>641</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>638</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>533</v>
@@ -6172,16 +6113,16 @@
     </row>
     <row r="41">
       <c r="A41" s="27" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>533</v>
@@ -6226,16 +6167,16 @@
     </row>
     <row r="42">
       <c r="A42" s="27" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>533</v>
@@ -6280,70 +6221,48 @@
     </row>
     <row r="43">
       <c r="A43" s="27" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="F43" s="7"/>
       <c r="G43" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
       <c r="M43" s="9">
         <v>45627.0</v>
       </c>
-      <c r="N43" s="7"/>
+      <c r="N43" s="9">
+        <v>45868.0</v>
+      </c>
       <c r="O43" s="6" t="s">
-        <v>21</v>
+        <v>559</v>
       </c>
       <c r="P43" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="7"/>
-      <c r="S43" s="7"/>
-      <c r="T43" s="7"/>
-      <c r="U43" s="7"/>
-      <c r="V43" s="7"/>
-      <c r="W43" s="7"/>
-      <c r="X43" s="7"/>
-      <c r="Y43" s="7"/>
-      <c r="Z43" s="7"/>
-      <c r="AA43" s="7"/>
-      <c r="AB43" s="7"/>
-      <c r="AC43" s="7"/>
-      <c r="AD43" s="7"/>
-      <c r="AE43" s="7"/>
-      <c r="AF43" s="7"/>
-      <c r="AG43" s="7"/>
-      <c r="AH43" s="7"/>
     </row>
     <row r="44">
       <c r="A44" s="27" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>533</v>
@@ -6388,16 +6307,16 @@
     </row>
     <row r="45">
       <c r="A45" s="27" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>533</v>
@@ -6442,16 +6361,16 @@
     </row>
     <row r="46">
       <c r="A46" s="27" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>533</v>
@@ -6496,16 +6415,16 @@
     </row>
     <row r="47">
       <c r="A47" s="27" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>533</v>
@@ -6550,16 +6469,16 @@
     </row>
     <row r="48">
       <c r="A48" s="27" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>533</v>
@@ -6604,70 +6523,48 @@
     </row>
     <row r="49">
       <c r="A49" s="27" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="F49" s="7"/>
       <c r="G49" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
       <c r="M49" s="9">
         <v>45627.0</v>
       </c>
-      <c r="N49" s="7"/>
+      <c r="N49" s="9">
+        <v>45868.0</v>
+      </c>
       <c r="O49" s="6" t="s">
-        <v>21</v>
+        <v>559</v>
       </c>
       <c r="P49" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q49" s="7"/>
-      <c r="R49" s="7"/>
-      <c r="S49" s="7"/>
-      <c r="T49" s="7"/>
-      <c r="U49" s="7"/>
-      <c r="V49" s="7"/>
-      <c r="W49" s="7"/>
-      <c r="X49" s="7"/>
-      <c r="Y49" s="7"/>
-      <c r="Z49" s="7"/>
-      <c r="AA49" s="7"/>
-      <c r="AB49" s="7"/>
-      <c r="AC49" s="7"/>
-      <c r="AD49" s="7"/>
-      <c r="AE49" s="7"/>
-      <c r="AF49" s="7"/>
-      <c r="AG49" s="7"/>
-      <c r="AH49" s="7"/>
     </row>
     <row r="50">
       <c r="A50" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>533</v>
@@ -6712,16 +6609,16 @@
     </row>
     <row r="51">
       <c r="A51" s="6" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>533</v>
@@ -6766,16 +6663,16 @@
     </row>
     <row r="52">
       <c r="A52" s="6" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>533</v>
@@ -6823,13 +6720,13 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>538</v>
@@ -6877,26 +6774,26 @@
     </row>
     <row r="55">
       <c r="A55" s="27" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>533</v>
       </c>
       <c r="F55" s="26"/>
       <c r="G55" s="27" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="H55" s="27" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="I55" s="26"/>
       <c r="J55" s="26"/>
@@ -6933,26 +6830,26 @@
     </row>
     <row r="56">
       <c r="A56" s="27" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C56" s="26" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>533</v>
       </c>
       <c r="F56" s="26"/>
       <c r="G56" s="27" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="H56" s="27" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="I56" s="26"/>
       <c r="J56" s="26"/>
@@ -6989,31 +6886,31 @@
     </row>
     <row r="57">
       <c r="A57" s="27" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="C57" s="26" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>533</v>
       </c>
       <c r="F57" s="26"/>
       <c r="G57" s="27" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="H57" s="27" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="I57" s="26"/>
       <c r="J57" s="26"/>
       <c r="K57" s="6" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="L57" s="26"/>
       <c r="M57" s="9">
@@ -7047,31 +6944,31 @@
     </row>
     <row r="58">
       <c r="A58" s="27" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C58" s="26" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>533</v>
       </c>
       <c r="F58" s="26"/>
       <c r="G58" s="27" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="H58" s="27" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="I58" s="26"/>
       <c r="J58" s="26"/>
       <c r="K58" s="45" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="L58" s="26"/>
       <c r="M58" s="9">
@@ -7108,13 +7005,13 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>538</v>
@@ -7165,13 +7062,13 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>538</v>
@@ -7222,13 +7119,13 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>538</v>
@@ -7276,16 +7173,16 @@
     </row>
     <row r="66">
       <c r="A66" s="15" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C66" s="50" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>533</v>
@@ -7305,7 +7202,7 @@
         <v>21</v>
       </c>
       <c r="P66" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q66" s="11"/>
       <c r="R66" s="11"/>
@@ -7328,16 +7225,16 @@
     </row>
     <row r="67">
       <c r="A67" s="50" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B67" s="50" t="s">
-        <v>714</v>
-      </c>
-      <c r="C67" s="50" t="s">
         <v>715</v>
       </c>
+      <c r="C67" s="51" t="s">
+        <v>716</v>
+      </c>
       <c r="D67" s="51" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>533</v>
@@ -7349,17 +7246,19 @@
       <c r="H67" s="11"/>
       <c r="K67" s="11"/>
       <c r="L67" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M67" s="52">
         <v>45548.0</v>
       </c>
-      <c r="N67" s="17"/>
-      <c r="O67" s="11" t="s">
-        <v>21</v>
+      <c r="N67" s="53">
+        <v>45868.0</v>
+      </c>
+      <c r="O67" s="10" t="s">
+        <v>559</v>
       </c>
       <c r="P67" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q67" s="11"/>
       <c r="R67" s="11"/>
@@ -7377,21 +7276,19 @@
       <c r="AD67" s="26"/>
       <c r="AE67" s="26"/>
       <c r="AF67" s="26"/>
-      <c r="AG67" s="7"/>
-      <c r="AH67" s="7"/>
     </row>
     <row r="68">
       <c r="A68" s="50" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B68" s="50" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C68" s="50" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="D68" s="51" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>533</v>
@@ -7403,7 +7300,7 @@
       <c r="H68" s="11"/>
       <c r="K68" s="11"/>
       <c r="L68" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M68" s="52">
         <v>45548.0</v>
@@ -7413,7 +7310,7 @@
         <v>21</v>
       </c>
       <c r="P68" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q68" s="11"/>
       <c r="R68" s="11"/>
@@ -7436,16 +7333,16 @@
     </row>
     <row r="69">
       <c r="A69" s="50" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B69" s="50" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C69" s="50" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="D69" s="51" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>533</v>
@@ -7457,17 +7354,17 @@
       <c r="H69" s="11"/>
       <c r="K69" s="11"/>
       <c r="L69" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M69" s="52">
         <v>45548.0</v>
       </c>
-      <c r="N69" s="17"/>
-      <c r="O69" s="11" t="s">
+      <c r="N69" s="53"/>
+      <c r="O69" s="10" t="s">
         <v>21</v>
       </c>
       <c r="P69" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q69" s="11"/>
       <c r="R69" s="11"/>
@@ -7490,16 +7387,16 @@
     </row>
     <row r="70">
       <c r="A70" s="50" t="s">
+        <v>727</v>
+      </c>
+      <c r="B70" s="50" t="s">
+        <v>728</v>
+      </c>
+      <c r="C70" s="50" t="s">
+        <v>729</v>
+      </c>
+      <c r="D70" s="51" t="s">
         <v>726</v>
-      </c>
-      <c r="B70" s="50" t="s">
-        <v>727</v>
-      </c>
-      <c r="C70" s="50" t="s">
-        <v>728</v>
-      </c>
-      <c r="D70" s="51" t="s">
-        <v>725</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>533</v>
@@ -7511,7 +7408,7 @@
       <c r="H70" s="11"/>
       <c r="K70" s="11"/>
       <c r="L70" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M70" s="52">
         <v>45548.0</v>
@@ -7521,7 +7418,7 @@
         <v>21</v>
       </c>
       <c r="P70" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q70" s="11"/>
       <c r="R70" s="11"/>
@@ -7544,16 +7441,16 @@
     </row>
     <row r="71">
       <c r="A71" s="50" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B71" s="50" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C71" s="50" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D71" s="51" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>533</v>
@@ -7564,10 +7461,10 @@
       </c>
       <c r="H71" s="11"/>
       <c r="K71" s="50" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="L71" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M71" s="52">
         <v>45548.0</v>
@@ -7577,7 +7474,7 @@
         <v>21</v>
       </c>
       <c r="P71" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q71" s="11"/>
       <c r="R71" s="11"/>
@@ -7600,16 +7497,16 @@
     </row>
     <row r="72">
       <c r="A72" s="50" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B72" s="50" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C72" s="50" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="D72" s="51" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>533</v>
@@ -7621,7 +7518,7 @@
       <c r="H72" s="11"/>
       <c r="K72" s="11"/>
       <c r="L72" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M72" s="52">
         <v>45548.0</v>
@@ -7631,7 +7528,7 @@
         <v>21</v>
       </c>
       <c r="P72" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q72" s="11"/>
       <c r="R72" s="11"/>
@@ -7654,16 +7551,16 @@
     </row>
     <row r="73">
       <c r="A73" s="50" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B73" s="50" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C73" s="50" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="D73" s="51" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>533</v>
@@ -7675,7 +7572,7 @@
       <c r="H73" s="11"/>
       <c r="K73" s="11"/>
       <c r="L73" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M73" s="52">
         <v>45548.0</v>
@@ -7685,7 +7582,7 @@
         <v>21</v>
       </c>
       <c r="P73" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q73" s="11"/>
       <c r="R73" s="11"/>
@@ -7708,16 +7605,16 @@
     </row>
     <row r="74">
       <c r="A74" s="50" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B74" s="50" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C74" s="50" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="D74" s="51" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>533</v>
@@ -7728,10 +7625,10 @@
       </c>
       <c r="H74" s="11"/>
       <c r="K74" s="50" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="L74" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M74" s="52">
         <v>45548.0</v>
@@ -7741,7 +7638,7 @@
         <v>21</v>
       </c>
       <c r="P74" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q74" s="11"/>
       <c r="R74" s="11"/>
@@ -7764,16 +7661,16 @@
     </row>
     <row r="75">
       <c r="A75" s="50" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B75" s="50" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C75" s="50" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="D75" s="51" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>533</v>
@@ -7785,7 +7682,7 @@
       <c r="H75" s="11"/>
       <c r="K75" s="11"/>
       <c r="L75" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M75" s="52">
         <v>45548.0</v>
@@ -7795,7 +7692,7 @@
         <v>21</v>
       </c>
       <c r="P75" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q75" s="11"/>
       <c r="R75" s="11"/>
@@ -7818,16 +7715,16 @@
     </row>
     <row r="76">
       <c r="A76" s="50" t="s">
+        <v>748</v>
+      </c>
+      <c r="B76" s="50" t="s">
+        <v>749</v>
+      </c>
+      <c r="C76" s="50" t="s">
+        <v>750</v>
+      </c>
+      <c r="D76" s="51" t="s">
         <v>747</v>
-      </c>
-      <c r="B76" s="50" t="s">
-        <v>748</v>
-      </c>
-      <c r="C76" s="50" t="s">
-        <v>749</v>
-      </c>
-      <c r="D76" s="51" t="s">
-        <v>746</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>533</v>
@@ -7839,7 +7736,7 @@
       <c r="H76" s="11"/>
       <c r="K76" s="11"/>
       <c r="L76" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M76" s="52">
         <v>45548.0</v>
@@ -7849,7 +7746,7 @@
         <v>21</v>
       </c>
       <c r="P76" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q76" s="11"/>
       <c r="R76" s="11"/>
@@ -7872,16 +7769,16 @@
     </row>
     <row r="77">
       <c r="A77" s="50" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B77" s="50" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C77" s="50" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="D77" s="51" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>533</v>
@@ -7893,7 +7790,7 @@
       <c r="H77" s="11"/>
       <c r="K77" s="11"/>
       <c r="L77" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M77" s="52">
         <v>45548.0</v>
@@ -7903,7 +7800,7 @@
         <v>21</v>
       </c>
       <c r="P77" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q77" s="11"/>
       <c r="R77" s="11"/>
@@ -7926,16 +7823,16 @@
     </row>
     <row r="78">
       <c r="A78" s="50" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B78" s="50" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C78" s="50" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="D78" s="51" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>533</v>
@@ -7946,10 +7843,10 @@
       </c>
       <c r="H78" s="11"/>
       <c r="K78" s="50" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="L78" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M78" s="52">
         <v>45548.0</v>
@@ -7959,7 +7856,7 @@
         <v>21</v>
       </c>
       <c r="P78" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q78" s="11"/>
       <c r="R78" s="11"/>
@@ -7982,16 +7879,16 @@
     </row>
     <row r="79">
       <c r="A79" s="50" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B79" s="50" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C79" s="50" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="D79" s="51" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>533</v>
@@ -8003,7 +7900,7 @@
       <c r="H79" s="11"/>
       <c r="K79" s="11"/>
       <c r="L79" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M79" s="52">
         <v>45548.0</v>
@@ -8013,7 +7910,7 @@
         <v>21</v>
       </c>
       <c r="P79" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q79" s="11"/>
       <c r="R79" s="11"/>
@@ -8036,16 +7933,16 @@
     </row>
     <row r="80">
       <c r="A80" s="50" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B80" s="50" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C80" s="50" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="D80" s="51" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>533</v>
@@ -8057,7 +7954,7 @@
       <c r="H80" s="11"/>
       <c r="K80" s="11"/>
       <c r="L80" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M80" s="52">
         <v>45548.0</v>
@@ -8067,7 +7964,7 @@
         <v>21</v>
       </c>
       <c r="P80" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q80" s="11"/>
       <c r="R80" s="11"/>
@@ -8090,16 +7987,16 @@
     </row>
     <row r="81">
       <c r="A81" s="50" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B81" s="50" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="C81" s="50" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="D81" s="51" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>533</v>
@@ -8111,7 +8008,7 @@
       <c r="H81" s="11"/>
       <c r="K81" s="11"/>
       <c r="L81" s="50" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M81" s="52">
         <v>45548.0</v>
@@ -8121,7 +8018,7 @@
         <v>21</v>
       </c>
       <c r="P81" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q81" s="11"/>
       <c r="R81" s="11"/>

</xml_diff>

<commit_message>
fixes typos submitted by @bact in #327 and others
- this commit includes fixes to typos in RDF and HTML but without any
  breaking changes (e.g. they are in definitions, notes)
- all typos identified and fixed by @bact (see #327 and PRs)
- this commit essentially regenrates all RDF and HTML outputs, so there
  may be outputs/changes from other commits also expressed here
- one change included is "Example" title in RDF files

Co-authored-by: Arthit Suriyawongkul <arthit@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ai.xlsx
+++ b/code/vocab_csv/ai.xlsx
@@ -321,7 +321,7 @@
     <t>NarrowAI</t>
   </si>
   <si>
-    <t xml:space="preserve">Narrow AI </t>
+    <t>Narrow AI</t>
   </si>
   <si>
     <t>Type of AI system that is focused on defined tasks to address a specific problem i.e. it addresses a narrow scope of tasks and problems</t>
@@ -342,7 +342,7 @@
     <t>IndustrialRobot</t>
   </si>
   <si>
-    <t xml:space="preserve">Industrial Robot </t>
+    <t>Industrial Robot</t>
   </si>
   <si>
     <t>A robot or robotic system for use in industrial automation applications</t>
@@ -396,7 +396,7 @@
     <t>Machine Learning Model</t>
   </si>
   <si>
-    <t>Mathematical construct that generates an inference or prediction  based on input data or information</t>
+    <t>Mathematical construct that generates an inference or prediction based on input data or information</t>
   </si>
   <si>
     <t>ISO/IEC 22989:2022 3.3.7</t>
@@ -414,7 +414,7 @@
     <t>MachineLearningPlatform</t>
   </si>
   <si>
-    <t xml:space="preserve">Machine Learning Platform </t>
+    <t>Machine Learning Platform</t>
   </si>
   <si>
     <t>Technology platform for developing, deploying, and managing machine learning models and resources</t>
@@ -543,7 +543,7 @@
     <t>Machine Learning</t>
   </si>
   <si>
-    <t>Process of optimizing model parameters through computational techniques, such that the model's behaviour reflects the data or experience</t>
+    <t>Process of optimising model parameters through computational techniques, such that the model's behaviour reflects the data or experience</t>
   </si>
   <si>
     <t>ISO/IEC 22989:2022 3.3.5</t>
@@ -570,10 +570,10 @@
     <t>ReinforcementLearning</t>
   </si>
   <si>
-    <t xml:space="preserve">Reinforcement Learning </t>
-  </si>
-  <si>
-    <t>Learning of an optimal sequence of actions to maximize a reward through interaction with an environment</t>
+    <t>Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>Learning of an optimal sequence of actions to maximise a reward through interaction with an environment</t>
   </si>
   <si>
     <t>ISO/IEC 22989:2022 3.3.9</t>
@@ -585,7 +585,7 @@
     <t>Semi Supervised Learning</t>
   </si>
   <si>
-    <t xml:space="preserve">Machine learning that makes use of both labelled and unlabelled data during training </t>
+    <t>Machine learning that makes use of both labelled and unlabelled data during training</t>
   </si>
   <si>
     <t>ISO/IEC 22989:2022 3.3.11</t>
@@ -663,7 +663,7 @@
     <t>FeedForwardNeuralNetwork</t>
   </si>
   <si>
-    <t xml:space="preserve">Feed Forward Neural Network </t>
+    <t>Feed Forward Neural Network</t>
   </si>
   <si>
     <t>Neural network where information is fed from the input layer to the output layer in one direction only</t>
@@ -681,7 +681,7 @@
     <t>Convolutional Neural Network (CNN)</t>
   </si>
   <si>
-    <t>Feed forward neural network using convolution  in at least one of its layers</t>
+    <t>Feed forward neural network using convolution in at least one of its layers</t>
   </si>
   <si>
     <t>ISO/IEC 22989:2022 3.4.2</t>
@@ -744,7 +744,7 @@
     <t>BayesianOptimisation</t>
   </si>
   <si>
-    <t xml:space="preserve">Bayesian Optimisation </t>
+    <t>Bayesian Optimisation</t>
   </si>
   <si>
     <t>Refers to Bayesian optimisation technique</t>
@@ -753,7 +753,7 @@
     <t>BayesianNetwork</t>
   </si>
   <si>
-    <t xml:space="preserve">Bayesian Network </t>
+    <t>Bayesian Network</t>
   </si>
   <si>
     <t>Probabilistic technique that uses Bayesian inference for probability computations using a directed acyclic graph</t>
@@ -777,7 +777,7 @@
     <t>Search Method</t>
   </si>
   <si>
-    <t xml:space="preserve">Refers to statistical-based search Methods </t>
+    <t>Refers to statistical-based search Methods</t>
   </si>
   <si>
     <t>AudioProcessing</t>
@@ -786,7 +786,7 @@
     <t>Audio Processing</t>
   </si>
   <si>
-    <t xml:space="preserve">Technique involving processing audio </t>
+    <t>Technique involving processing audio</t>
   </si>
   <si>
     <t>(AI Watch,https://ai-watch.ec.europa.eu/);(Defining Artificial Intelligence 2.0,https://publications.jrc.ec.europa.eu/repository/handle/JRC126426)</t>
@@ -828,7 +828,7 @@
     <t>Symbolic Reasoning</t>
   </si>
   <si>
-    <t xml:space="preserve">Reasoning based on the knowledge encoded in a formal language </t>
+    <t>Reasoning based on the knowledge encoded in a formal language</t>
   </si>
   <si>
     <t>LogicTechnique</t>
@@ -951,7 +951,7 @@
     <t>Biometric Categorisation</t>
   </si>
   <si>
-    <t xml:space="preserve">Capability involving assigning natural persons to specific categories based on their biometric data </t>
+    <t>Capability involving assigning natural persons to specific categories based on their biometric data</t>
   </si>
   <si>
     <t>ai:BiometricCapability</t>
@@ -1015,7 +1015,7 @@
     <t>Real-Time Biometric Identification</t>
   </si>
   <si>
-    <t>Capability involving biometric identification carried out in real-time or instataneously</t>
+    <t>Capability involving biometric identification carried out in real-time or instantaneously</t>
   </si>
   <si>
     <t>PostTimeBiometricIdentification</t>
@@ -1024,7 +1024,7 @@
     <t>Post-Time Biometric Identification</t>
   </si>
   <si>
-    <t>Capability involving biometric identification carried out later or not in real-time or not-instaneously</t>
+    <t>Capability involving biometric identification carried out later or not in real-time or non-instantaneously</t>
   </si>
   <si>
     <t>EmotionRecognition</t>
@@ -1033,7 +1033,7 @@
     <t>Emotion Recognition</t>
   </si>
   <si>
-    <t>Capability for identifying and categorizing emotions expressed in a piece of text, speech, video or image or combination thereof</t>
+    <t>Capability for identifying and categorising emotions expressed in a piece of text, speech, video or image or combination thereof</t>
   </si>
   <si>
     <t>ISO/IEC 22989:2022 3.6.3</t>
@@ -1045,7 +1045,7 @@
     <t>Biometric Emotion Recognition</t>
   </si>
   <si>
-    <t>Capability for recognisting emtions based on biometrics information</t>
+    <t>Capability for recognising emotions based on biometrics information</t>
   </si>
   <si>
     <t>ai:EmotionRecognition</t>
@@ -1129,7 +1129,7 @@
     <t>Object Recognition</t>
   </si>
   <si>
-    <t xml:space="preserve">Capability to recognise objects </t>
+    <t>Capability to recognise objects</t>
   </si>
   <si>
     <t>ai:ComputerVision</t>
@@ -1165,7 +1165,7 @@
     <t>Music Information Retrieval (MIR)</t>
   </si>
   <si>
-    <t>Capability for retrieving, analyzing, and categorizing music-related information such as audio files, melodies, or lyrics using audio features, metadata, and user queries</t>
+    <t>Capability for retrieving, analysing, and categorising music-related information such as audio files, melodies, or lyrics using audio features, metadata, and user queries</t>
   </si>
   <si>
     <t>ai:InformationRetrieval</t>
@@ -1228,7 +1228,7 @@
     <t>Named Entity Recognition</t>
   </si>
   <si>
-    <t>Capability for recognizing and labelling the denotational names of entities and their categories for sequences of words in a stream of text or speech</t>
+    <t>Capability for recognising and labelling the denotational names of entities and their categories for sequences of words in a stream of text or speech</t>
   </si>
   <si>
     <t>ISO/IEC 22989:2022 3.6.6</t>
@@ -1288,7 +1288,7 @@
     <t>Sentiment Analysis</t>
   </si>
   <si>
-    <t>Capability for computationally identifying and categorizing opinions expressed in a piece of text, speech or image, to determine a range of feeling such as from positive to negative</t>
+    <t>Capability for computationally identifying and categorising opinions expressed in a piece of text, speech or image, to determine a range of feeling such as from positive to negative</t>
   </si>
   <si>
     <t>ai:HumanOrientedCapability,ai:LanguageCapability</t>
@@ -1312,13 +1312,13 @@
     <t>ISO/IEC 22989:2022 3.6.1</t>
   </si>
   <si>
-    <t xml:space="preserve">DialogueManagement </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dialogue Management </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capability for choosing the appropriate next move in a dialogue based on user input, the dialogue history and other contextual knowledge to meet a desired goal </t>
+    <t>DialogueManagement</t>
+  </si>
+  <si>
+    <t>Dialogue Management</t>
+  </si>
+  <si>
+    <t>Capability for choosing the appropriate next move in a dialogue based on user input, the dialogue history and other contextual knowledge to meet a desired goal</t>
   </si>
   <si>
     <t>ContentGeneration</t>
@@ -1375,7 +1375,7 @@
     <t>Sensitive Attribute Inference</t>
   </si>
   <si>
-    <t>The capability of infering sensitive or protected attributes or characteristics</t>
+    <t>The capability of inferring sensitive or protected attributes or characteristics</t>
   </si>
   <si>
     <t>Measure</t>
@@ -1408,7 +1408,7 @@
     <t>Inception Stage</t>
   </si>
   <si>
-    <t xml:space="preserve">The stage in the lifecycle where inception regarding AI occurs and one or more stakeholders decide to turn an idea into a tangible system </t>
+    <t>The stage in the lifecycle where inception regarding AI occurs and one or more stakeholders decide to turn an idea into a tangible system</t>
   </si>
   <si>
     <t>ai:LifecycleStage</t>
@@ -1456,7 +1456,7 @@
     <t>Deployment Stage</t>
   </si>
   <si>
-    <t>The stage in the lifecycle where  the AI system is installed, released or configured for deployment and operation in a target environment</t>
+    <t>The stage in the lifecycle where the AI system is installed, released or configured for deployment and operation in a target environment</t>
   </si>
   <si>
     <t>OperationStage</t>
@@ -1486,7 +1486,7 @@
     <t>Repair Stage</t>
   </si>
   <si>
-    <t>The stage in the lifecycle where  an AI system is being repaired due to suspected or occured incidents</t>
+    <t>The stage in the lifecycle where an AI system is being repaired due to suspected or occurred incidents</t>
   </si>
   <si>
     <t>UpdateStage</t>
@@ -1522,7 +1522,7 @@
     <t>Retirement Stage</t>
   </si>
   <si>
-    <t xml:space="preserve">The stage in the lifecycle where the AI system is retired and becomes obsolete </t>
+    <t>The stage in the lifecycle where the AI system is retired and becomes obsolete</t>
   </si>
   <si>
     <t>DecomissionStage</t>
@@ -1531,7 +1531,7 @@
     <t>Decommission Stage</t>
   </si>
   <si>
-    <t>The stage in the lifecycle where the AI system is being decomissioned as part of retirement</t>
+    <t>The stage in the lifecycle where the AI system is being decommissioned as part of retirement</t>
   </si>
   <si>
     <t>ai:RetirementStage</t>
@@ -1573,7 +1573,7 @@
     <t>Scott Kellum, Harshvardhan J. Pandit, Delaram Golpayegani, Georg P. Krog, Julian Flake</t>
   </si>
   <si>
-    <t>ai:DevelopmentOperation as a concept that defines how ai processeses and operates (as data)</t>
+    <t>ai:DevelopmentOperation as a concept that defines how ai processes and operates (as data)</t>
   </si>
   <si>
     <t>DataCollection</t>
@@ -8650,7 +8650,7 @@
       <c r="A7" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="27" t="s">
         <v>96</v>
       </c>
       <c r="C7" s="27" t="s">
@@ -8754,7 +8754,7 @@
       <c r="A9" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C9" s="27" t="s">
@@ -8984,7 +8984,7 @@
       <c r="B18" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="27" t="s">
         <v>121</v>
       </c>
       <c r="D18" s="27" t="s">
@@ -9085,7 +9085,7 @@
       <c r="A21" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="27" t="s">
         <v>127</v>
       </c>
       <c r="C21" s="27" t="s">
@@ -10018,7 +10018,7 @@
       <c r="B7" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="27" t="s">
         <v>170</v>
       </c>
       <c r="D7" s="26"/>
@@ -10117,10 +10117,10 @@
       <c r="A9" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="27" t="s">
         <v>180</v>
       </c>
       <c r="D9" s="26" t="s">
@@ -10172,7 +10172,7 @@
       <c r="B10" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="27" t="s">
         <v>184</v>
       </c>
       <c r="D10" s="26" t="s">
@@ -10525,7 +10525,7 @@
       <c r="A17" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="27" t="s">
         <v>210</v>
       </c>
       <c r="C17" s="26" t="s">
@@ -10580,7 +10580,7 @@
       <c r="B18" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="27" t="s">
         <v>216</v>
       </c>
       <c r="D18" s="26" t="s">
@@ -10879,7 +10879,7 @@
       <c r="A24" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="27" t="s">
         <v>237</v>
       </c>
       <c r="C24" s="26" t="s">
@@ -10929,7 +10929,7 @@
       <c r="A25" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="27" t="s">
         <v>240</v>
       </c>
       <c r="C25" s="27" t="s">
@@ -11034,7 +11034,7 @@
       <c r="B27" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="27" t="s">
         <v>248</v>
       </c>
       <c r="D27" s="26" t="s">
@@ -11282,7 +11282,7 @@
       <c r="B32" s="26" t="s">
         <v>264</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="27" t="s">
         <v>265</v>
       </c>
       <c r="D32" s="27" t="s">
@@ -14040,7 +14040,7 @@
       <c r="B55" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="C55" s="26" t="s">
+      <c r="C55" s="27" t="s">
         <v>441</v>
       </c>
       <c r="D55" s="26"/>

</xml_diff>

<commit_message>
fix duplicate concept metadata in AI
`ai:DecisionTree` and `ai:GeneticAlgorithm` had duplicate entries which
caused multiple creation dates, leading to fluctuations in HTML output.
Fixed by removing the duplicacy in source spreadsheets.
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ai.xlsx
+++ b/code/vocab_csv/ai.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="769">
   <si>
     <t>Term</t>
   </si>
@@ -11448,38 +11448,20 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B39" s="40" t="s">
-        <v>195</v>
-      </c>
-      <c r="C39" s="39" t="s">
-        <v>196</v>
-      </c>
-      <c r="D39" s="40" t="s">
-        <v>236</v>
-      </c>
-      <c r="E39" s="40" t="s">
-        <v>46</v>
-      </c>
+      <c r="A39" s="39"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
       <c r="F39" s="40"/>
       <c r="G39" s="40"/>
       <c r="H39" s="40"/>
       <c r="I39" s="40"/>
-      <c r="J39" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="K39" s="41">
-        <v>45627.0</v>
-      </c>
+      <c r="J39" s="39"/>
+      <c r="K39" s="41"/>
       <c r="L39" s="42"/>
-      <c r="M39" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="N39" s="40" t="s">
-        <v>22</v>
-      </c>
+      <c r="M39" s="42"/>
+      <c r="N39" s="40"/>
       <c r="O39" s="43"/>
       <c r="P39" s="43"/>
       <c r="Q39" s="43"/>
@@ -11500,36 +11482,20 @@
       <c r="AF39" s="43"/>
     </row>
     <row r="40">
-      <c r="A40" s="44" t="s">
-        <v>198</v>
-      </c>
-      <c r="B40" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="C40" s="40" t="s">
-        <v>200</v>
-      </c>
+      <c r="A40" s="44"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
       <c r="D40" s="43"/>
-      <c r="E40" s="40" t="s">
-        <v>46</v>
-      </c>
+      <c r="E40" s="40"/>
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
       <c r="H40" s="43"/>
       <c r="I40" s="43"/>
-      <c r="J40" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="K40" s="41">
-        <v>45627.0</v>
-      </c>
+      <c r="J40" s="39"/>
+      <c r="K40" s="41"/>
       <c r="L40" s="42"/>
-      <c r="M40" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="N40" s="40" t="s">
-        <v>22</v>
-      </c>
+      <c r="M40" s="42"/>
+      <c r="N40" s="40"/>
       <c r="O40" s="43"/>
       <c r="P40" s="43"/>
       <c r="Q40" s="43"/>

</xml_diff>

<commit_message>
fix `ai:DataOperation` taxonomy in AI #294
The parents were incorrectly structured, which resulted in the hierarchy
not being displayed correctly in HTML. Fixed this by declaring all AI
data operations as `dpv:Processing` instances, with the hierarchy
specified between AI extension concepts.
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ai.xlsx
+++ b/code/vocab_csv/ai.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="1113">
   <si>
     <t>Term</t>
   </si>
@@ -2166,10 +2166,7 @@
     <t>Processing operation where data is collected, e.g. in a raw or unrefined form</t>
   </si>
   <si>
-    <t>dpv:Collect</t>
-  </si>
-  <si>
-    <t>ai:DataOperation</t>
+    <t>dpv:Collect,ai:DataOperation</t>
   </si>
   <si>
     <t xml:space="preserve">DataPreparation </t>
@@ -2181,7 +2178,7 @@
     <t>Processing operation where data is prepared, e.g. organising and transforming it to make it ready for use</t>
   </si>
   <si>
-    <t>dpv:Organise,dpv:Transform</t>
+    <t>dpv:Organise,dpv:Transform,ai:DataOperation</t>
   </si>
   <si>
     <t>DataAnnotation</t>
@@ -2193,7 +2190,7 @@
     <t>Processing operation where data is annoated, e.g. by adding additional metadata or context to make it useful</t>
   </si>
   <si>
-    <t>dpv:Obtain,ai:Preparation</t>
+    <t>dpv:Obtain,ai:DataPreparation</t>
   </si>
   <si>
     <t>DataLabelling</t>
@@ -2205,7 +2202,7 @@
     <t>Processing operation where data annotation is carried out through labelling, e.g. by assigning tags or categories</t>
   </si>
   <si>
-    <t>dpv:Obtain,ai:Annotation</t>
+    <t>dpv:Obtain,ai:DataAnnotation</t>
   </si>
   <si>
     <t>DataCleaning</t>
@@ -4773,7 +4770,7 @@
       <c r="C5" s="27" t="s">
         <v>688</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="26" t="s">
         <v>206</v>
       </c>
@@ -4824,8 +4821,8 @@
       <c r="D6" s="27" t="s">
         <v>692</v>
       </c>
-      <c r="E6" s="27" t="s">
-        <v>693</v>
+      <c r="E6" s="26" t="s">
+        <v>206</v>
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
@@ -4863,19 +4860,19 @@
     </row>
     <row r="7">
       <c r="A7" s="27" t="s">
+        <v>693</v>
+      </c>
+      <c r="B7" s="26" t="s">
         <v>694</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="C7" s="27" t="s">
         <v>695</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="D7" s="6" t="s">
         <v>696</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>697</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>693</v>
+      <c r="E7" s="26" t="s">
+        <v>206</v>
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
@@ -4913,19 +4910,19 @@
     </row>
     <row r="8">
       <c r="A8" s="27" t="s">
+        <v>697</v>
+      </c>
+      <c r="B8" s="34" t="s">
         <v>698</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="C8" s="27" t="s">
         <v>699</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="D8" s="27" t="s">
         <v>700</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>701</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>693</v>
+      <c r="E8" s="26" t="s">
+        <v>206</v>
       </c>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
@@ -4963,19 +4960,19 @@
     </row>
     <row r="9">
       <c r="A9" s="27" t="s">
+        <v>701</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>702</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="C9" s="27" t="s">
         <v>703</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="D9" s="27" t="s">
         <v>704</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>705</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>693</v>
+      <c r="E9" s="26" t="s">
+        <v>206</v>
       </c>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
@@ -5013,19 +5010,19 @@
     </row>
     <row r="10">
       <c r="A10" s="27" t="s">
+        <v>705</v>
+      </c>
+      <c r="B10" s="26" t="s">
         <v>706</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="C10" s="27" t="s">
         <v>707</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="D10" s="27" t="s">
         <v>708</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>709</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>693</v>
+      <c r="E10" s="26" t="s">
+        <v>206</v>
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
@@ -5063,19 +5060,19 @@
     </row>
     <row r="11">
       <c r="A11" s="27" t="s">
+        <v>709</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>710</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="C11" s="27" t="s">
         <v>711</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="D11" s="27" t="s">
         <v>712</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>713</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>693</v>
+      <c r="E11" s="26" t="s">
+        <v>206</v>
       </c>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
@@ -5113,19 +5110,19 @@
     </row>
     <row r="12">
       <c r="A12" s="27" t="s">
+        <v>713</v>
+      </c>
+      <c r="B12" s="26" t="s">
         <v>714</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>715</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>716</v>
-      </c>
       <c r="D12" s="27" t="s">
-        <v>713</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>693</v>
+        <v>712</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>206</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
@@ -5163,19 +5160,19 @@
     </row>
     <row r="13">
       <c r="A13" s="27" t="s">
+        <v>716</v>
+      </c>
+      <c r="B13" s="26" t="s">
         <v>717</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="C13" s="27" t="s">
         <v>718</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>719</v>
-      </c>
       <c r="D13" s="27" t="s">
-        <v>681</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>693</v>
+        <v>708</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>206</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -5280,10 +5277,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>720</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>721</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -5315,23 +5312,23 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>722</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="27" t="s">
         <v>723</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>724</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="44"/>
       <c r="G2" s="5" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H2" s="44"/>
       <c r="I2" s="8"/>
@@ -5370,23 +5367,23 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>726</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>727</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>729</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -5459,23 +5456,23 @@
     </row>
     <row r="6">
       <c r="A6" s="36" t="s">
+        <v>729</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>730</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="C6" s="6" t="s">
         <v>731</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>732</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>733</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -5513,23 +5510,23 @@
     </row>
     <row r="7">
       <c r="A7" s="27" t="s">
+        <v>733</v>
+      </c>
+      <c r="B7" s="27" t="s">
         <v>734</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="C7" s="6" t="s">
         <v>735</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>736</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>737</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -5567,23 +5564,23 @@
     </row>
     <row r="8">
       <c r="A8" s="27" t="s">
+        <v>737</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>738</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="C8" s="6" t="s">
         <v>739</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>740</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -5621,23 +5618,23 @@
     </row>
     <row r="9">
       <c r="A9" s="27" t="s">
+        <v>740</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>741</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="C9" s="6" t="s">
         <v>742</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>743</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -5675,23 +5672,23 @@
     </row>
     <row r="10">
       <c r="A10" s="27" t="s">
+        <v>743</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>744</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="C10" s="6" t="s">
         <v>745</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>746</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -5729,22 +5726,22 @@
     </row>
     <row r="11">
       <c r="A11" s="27" t="s">
+        <v>746</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>747</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="C11" s="6" t="s">
         <v>748</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>749</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>724</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>725</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -5784,23 +5781,23 @@
     </row>
     <row r="12">
       <c r="A12" s="27" t="s">
+        <v>749</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>750</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="C12" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>752</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -5838,23 +5835,23 @@
     </row>
     <row r="13">
       <c r="A13" s="27" t="s">
+        <v>752</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>753</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="C13" s="6" t="s">
         <v>754</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>755</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="26"/>
@@ -5892,23 +5889,23 @@
     </row>
     <row r="14">
       <c r="A14" s="27" t="s">
+        <v>755</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>756</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="C14" s="6" t="s">
         <v>757</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>758</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
@@ -5946,23 +5943,23 @@
     </row>
     <row r="15">
       <c r="A15" s="27" t="s">
+        <v>758</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>759</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="C15" s="6" t="s">
         <v>760</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>761</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
@@ -6000,23 +5997,23 @@
     </row>
     <row r="16">
       <c r="A16" s="27" t="s">
+        <v>761</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>762</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="C16" s="6" t="s">
         <v>763</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>764</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -6054,22 +6051,22 @@
     </row>
     <row r="17">
       <c r="A17" s="27" t="s">
+        <v>764</v>
+      </c>
+      <c r="B17" s="27" t="s">
         <v>765</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="C17" s="6" t="s">
         <v>766</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>767</v>
-      </c>
       <c r="D17" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E17" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>724</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>725</v>
       </c>
       <c r="M17" s="9">
         <v>45627.0</v>
@@ -6086,23 +6083,23 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
+        <v>767</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>768</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>769</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>770</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -6140,23 +6137,23 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
+        <v>770</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>771</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>772</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>773</v>
-      </c>
       <c r="D19" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -6194,23 +6191,23 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
+        <v>773</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>774</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>775</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>776</v>
-      </c>
       <c r="D20" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -6251,23 +6248,23 @@
     </row>
     <row r="22">
       <c r="A22" s="36" t="s">
+        <v>776</v>
+      </c>
+      <c r="B22" s="36" t="s">
         <v>777</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="C22" s="6" t="s">
         <v>778</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>779</v>
-      </c>
       <c r="D22" s="6" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -6305,23 +6302,23 @@
     </row>
     <row r="23">
       <c r="A23" s="27" t="s">
+        <v>779</v>
+      </c>
+      <c r="B23" s="27" t="s">
         <v>780</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="C23" s="6" t="s">
         <v>781</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>782</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>783</v>
-      </c>
       <c r="E23" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
@@ -6359,23 +6356,23 @@
     </row>
     <row r="24">
       <c r="A24" s="27" t="s">
+        <v>783</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>784</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="C24" s="6" t="s">
         <v>785</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>786</v>
-      </c>
       <c r="D24" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -6413,23 +6410,23 @@
     </row>
     <row r="25">
       <c r="A25" s="27" t="s">
+        <v>786</v>
+      </c>
+      <c r="B25" s="27" t="s">
         <v>787</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="C25" s="6" t="s">
         <v>788</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>789</v>
-      </c>
       <c r="D25" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -6467,23 +6464,23 @@
     </row>
     <row r="26">
       <c r="A26" s="27" t="s">
+        <v>789</v>
+      </c>
+      <c r="B26" s="27" t="s">
         <v>790</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="C26" s="6" t="s">
         <v>791</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>792</v>
-      </c>
       <c r="D26" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -6521,22 +6518,22 @@
     </row>
     <row r="27">
       <c r="A27" s="27" t="s">
+        <v>792</v>
+      </c>
+      <c r="B27" s="27" t="s">
         <v>793</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="C27" s="6" t="s">
         <v>794</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>795</v>
-      </c>
       <c r="D27" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E27" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>724</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>725</v>
       </c>
       <c r="M27" s="9">
         <v>45627.0</v>
@@ -6553,23 +6550,23 @@
     </row>
     <row r="28">
       <c r="A28" s="27" t="s">
+        <v>795</v>
+      </c>
+      <c r="B28" s="27" t="s">
         <v>796</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="C28" s="6" t="s">
         <v>797</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>798</v>
-      </c>
       <c r="D28" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
@@ -6607,23 +6604,23 @@
     </row>
     <row r="29">
       <c r="A29" s="27" t="s">
+        <v>798</v>
+      </c>
+      <c r="B29" s="27" t="s">
         <v>799</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="C29" s="6" t="s">
         <v>800</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>801</v>
-      </c>
       <c r="D29" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -6661,23 +6658,23 @@
     </row>
     <row r="30">
       <c r="A30" s="27" t="s">
+        <v>801</v>
+      </c>
+      <c r="B30" s="27" t="s">
         <v>802</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="C30" s="6" t="s">
         <v>803</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>804</v>
-      </c>
       <c r="D30" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -6715,23 +6712,23 @@
     </row>
     <row r="31">
       <c r="A31" s="27" t="s">
+        <v>804</v>
+      </c>
+      <c r="B31" s="27" t="s">
         <v>805</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="C31" s="6" t="s">
         <v>806</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>807</v>
-      </c>
       <c r="D31" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
@@ -6769,23 +6766,23 @@
     </row>
     <row r="32">
       <c r="A32" s="27" t="s">
+        <v>807</v>
+      </c>
+      <c r="B32" s="27" t="s">
         <v>808</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="C32" s="6" t="s">
         <v>809</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>810</v>
-      </c>
       <c r="D32" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
@@ -6823,22 +6820,22 @@
     </row>
     <row r="33">
       <c r="A33" s="27" t="s">
+        <v>810</v>
+      </c>
+      <c r="B33" s="27" t="s">
         <v>811</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="C33" s="6" t="s">
         <v>812</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>813</v>
-      </c>
       <c r="D33" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E33" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>724</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>725</v>
       </c>
       <c r="M33" s="9">
         <v>45627.0</v>
@@ -6855,23 +6852,23 @@
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>814</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>815</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>816</v>
-      </c>
       <c r="D34" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
@@ -6909,23 +6906,23 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
+        <v>816</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>817</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>818</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>819</v>
-      </c>
       <c r="D35" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -6963,23 +6960,23 @@
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>820</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>821</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>822</v>
-      </c>
       <c r="D36" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
@@ -7021,23 +7018,23 @@
     </row>
     <row r="38">
       <c r="A38" s="36" t="s">
+        <v>822</v>
+      </c>
+      <c r="B38" s="36" t="s">
         <v>823</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="C38" s="6" t="s">
         <v>824</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>825</v>
-      </c>
       <c r="D38" s="6" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
@@ -7075,23 +7072,23 @@
     </row>
     <row r="39">
       <c r="A39" s="27" t="s">
+        <v>825</v>
+      </c>
+      <c r="B39" s="27" t="s">
         <v>826</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="C39" s="6" t="s">
         <v>827</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>828</v>
       </c>
-      <c r="D39" s="6" t="s">
-        <v>829</v>
-      </c>
       <c r="E39" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -7129,23 +7126,23 @@
     </row>
     <row r="40">
       <c r="A40" s="27" t="s">
+        <v>829</v>
+      </c>
+      <c r="B40" s="27" t="s">
         <v>830</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="C40" s="6" t="s">
         <v>831</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>832</v>
-      </c>
       <c r="D40" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -7183,23 +7180,23 @@
     </row>
     <row r="41">
       <c r="A41" s="27" t="s">
+        <v>832</v>
+      </c>
+      <c r="B41" s="27" t="s">
         <v>833</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="C41" s="6" t="s">
         <v>834</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>835</v>
-      </c>
       <c r="D41" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
@@ -7237,23 +7234,23 @@
     </row>
     <row r="42">
       <c r="A42" s="27" t="s">
+        <v>835</v>
+      </c>
+      <c r="B42" s="27" t="s">
         <v>836</v>
       </c>
-      <c r="B42" s="27" t="s">
+      <c r="C42" s="6" t="s">
         <v>837</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>838</v>
-      </c>
       <c r="D42" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
@@ -7291,22 +7288,22 @@
     </row>
     <row r="43">
       <c r="A43" s="27" t="s">
+        <v>838</v>
+      </c>
+      <c r="B43" s="27" t="s">
         <v>839</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="C43" s="6" t="s">
         <v>840</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>841</v>
-      </c>
       <c r="D43" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E43" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>724</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>725</v>
       </c>
       <c r="M43" s="9">
         <v>45627.0</v>
@@ -7323,23 +7320,23 @@
     </row>
     <row r="44">
       <c r="A44" s="27" t="s">
+        <v>841</v>
+      </c>
+      <c r="B44" s="27" t="s">
         <v>842</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="C44" s="6" t="s">
         <v>843</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>844</v>
-      </c>
       <c r="D44" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
@@ -7377,23 +7374,23 @@
     </row>
     <row r="45">
       <c r="A45" s="27" t="s">
+        <v>844</v>
+      </c>
+      <c r="B45" s="27" t="s">
         <v>845</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="C45" s="6" t="s">
         <v>846</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>847</v>
-      </c>
       <c r="D45" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
@@ -7431,23 +7428,23 @@
     </row>
     <row r="46">
       <c r="A46" s="27" t="s">
+        <v>847</v>
+      </c>
+      <c r="B46" s="27" t="s">
         <v>848</v>
       </c>
-      <c r="B46" s="27" t="s">
+      <c r="C46" s="6" t="s">
         <v>849</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>850</v>
-      </c>
       <c r="D46" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
@@ -7485,23 +7482,23 @@
     </row>
     <row r="47">
       <c r="A47" s="27" t="s">
+        <v>850</v>
+      </c>
+      <c r="B47" s="27" t="s">
         <v>851</v>
       </c>
-      <c r="B47" s="27" t="s">
+      <c r="C47" s="6" t="s">
         <v>852</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>853</v>
-      </c>
       <c r="D47" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
@@ -7539,23 +7536,23 @@
     </row>
     <row r="48">
       <c r="A48" s="27" t="s">
+        <v>853</v>
+      </c>
+      <c r="B48" s="27" t="s">
         <v>854</v>
       </c>
-      <c r="B48" s="27" t="s">
+      <c r="C48" s="6" t="s">
         <v>855</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>856</v>
-      </c>
       <c r="D48" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
@@ -7593,22 +7590,22 @@
     </row>
     <row r="49">
       <c r="A49" s="27" t="s">
+        <v>856</v>
+      </c>
+      <c r="B49" s="27" t="s">
         <v>857</v>
       </c>
-      <c r="B49" s="27" t="s">
+      <c r="C49" s="6" t="s">
         <v>858</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>859</v>
-      </c>
       <c r="D49" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E49" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="G49" s="6" t="s">
         <v>724</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>725</v>
       </c>
       <c r="M49" s="9">
         <v>45627.0</v>
@@ -7625,23 +7622,23 @@
     </row>
     <row r="50">
       <c r="A50" s="6" t="s">
+        <v>859</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>860</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="C50" s="6" t="s">
         <v>861</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>862</v>
-      </c>
       <c r="D50" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
@@ -7679,23 +7676,23 @@
     </row>
     <row r="51">
       <c r="A51" s="6" t="s">
+        <v>862</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>863</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>864</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>865</v>
-      </c>
       <c r="D51" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
@@ -7733,23 +7730,23 @@
     </row>
     <row r="52">
       <c r="A52" s="6" t="s">
+        <v>865</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>866</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="C52" s="6" t="s">
         <v>867</v>
       </c>
-      <c r="C52" s="6" t="s">
-        <v>868</v>
-      </c>
       <c r="D52" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
@@ -7790,23 +7787,23 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
+        <v>868</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>869</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>870</v>
       </c>
-      <c r="C54" s="6" t="s">
-        <v>871</v>
-      </c>
       <c r="D54" s="6" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
@@ -7844,26 +7841,26 @@
     </row>
     <row r="55">
       <c r="A55" s="27" t="s">
+        <v>871</v>
+      </c>
+      <c r="B55" s="34" t="s">
         <v>872</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="C55" s="26" t="s">
         <v>873</v>
       </c>
-      <c r="C55" s="26" t="s">
+      <c r="D55" s="27" t="s">
         <v>874</v>
       </c>
-      <c r="D55" s="27" t="s">
-        <v>875</v>
-      </c>
       <c r="E55" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F55" s="26"/>
       <c r="G55" s="27" t="s">
+        <v>875</v>
+      </c>
+      <c r="H55" s="27" t="s">
         <v>876</v>
-      </c>
-      <c r="H55" s="27" t="s">
-        <v>877</v>
       </c>
       <c r="I55" s="26"/>
       <c r="J55" s="26"/>
@@ -7900,26 +7897,26 @@
     </row>
     <row r="56">
       <c r="A56" s="27" t="s">
+        <v>877</v>
+      </c>
+      <c r="B56" s="26" t="s">
         <v>878</v>
       </c>
-      <c r="B56" s="26" t="s">
+      <c r="C56" s="26" t="s">
         <v>879</v>
       </c>
-      <c r="C56" s="26" t="s">
-        <v>880</v>
-      </c>
       <c r="D56" s="27" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F56" s="26"/>
       <c r="G56" s="27" t="s">
+        <v>875</v>
+      </c>
+      <c r="H56" s="27" t="s">
         <v>876</v>
-      </c>
-      <c r="H56" s="27" t="s">
-        <v>877</v>
       </c>
       <c r="I56" s="26"/>
       <c r="J56" s="26"/>
@@ -7956,31 +7953,31 @@
     </row>
     <row r="57">
       <c r="A57" s="27" t="s">
+        <v>880</v>
+      </c>
+      <c r="B57" s="26" t="s">
         <v>881</v>
       </c>
-      <c r="B57" s="26" t="s">
+      <c r="C57" s="26" t="s">
         <v>882</v>
       </c>
-      <c r="C57" s="26" t="s">
-        <v>883</v>
-      </c>
       <c r="D57" s="27" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F57" s="26"/>
       <c r="G57" s="27" t="s">
+        <v>875</v>
+      </c>
+      <c r="H57" s="27" t="s">
         <v>876</v>
-      </c>
-      <c r="H57" s="27" t="s">
-        <v>877</v>
       </c>
       <c r="I57" s="26"/>
       <c r="J57" s="26"/>
       <c r="K57" s="6" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="L57" s="26"/>
       <c r="M57" s="9">
@@ -8014,31 +8011,31 @@
     </row>
     <row r="58">
       <c r="A58" s="27" t="s">
+        <v>884</v>
+      </c>
+      <c r="B58" s="26" t="s">
         <v>885</v>
       </c>
-      <c r="B58" s="26" t="s">
+      <c r="C58" s="26" t="s">
         <v>886</v>
       </c>
-      <c r="C58" s="26" t="s">
-        <v>887</v>
-      </c>
       <c r="D58" s="27" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F58" s="26"/>
       <c r="G58" s="27" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H58" s="27" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="I58" s="26"/>
       <c r="J58" s="26"/>
       <c r="K58" s="38" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L58" s="26"/>
       <c r="M58" s="9">
@@ -8075,23 +8072,23 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
+        <v>889</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>890</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>891</v>
       </c>
-      <c r="C60" s="6" t="s">
-        <v>892</v>
-      </c>
       <c r="D60" s="6" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
@@ -8132,23 +8129,23 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>893</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>894</v>
       </c>
-      <c r="C62" s="6" t="s">
-        <v>895</v>
-      </c>
       <c r="D62" s="6" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
@@ -8189,23 +8186,23 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>896</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>897</v>
       </c>
-      <c r="C64" s="6" t="s">
-        <v>898</v>
-      </c>
       <c r="D64" s="6" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
@@ -8243,23 +8240,23 @@
     </row>
     <row r="66">
       <c r="A66" s="15" t="s">
+        <v>898</v>
+      </c>
+      <c r="B66" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="C66" s="45" t="s">
         <v>900</v>
       </c>
-      <c r="C66" s="45" t="s">
+      <c r="D66" s="10" t="s">
         <v>901</v>
       </c>
-      <c r="D66" s="10" t="s">
-        <v>902</v>
-      </c>
       <c r="E66" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F66" s="11"/>
       <c r="G66" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H66" s="11"/>
       <c r="K66" s="11"/>
@@ -8272,7 +8269,7 @@
         <v>21</v>
       </c>
       <c r="P66" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q66" s="11"/>
       <c r="R66" s="11"/>
@@ -8295,28 +8292,28 @@
     </row>
     <row r="67">
       <c r="A67" s="45" t="s">
+        <v>903</v>
+      </c>
+      <c r="B67" s="45" t="s">
         <v>904</v>
       </c>
-      <c r="B67" s="45" t="s">
+      <c r="C67" s="46" t="s">
         <v>905</v>
       </c>
-      <c r="C67" s="46" t="s">
+      <c r="D67" s="46" t="s">
         <v>906</v>
       </c>
-      <c r="D67" s="46" t="s">
-        <v>907</v>
-      </c>
       <c r="E67" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F67" s="11"/>
       <c r="G67" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H67" s="11"/>
       <c r="K67" s="11"/>
       <c r="L67" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M67" s="47">
         <v>45548.0</v>
@@ -8328,7 +8325,7 @@
         <v>32</v>
       </c>
       <c r="P67" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q67" s="11"/>
       <c r="R67" s="11"/>
@@ -8349,28 +8346,28 @@
     </row>
     <row r="68">
       <c r="A68" s="45" t="s">
+        <v>908</v>
+      </c>
+      <c r="B68" s="45" t="s">
         <v>909</v>
       </c>
-      <c r="B68" s="45" t="s">
+      <c r="C68" s="45" t="s">
         <v>910</v>
       </c>
-      <c r="C68" s="45" t="s">
+      <c r="D68" s="46" t="s">
         <v>911</v>
       </c>
-      <c r="D68" s="46" t="s">
-        <v>912</v>
-      </c>
       <c r="E68" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F68" s="11"/>
       <c r="G68" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H68" s="11"/>
       <c r="K68" s="11"/>
       <c r="L68" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M68" s="47">
         <v>45548.0</v>
@@ -8380,7 +8377,7 @@
         <v>21</v>
       </c>
       <c r="P68" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q68" s="11"/>
       <c r="R68" s="11"/>
@@ -8403,28 +8400,28 @@
     </row>
     <row r="69">
       <c r="A69" s="46" t="s">
+        <v>912</v>
+      </c>
+      <c r="B69" s="46" t="s">
         <v>913</v>
       </c>
-      <c r="B69" s="46" t="s">
+      <c r="C69" s="45" t="s">
         <v>914</v>
       </c>
-      <c r="C69" s="45" t="s">
+      <c r="D69" s="46" t="s">
         <v>915</v>
       </c>
-      <c r="D69" s="46" t="s">
-        <v>916</v>
-      </c>
       <c r="E69" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F69" s="11"/>
       <c r="G69" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H69" s="11"/>
       <c r="K69" s="11"/>
       <c r="L69" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M69" s="47">
         <v>45548.0</v>
@@ -8436,7 +8433,7 @@
         <v>32</v>
       </c>
       <c r="P69" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q69" s="11"/>
       <c r="R69" s="11"/>
@@ -8457,28 +8454,28 @@
     </row>
     <row r="70">
       <c r="A70" s="45" t="s">
+        <v>916</v>
+      </c>
+      <c r="B70" s="45" t="s">
         <v>917</v>
       </c>
-      <c r="B70" s="45" t="s">
+      <c r="C70" s="45" t="s">
         <v>918</v>
       </c>
-      <c r="C70" s="45" t="s">
-        <v>919</v>
-      </c>
       <c r="D70" s="46" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F70" s="11"/>
       <c r="G70" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H70" s="11"/>
       <c r="K70" s="11"/>
       <c r="L70" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M70" s="47">
         <v>45548.0</v>
@@ -8488,7 +8485,7 @@
         <v>21</v>
       </c>
       <c r="P70" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q70" s="11"/>
       <c r="R70" s="11"/>
@@ -8511,30 +8508,30 @@
     </row>
     <row r="71">
       <c r="A71" s="46" t="s">
+        <v>919</v>
+      </c>
+      <c r="B71" s="46" t="s">
         <v>920</v>
       </c>
-      <c r="B71" s="46" t="s">
+      <c r="C71" s="45" t="s">
         <v>921</v>
       </c>
-      <c r="C71" s="45" t="s">
-        <v>922</v>
-      </c>
       <c r="D71" s="46" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F71" s="11"/>
       <c r="G71" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H71" s="11"/>
       <c r="K71" s="45" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="L71" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M71" s="47">
         <v>45548.0</v>
@@ -8546,7 +8543,7 @@
         <v>32</v>
       </c>
       <c r="P71" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q71" s="11"/>
       <c r="R71" s="11"/>
@@ -8567,28 +8564,28 @@
     </row>
     <row r="72">
       <c r="A72" s="45" t="s">
+        <v>923</v>
+      </c>
+      <c r="B72" s="45" t="s">
         <v>924</v>
       </c>
-      <c r="B72" s="45" t="s">
+      <c r="C72" s="45" t="s">
         <v>925</v>
       </c>
-      <c r="C72" s="45" t="s">
-        <v>926</v>
-      </c>
       <c r="D72" s="46" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F72" s="11"/>
       <c r="G72" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H72" s="11"/>
       <c r="K72" s="11"/>
       <c r="L72" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M72" s="47">
         <v>45548.0</v>
@@ -8598,7 +8595,7 @@
         <v>21</v>
       </c>
       <c r="P72" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q72" s="11"/>
       <c r="R72" s="11"/>
@@ -8621,28 +8618,28 @@
     </row>
     <row r="73">
       <c r="A73" s="45" t="s">
+        <v>926</v>
+      </c>
+      <c r="B73" s="45" t="s">
         <v>927</v>
       </c>
-      <c r="B73" s="45" t="s">
+      <c r="C73" s="45" t="s">
         <v>928</v>
       </c>
-      <c r="C73" s="45" t="s">
-        <v>929</v>
-      </c>
       <c r="D73" s="46" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F73" s="11"/>
       <c r="G73" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H73" s="11"/>
       <c r="K73" s="11"/>
       <c r="L73" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M73" s="47">
         <v>45548.0</v>
@@ -8652,7 +8649,7 @@
         <v>21</v>
       </c>
       <c r="P73" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q73" s="11"/>
       <c r="R73" s="11"/>
@@ -8675,30 +8672,30 @@
     </row>
     <row r="74">
       <c r="A74" s="45" t="s">
+        <v>929</v>
+      </c>
+      <c r="B74" s="45" t="s">
         <v>930</v>
       </c>
-      <c r="B74" s="45" t="s">
+      <c r="C74" s="45" t="s">
         <v>931</v>
       </c>
-      <c r="C74" s="45" t="s">
-        <v>932</v>
-      </c>
       <c r="D74" s="46" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F74" s="11"/>
       <c r="G74" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H74" s="11"/>
       <c r="K74" s="45" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="L74" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M74" s="47">
         <v>45548.0</v>
@@ -8708,7 +8705,7 @@
         <v>21</v>
       </c>
       <c r="P74" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q74" s="11"/>
       <c r="R74" s="11"/>
@@ -8731,28 +8728,28 @@
     </row>
     <row r="75">
       <c r="A75" s="45" t="s">
+        <v>933</v>
+      </c>
+      <c r="B75" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="B75" s="45" t="s">
+      <c r="C75" s="45" t="s">
         <v>935</v>
       </c>
-      <c r="C75" s="45" t="s">
+      <c r="D75" s="46" t="s">
         <v>936</v>
       </c>
-      <c r="D75" s="46" t="s">
-        <v>937</v>
-      </c>
       <c r="E75" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F75" s="11"/>
       <c r="G75" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H75" s="11"/>
       <c r="K75" s="11"/>
       <c r="L75" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M75" s="47">
         <v>45548.0</v>
@@ -8762,7 +8759,7 @@
         <v>21</v>
       </c>
       <c r="P75" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q75" s="11"/>
       <c r="R75" s="11"/>
@@ -8785,28 +8782,28 @@
     </row>
     <row r="76">
       <c r="A76" s="45" t="s">
+        <v>937</v>
+      </c>
+      <c r="B76" s="45" t="s">
         <v>938</v>
       </c>
-      <c r="B76" s="45" t="s">
+      <c r="C76" s="45" t="s">
         <v>939</v>
       </c>
-      <c r="C76" s="45" t="s">
-        <v>940</v>
-      </c>
       <c r="D76" s="46" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F76" s="11"/>
       <c r="G76" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H76" s="11"/>
       <c r="K76" s="11"/>
       <c r="L76" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M76" s="47">
         <v>45548.0</v>
@@ -8816,7 +8813,7 @@
         <v>21</v>
       </c>
       <c r="P76" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q76" s="11"/>
       <c r="R76" s="11"/>
@@ -8839,28 +8836,28 @@
     </row>
     <row r="77">
       <c r="A77" s="45" t="s">
+        <v>940</v>
+      </c>
+      <c r="B77" s="45" t="s">
         <v>941</v>
       </c>
-      <c r="B77" s="45" t="s">
+      <c r="C77" s="45" t="s">
         <v>942</v>
       </c>
-      <c r="C77" s="45" t="s">
-        <v>943</v>
-      </c>
       <c r="D77" s="46" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F77" s="11"/>
       <c r="G77" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H77" s="11"/>
       <c r="K77" s="11"/>
       <c r="L77" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M77" s="47">
         <v>45548.0</v>
@@ -8870,7 +8867,7 @@
         <v>21</v>
       </c>
       <c r="P77" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q77" s="11"/>
       <c r="R77" s="11"/>
@@ -8893,30 +8890,30 @@
     </row>
     <row r="78">
       <c r="A78" s="45" t="s">
+        <v>943</v>
+      </c>
+      <c r="B78" s="45" t="s">
         <v>944</v>
       </c>
-      <c r="B78" s="45" t="s">
+      <c r="C78" s="45" t="s">
         <v>945</v>
       </c>
-      <c r="C78" s="45" t="s">
-        <v>946</v>
-      </c>
       <c r="D78" s="46" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F78" s="11"/>
       <c r="G78" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H78" s="11"/>
       <c r="K78" s="45" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="L78" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M78" s="47">
         <v>45548.0</v>
@@ -8926,7 +8923,7 @@
         <v>21</v>
       </c>
       <c r="P78" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q78" s="11"/>
       <c r="R78" s="11"/>
@@ -8949,28 +8946,28 @@
     </row>
     <row r="79">
       <c r="A79" s="45" t="s">
+        <v>947</v>
+      </c>
+      <c r="B79" s="45" t="s">
         <v>948</v>
       </c>
-      <c r="B79" s="45" t="s">
+      <c r="C79" s="45" t="s">
         <v>949</v>
       </c>
-      <c r="C79" s="45" t="s">
-        <v>950</v>
-      </c>
       <c r="D79" s="46" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F79" s="11"/>
       <c r="G79" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H79" s="11"/>
       <c r="K79" s="11"/>
       <c r="L79" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M79" s="47">
         <v>45548.0</v>
@@ -8980,7 +8977,7 @@
         <v>21</v>
       </c>
       <c r="P79" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q79" s="11"/>
       <c r="R79" s="11"/>
@@ -9003,28 +9000,28 @@
     </row>
     <row r="80">
       <c r="A80" s="45" t="s">
+        <v>950</v>
+      </c>
+      <c r="B80" s="45" t="s">
         <v>951</v>
       </c>
-      <c r="B80" s="45" t="s">
+      <c r="C80" s="45" t="s">
         <v>952</v>
       </c>
-      <c r="C80" s="45" t="s">
-        <v>953</v>
-      </c>
       <c r="D80" s="46" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F80" s="11"/>
       <c r="G80" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H80" s="11"/>
       <c r="K80" s="11"/>
       <c r="L80" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M80" s="47">
         <v>45548.0</v>
@@ -9034,7 +9031,7 @@
         <v>21</v>
       </c>
       <c r="P80" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q80" s="11"/>
       <c r="R80" s="11"/>
@@ -9057,28 +9054,28 @@
     </row>
     <row r="81">
       <c r="A81" s="45" t="s">
+        <v>953</v>
+      </c>
+      <c r="B81" s="45" t="s">
         <v>954</v>
       </c>
-      <c r="B81" s="45" t="s">
+      <c r="C81" s="45" t="s">
         <v>955</v>
       </c>
-      <c r="C81" s="45" t="s">
+      <c r="D81" s="46" t="s">
         <v>956</v>
       </c>
-      <c r="D81" s="46" t="s">
-        <v>957</v>
-      </c>
       <c r="E81" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F81" s="11"/>
       <c r="G81" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H81" s="11"/>
       <c r="K81" s="11"/>
       <c r="L81" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M81" s="47">
         <v>45548.0</v>
@@ -9088,7 +9085,7 @@
         <v>21</v>
       </c>
       <c r="P81" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q81" s="11"/>
       <c r="R81" s="11"/>
@@ -9198,25 +9195,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="40" t="s">
+        <v>957</v>
+      </c>
+      <c r="B1" s="40" t="s">
         <v>958</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="C1" s="6" t="s">
         <v>959</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="40" t="s">
         <v>960</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="E1" s="6" t="s">
         <v>961</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>962</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>963</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>964</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>91</v>
@@ -9224,13 +9221,13 @@
     </row>
     <row r="2">
       <c r="A2" s="48" t="s">
+        <v>964</v>
+      </c>
+      <c r="B2" s="49" t="s">
         <v>965</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="C2" s="40" t="s">
         <v>966</v>
-      </c>
-      <c r="C2" s="40" t="s">
-        <v>967</v>
       </c>
       <c r="D2" s="50"/>
       <c r="E2" s="6" t="s">
@@ -9239,16 +9236,16 @@
     </row>
     <row r="3">
       <c r="A3" s="51" t="s">
+        <v>967</v>
+      </c>
+      <c r="B3" s="40" t="s">
         <v>968</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="C3" s="40" t="s">
         <v>969</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>970</v>
-      </c>
       <c r="D3" s="40" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>85</v>
@@ -9257,24 +9254,24 @@
         <v>215</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>970</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>971</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>972</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="51" t="s">
+        <v>972</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>973</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="C4" s="40" t="s">
         <v>974</v>
       </c>
-      <c r="C4" s="40" t="s">
-        <v>975</v>
-      </c>
       <c r="D4" s="40" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>85</v>
@@ -9283,21 +9280,21 @@
         <v>310</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="51" t="s">
+        <v>976</v>
+      </c>
+      <c r="B5" s="40" t="s">
         <v>977</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="C5" s="40" t="s">
         <v>978</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>979</v>
-      </c>
       <c r="D5" s="40" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>85</v>
@@ -9306,24 +9303,24 @@
         <v>85</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="51" t="s">
+        <v>980</v>
+      </c>
+      <c r="B6" s="40" t="s">
         <v>981</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="C6" s="40" t="s">
         <v>982</v>
       </c>
-      <c r="C6" s="40" t="s">
-        <v>983</v>
-      </c>
       <c r="D6" s="40" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>85</v>
@@ -9332,47 +9329,47 @@
         <v>85</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="51" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>312</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>85</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="51" t="s">
+        <v>987</v>
+      </c>
+      <c r="B8" s="40" t="s">
         <v>988</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="C8" s="40" t="s">
         <v>989</v>
       </c>
-      <c r="C8" s="40" t="s">
-        <v>990</v>
-      </c>
       <c r="D8" s="40" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>81</v>
@@ -9381,7 +9378,7 @@
         <v>472</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>512</v>
@@ -9389,16 +9386,16 @@
     </row>
     <row r="9">
       <c r="A9" s="51" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>510</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>81</v>
@@ -9407,47 +9404,47 @@
         <v>81</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="51" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B10" s="40" t="s">
         <v>470</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>81</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="51" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B11" s="40" t="s">
         <v>514</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>81</v>
@@ -9456,24 +9453,24 @@
         <v>81</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="51" t="s">
+        <v>999</v>
+      </c>
+      <c r="B12" s="40" t="s">
         <v>1000</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="C12" s="40" t="s">
         <v>1001</v>
       </c>
-      <c r="C12" s="40" t="s">
-        <v>1002</v>
-      </c>
       <c r="D12" s="40" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>81</v>
@@ -9482,24 +9479,24 @@
         <v>81</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="51" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B13" s="40" t="s">
         <v>431</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>81</v>
@@ -9508,21 +9505,21 @@
         <v>422</v>
       </c>
       <c r="G13" s="6" t="s">
+        <v>1005</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>1006</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>1007</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="51" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B14" s="40" t="s">
         <v>434</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D14" s="40" t="s">
         <v>431</v>
@@ -9534,21 +9531,21 @@
         <v>81</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="51" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B15" s="40" t="s">
         <v>404</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D15" s="40" t="s">
         <v>431</v>
@@ -9560,12 +9557,12 @@
         <v>422</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="51" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B16" s="40" t="s">
         <v>424</v>
@@ -9580,21 +9577,21 @@
         <v>81</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="51" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B17" s="40" t="s">
         <v>1015</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="C17" s="40" t="s">
         <v>1016</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>1017</v>
       </c>
       <c r="D17" s="40" t="s">
         <v>404</v>
@@ -9603,21 +9600,21 @@
         <v>81</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="51" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B18" s="40" t="s">
         <v>427</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D18" s="40" t="s">
         <v>404</v>
@@ -9626,21 +9623,21 @@
         <v>81</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="51" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B19" s="40" t="s">
         <v>438</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>404</v>
@@ -9652,21 +9649,21 @@
         <v>81</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="51" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B20" s="40" t="s">
         <v>441</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D20" s="40" t="s">
         <v>404</v>
@@ -9675,21 +9672,21 @@
         <v>81</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="51" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B21" s="40" t="s">
         <v>444</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D21" s="40" t="s">
         <v>404</v>
@@ -9701,21 +9698,21 @@
         <v>81</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="51" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B22" s="40" t="s">
         <v>447</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D22" s="40" t="s">
         <v>404</v>
@@ -9724,27 +9721,27 @@
         <v>81</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="51" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B23" s="40" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>81</v>
@@ -9753,21 +9750,21 @@
         <v>81</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="51" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B24" s="40" t="s">
         <v>163</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D24" s="40" t="s">
         <v>47</v>
@@ -9779,15 +9776,15 @@
         <v>72</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="51" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B25" s="40" t="s">
         <v>401</v>
@@ -9805,21 +9802,21 @@
         <v>358</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="48" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B27" s="49" t="s">
         <v>209</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>85</v>
@@ -9827,13 +9824,13 @@
     </row>
     <row r="28">
       <c r="A28" s="51" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B28" s="40" t="s">
         <v>219</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D28" s="40" t="s">
         <v>209</v>
@@ -9845,18 +9842,18 @@
         <v>224</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="51" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B29" s="40" t="s">
         <v>1045</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="C29" s="40" t="s">
         <v>1046</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>1047</v>
       </c>
       <c r="D29" s="40" t="s">
         <v>219</v>
@@ -9868,18 +9865,18 @@
         <v>262</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="51" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B30" s="40" t="s">
         <v>1049</v>
-      </c>
-      <c r="B30" s="40" t="s">
-        <v>1050</v>
       </c>
       <c r="C30" s="40" t="s">
         <v>223</v>
@@ -9894,21 +9891,21 @@
         <v>224</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="51" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B31" s="40" t="s">
         <v>234</v>
       </c>
       <c r="C31" s="40" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D31" s="40" t="s">
         <v>209</v>
@@ -9917,18 +9914,18 @@
         <v>85</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="51" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B32" s="40" t="s">
         <v>1055</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="C32" s="40" t="s">
         <v>1056</v>
-      </c>
-      <c r="C32" s="40" t="s">
-        <v>1057</v>
       </c>
       <c r="D32" s="40" t="s">
         <v>234</v>
@@ -9937,18 +9934,18 @@
         <v>85</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="51" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B33" s="40" t="s">
         <v>1059</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="C33" s="40" t="s">
         <v>1060</v>
-      </c>
-      <c r="C33" s="40" t="s">
-        <v>1061</v>
       </c>
       <c r="D33" s="40" t="s">
         <v>234</v>
@@ -9957,18 +9954,18 @@
         <v>85</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="51" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B34" s="40" t="s">
         <v>237</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D34" s="40" t="s">
         <v>209</v>
@@ -9977,18 +9974,18 @@
         <v>85</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="51" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B35" s="40" t="s">
         <v>1066</v>
       </c>
-      <c r="B35" s="40" t="s">
+      <c r="C35" s="40" t="s">
         <v>1067</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>1068</v>
       </c>
       <c r="D35" s="40" t="s">
         <v>209</v>
@@ -9997,21 +9994,21 @@
         <v>85</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="51" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B36" s="40" t="s">
         <v>1070</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="C36" s="40" t="s">
         <v>1071</v>
-      </c>
-      <c r="C36" s="40" t="s">
-        <v>1072</v>
       </c>
       <c r="D36" s="40" t="s">
         <v>209</v>
@@ -10023,21 +10020,21 @@
         <v>215</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="51" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B37" s="40" t="s">
         <v>226</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D37" s="40" t="s">
         <v>209</v>
@@ -10046,18 +10043,18 @@
         <v>85</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="48" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B39" s="49" t="s">
         <v>1077</v>
       </c>
-      <c r="B39" s="49" t="s">
+      <c r="C39" s="40" t="s">
         <v>1078</v>
-      </c>
-      <c r="C39" s="40" t="s">
-        <v>1079</v>
       </c>
       <c r="D39" s="50"/>
       <c r="E39" s="6" t="s">
@@ -10066,16 +10063,16 @@
     </row>
     <row r="40">
       <c r="A40" s="51" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B40" s="40" t="s">
         <v>1080</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="C40" s="40" t="s">
         <v>1081</v>
       </c>
-      <c r="C40" s="40" t="s">
-        <v>1082</v>
-      </c>
       <c r="D40" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>67</v>
@@ -10084,24 +10081,24 @@
         <v>67</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="51" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B41" s="40" t="s">
         <v>133</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="D41" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>67</v>
@@ -10110,50 +10107,50 @@
         <v>67</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H41" s="6" t="s">
+        <v>1085</v>
+      </c>
+      <c r="I41" s="6" t="s">
         <v>1086</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>1087</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="51" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B42" s="40" t="s">
         <v>100</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>67</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="51" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B43" s="40" t="s">
         <v>137</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>67</v>
@@ -10162,24 +10159,24 @@
         <v>67</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="51" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B44" s="40" t="s">
         <v>139</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>67</v>
@@ -10188,24 +10185,24 @@
         <v>117</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="51" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B45" s="40" t="s">
         <v>142</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>67</v>
@@ -10214,24 +10211,24 @@
         <v>67</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="51" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B46" s="40" t="s">
         <v>145</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D46" s="40" t="s">
         <v>139</v>
@@ -10243,34 +10240,34 @@
         <v>67</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B48" s="52" t="s">
         <v>1103</v>
-      </c>
-      <c r="B48" s="52" t="s">
-        <v>1104</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="6" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B49" s="52" t="s">
         <v>1105</v>
-      </c>
-      <c r="B49" s="52" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="40" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B50" s="51" t="s">
         <v>1107</v>
-      </c>
-      <c r="B50" s="51" t="s">
-        <v>1108</v>
       </c>
       <c r="C50" s="40"/>
       <c r="D50" s="40"/>
@@ -10283,215 +10280,215 @@
     </row>
     <row r="52">
       <c r="A52" s="40" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="C52" s="40"/>
       <c r="D52" s="40" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="51" t="s">
+        <v>964</v>
+      </c>
+      <c r="B53" s="40" t="s">
         <v>965</v>
-      </c>
-      <c r="B53" s="40" t="s">
-        <v>966</v>
       </c>
       <c r="C53" s="50"/>
       <c r="D53" s="50"/>
       <c r="E53" s="40" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="51" t="s">
+        <v>967</v>
+      </c>
+      <c r="B54" s="40" t="s">
         <v>968</v>
-      </c>
-      <c r="B54" s="40" t="s">
-        <v>969</v>
       </c>
       <c r="C54" s="40"/>
       <c r="D54" s="40" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E54" s="40" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="51" t="s">
+        <v>972</v>
+      </c>
+      <c r="B55" s="40" t="s">
         <v>973</v>
-      </c>
-      <c r="B55" s="40" t="s">
-        <v>974</v>
       </c>
       <c r="C55" s="40"/>
       <c r="D55" s="40" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E55" s="40" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="51" t="s">
+        <v>976</v>
+      </c>
+      <c r="B56" s="40" t="s">
         <v>977</v>
-      </c>
-      <c r="B56" s="40" t="s">
-        <v>978</v>
       </c>
       <c r="C56" s="40"/>
       <c r="D56" s="40" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="E56" s="40" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="51" t="s">
+        <v>980</v>
+      </c>
+      <c r="B57" s="40" t="s">
         <v>981</v>
-      </c>
-      <c r="B57" s="40" t="s">
-        <v>982</v>
       </c>
       <c r="C57" s="40"/>
       <c r="D57" s="40" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="E57" s="40" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="51" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B58" s="40" t="s">
         <v>312</v>
       </c>
       <c r="C58" s="40"/>
       <c r="D58" s="40" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="E58" s="40" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="51" t="s">
+        <v>987</v>
+      </c>
+      <c r="B59" s="40" t="s">
         <v>988</v>
-      </c>
-      <c r="B59" s="40" t="s">
-        <v>989</v>
       </c>
       <c r="C59" s="40"/>
       <c r="D59" s="40" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E59" s="40" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="51" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B60" s="40" t="s">
         <v>510</v>
       </c>
       <c r="C60" s="40"/>
       <c r="D60" s="40" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E60" s="40" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="51" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B61" s="40" t="s">
         <v>470</v>
       </c>
       <c r="C61" s="40"/>
       <c r="D61" s="40" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E61" s="40" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="51" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B62" s="40" t="s">
         <v>514</v>
       </c>
       <c r="C62" s="40"/>
       <c r="D62" s="40" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E62" s="40" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="51" t="s">
+        <v>999</v>
+      </c>
+      <c r="B63" s="40" t="s">
         <v>1000</v>
-      </c>
-      <c r="B63" s="40" t="s">
-        <v>1001</v>
       </c>
       <c r="C63" s="40"/>
       <c r="D63" s="40" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E63" s="40" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="51" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B64" s="40" t="s">
         <v>431</v>
       </c>
       <c r="C64" s="40"/>
       <c r="D64" s="40" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E64" s="40" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="51" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B65" s="40" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="C65" s="40"/>
       <c r="D65" s="40" t="s">
         <v>431</v>
       </c>
       <c r="E65" s="40" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="51" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B66" s="40" t="s">
         <v>404</v>
@@ -10501,12 +10498,12 @@
         <v>431</v>
       </c>
       <c r="E66" s="40" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="51" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B67" s="40" t="s">
         <v>424</v>
@@ -10521,22 +10518,22 @@
     </row>
     <row r="68">
       <c r="A68" s="51" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B68" s="40" t="s">
         <v>1015</v>
-      </c>
-      <c r="B68" s="40" t="s">
-        <v>1016</v>
       </c>
       <c r="C68" s="40"/>
       <c r="D68" s="40" t="s">
         <v>404</v>
       </c>
       <c r="E68" s="40" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="51" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B69" s="40" t="s">
         <v>427</v>
@@ -10546,12 +10543,12 @@
         <v>404</v>
       </c>
       <c r="E69" s="40" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="51" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B70" s="40" t="s">
         <v>438</v>
@@ -10561,12 +10558,12 @@
         <v>404</v>
       </c>
       <c r="E70" s="40" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="51" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B71" s="40" t="s">
         <v>441</v>
@@ -10576,12 +10573,12 @@
         <v>404</v>
       </c>
       <c r="E71" s="40" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="51" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B72" s="40" t="s">
         <v>444</v>
@@ -10591,12 +10588,12 @@
         <v>404</v>
       </c>
       <c r="E72" s="40" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="51" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B73" s="40" t="s">
         <v>447</v>
@@ -10606,42 +10603,42 @@
         <v>404</v>
       </c>
       <c r="E73" s="40" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="51" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B74" s="40" t="s">
         <v>47</v>
       </c>
       <c r="C74" s="40"/>
       <c r="D74" s="40" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E74" s="40" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="51" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="C75" s="40"/>
       <c r="D75" s="40" t="s">
         <v>47</v>
       </c>
       <c r="E75" s="40" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="51" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B76" s="40" t="s">
         <v>401</v>
@@ -10656,7 +10653,7 @@
     </row>
     <row r="77">
       <c r="A77" s="51" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B77" s="40" t="s">
         <v>209</v>
@@ -10664,12 +10661,12 @@
       <c r="C77" s="50"/>
       <c r="D77" s="50"/>
       <c r="E77" s="40" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="51" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B78" s="40" t="s">
         <v>219</v>
@@ -10679,30 +10676,30 @@
         <v>209</v>
       </c>
       <c r="E78" s="40" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="51" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B79" s="40" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C79" s="40"/>
       <c r="D79" s="40" t="s">
         <v>219</v>
       </c>
       <c r="E79" s="40" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="51" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B80" s="40" t="s">
         <v>1049</v>
-      </c>
-      <c r="B80" s="40" t="s">
-        <v>1050</v>
       </c>
       <c r="C80" s="40"/>
       <c r="D80" s="40" t="s">
@@ -10714,7 +10711,7 @@
     </row>
     <row r="81">
       <c r="A81" s="51" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B81" s="40" t="s">
         <v>234</v>
@@ -10724,42 +10721,42 @@
         <v>209</v>
       </c>
       <c r="E81" s="40" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="51" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B82" s="40" t="s">
         <v>1055</v>
-      </c>
-      <c r="B82" s="40" t="s">
-        <v>1056</v>
       </c>
       <c r="C82" s="40"/>
       <c r="D82" s="40" t="s">
         <v>234</v>
       </c>
       <c r="E82" s="40" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="51" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B83" s="40" t="s">
         <v>1059</v>
-      </c>
-      <c r="B83" s="40" t="s">
-        <v>1060</v>
       </c>
       <c r="C83" s="40"/>
       <c r="D83" s="40" t="s">
         <v>234</v>
       </c>
       <c r="E83" s="40" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="51" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B84" s="40" t="s">
         <v>237</v>
@@ -10769,42 +10766,42 @@
         <v>209</v>
       </c>
       <c r="E84" s="40" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="51" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B85" s="40" t="s">
         <v>1066</v>
-      </c>
-      <c r="B85" s="40" t="s">
-        <v>1067</v>
       </c>
       <c r="C85" s="40"/>
       <c r="D85" s="40" t="s">
         <v>209</v>
       </c>
       <c r="E85" s="40" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="51" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B86" s="40" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C86" s="40"/>
       <c r="D86" s="40" t="s">
         <v>209</v>
       </c>
       <c r="E86" s="40" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="51" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B87" s="40" t="s">
         <v>226</v>
@@ -10814,115 +10811,115 @@
         <v>209</v>
       </c>
       <c r="E87" s="40" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="51" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B88" s="40" t="s">
         <v>1077</v>
-      </c>
-      <c r="B88" s="40" t="s">
-        <v>1078</v>
       </c>
       <c r="C88" s="50"/>
       <c r="D88" s="50"/>
       <c r="E88" s="40" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="51" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B89" s="40" t="s">
         <v>1080</v>
-      </c>
-      <c r="B89" s="40" t="s">
-        <v>1081</v>
       </c>
       <c r="C89" s="40"/>
       <c r="D89" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E89" s="40" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="51" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B90" s="40" t="s">
         <v>133</v>
       </c>
       <c r="C90" s="40"/>
       <c r="D90" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E90" s="40" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="51" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B91" s="40" t="s">
         <v>100</v>
       </c>
       <c r="C91" s="40"/>
       <c r="D91" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E91" s="40" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="51" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B92" s="40" t="s">
         <v>137</v>
       </c>
       <c r="C92" s="40"/>
       <c r="D92" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E92" s="40" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="51" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B93" s="40" t="s">
         <v>139</v>
       </c>
       <c r="C93" s="40"/>
       <c r="D93" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E93" s="40" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="51" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B94" s="40" t="s">
         <v>142</v>
       </c>
       <c r="C94" s="40"/>
       <c r="D94" s="40" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E94" s="40" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="51" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B95" s="40" t="s">
         <v>145</v>
@@ -10932,7 +10929,7 @@
         <v>139</v>
       </c>
       <c r="E95" s="40" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refine definitions in AI and DPV
- refined definitions for `ai:HumanIdentification` and
  `dpv:Data...Assessment` concepts (phrasing)
- fixed typo in `ai:HeuristicProgramming`
- added concept `ai:TransparencyRisk`

Co-authored-by: Delaram Golpayegani <sgolpays@tcd.ie>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ai.xlsx
+++ b/code/vocab_csv/ai.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2754" uniqueCount="1146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="1149">
   <si>
     <t>Term</t>
   </si>
@@ -1070,7 +1070,7 @@
     <t>Heuristic Programming</t>
   </si>
   <si>
-    <t>Pprogramming approach designed to tackle problems for which there lacks a systematic or optimized approach, frequently used in expert systems</t>
+    <t>Programming approach designed to tackle problems for which there lacks a systematic or optimized approach, frequently used in expert systems</t>
   </si>
   <si>
     <t>ai:RuleBasedTechnique</t>
@@ -1166,7 +1166,7 @@
     <t>Human Identification</t>
   </si>
   <si>
-    <t>Capability of a system that aims to identify a human whether at an individual or group level</t>
+    <t>Capability of a system that identifies a human whether at an individual or group level</t>
   </si>
   <si>
     <t>ai:HumanOrientedCapability</t>
@@ -3064,13 +3064,22 @@
     <t>ai:ModelInteractionBias</t>
   </si>
   <si>
+    <t>TransparencyRisk</t>
+  </si>
+  <si>
+    <t>Transparency Risk</t>
+  </si>
+  <si>
+    <t>Risk that an AI's design, performance, outputs, or other characteristics are not sufficiently transparent</t>
+  </si>
+  <si>
     <t>ExplainabilityRisk</t>
   </si>
   <si>
     <t>Explainability Risk</t>
   </si>
   <si>
-    <t>Risk that an AI system’s decisions or behaviors cannot be adequately understood, interpreted, or justified by relevant stakeholders.</t>
+    <t>Risk that an AI's decisions or behaviors cannot be adequately understood, interpreted, or justified by relevant stakeholders.</t>
   </si>
   <si>
     <t>ModelPoisoning</t>
@@ -3740,7 +3749,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3886,6 +3895,9 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -9248,10 +9260,10 @@
       <c r="A83" s="6" t="s">
         <v>978</v>
       </c>
-      <c r="B83" s="42" t="s">
+      <c r="B83" s="50" t="s">
         <v>979</v>
       </c>
-      <c r="C83" s="42" t="s">
+      <c r="C83" s="50" t="s">
         <v>980</v>
       </c>
       <c r="D83" s="7"/>
@@ -9296,38 +9308,70 @@
       <c r="AG83" s="7"/>
       <c r="AH83" s="7"/>
     </row>
-    <row r="85">
-      <c r="A85" s="27" t="s">
+    <row r="84">
+      <c r="A84" s="6" t="s">
         <v>981</v>
       </c>
-      <c r="B85" s="26" t="s">
+      <c r="B84" s="42" t="s">
         <v>982</v>
       </c>
-      <c r="C85" s="42" t="s">
+      <c r="C84" s="50" t="s">
         <v>983</v>
       </c>
-      <c r="D85" s="26" t="s">
-        <v>984</v>
-      </c>
-      <c r="E85" s="26"/>
-      <c r="F85" s="26"/>
-      <c r="G85" s="26"/>
-      <c r="H85" s="26"/>
-      <c r="I85" s="26"/>
-      <c r="J85" s="26" t="s">
-        <v>985</v>
-      </c>
+      <c r="D84" s="7"/>
+      <c r="E84" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="F84" s="7"/>
+      <c r="G84" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="H84" s="7"/>
+      <c r="I84" s="7"/>
+      <c r="J84" s="7"/>
+      <c r="K84" s="7"/>
+      <c r="L84" s="7"/>
+      <c r="M84" s="9">
+        <v>46062.0</v>
+      </c>
+      <c r="N84" s="7"/>
+      <c r="O84" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P84" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q84" s="7"/>
+      <c r="R84" s="7"/>
+      <c r="S84" s="7"/>
+      <c r="T84" s="7"/>
+      <c r="U84" s="7"/>
+      <c r="V84" s="7"/>
+      <c r="W84" s="7"/>
+      <c r="X84" s="7"/>
+      <c r="Y84" s="7"/>
+      <c r="Z84" s="7"/>
+      <c r="AA84" s="7"/>
+      <c r="AB84" s="7"/>
+      <c r="AC84" s="7"/>
+      <c r="AD84" s="7"/>
+      <c r="AE84" s="7"/>
+      <c r="AF84" s="7"/>
+      <c r="AG84" s="7"/>
+      <c r="AH84" s="7"/>
     </row>
     <row r="86">
       <c r="A86" s="27" t="s">
+        <v>984</v>
+      </c>
+      <c r="B86" s="26" t="s">
+        <v>985</v>
+      </c>
+      <c r="C86" s="42" t="s">
         <v>986</v>
       </c>
-      <c r="B86" s="26" t="s">
+      <c r="D86" s="26" t="s">
         <v>987</v>
-      </c>
-      <c r="C86" s="26"/>
-      <c r="D86" s="26" t="s">
-        <v>984</v>
       </c>
       <c r="E86" s="26"/>
       <c r="F86" s="26"/>
@@ -9335,46 +9379,66 @@
       <c r="H86" s="26"/>
       <c r="I86" s="26"/>
       <c r="J86" s="26" t="s">
-        <v>985</v>
+        <v>988</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="27" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C87" s="26"/>
-      <c r="D87" s="26"/>
+      <c r="D87" s="26" t="s">
+        <v>987</v>
+      </c>
       <c r="E87" s="26"/>
       <c r="F87" s="26"/>
-      <c r="G87" s="27" t="s">
-        <v>745</v>
-      </c>
+      <c r="G87" s="26"/>
       <c r="H87" s="26"/>
       <c r="I87" s="26"/>
       <c r="J87" s="26" t="s">
-        <v>985</v>
+        <v>988</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="27" t="s">
+        <v>991</v>
+      </c>
+      <c r="B88" s="26" t="s">
+        <v>992</v>
+      </c>
+      <c r="C88" s="26"/>
+      <c r="D88" s="26"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="26"/>
+      <c r="G88" s="27" t="s">
+        <v>745</v>
+      </c>
+      <c r="H88" s="26"/>
+      <c r="I88" s="26"/>
+      <c r="J88" s="26" t="s">
+        <v>988</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A66:AF81 E83">
+  <conditionalFormatting sqref="A66:AF81 E83:E84">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M66="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A66:AB81 E83">
+  <conditionalFormatting sqref="A66:AB81 E83:E84">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>$M66="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A66:AB81 E83">
+  <conditionalFormatting sqref="A66:AB81 E83:E84">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M66="changed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A66:AF81 E83">
+  <conditionalFormatting sqref="A66:AF81 E83:E84">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M66="deprecated"</formula>
     </cfRule>
@@ -9399,22 +9463,22 @@
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D65 AE2:AF65 AG2:AH139 A3:C65 E3:E139 F3:AD65 A82:D139 F82:AF139">
+  <conditionalFormatting sqref="D2:D65 AE2:AF65 AG2:AH140 A3:C65 E3:E140 F3:AD65 A82:D140 F82:AF140">
     <cfRule type="expression" dxfId="0" priority="9">
       <formula>$O2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D65 A3:C65 E3:E115 F3:AD65 A82:D115 F82:AD115">
+  <conditionalFormatting sqref="D2:D65 A3:C65 E3:E116 F3:AD65 A82:D116 F82:AD116">
     <cfRule type="expression" dxfId="1" priority="10">
       <formula>$O2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D65 A3:C65 E3:E115 F3:AD65 A82:D115 F82:AD115">
+  <conditionalFormatting sqref="D2:D65 A3:C65 E3:E116 F3:AD65 A82:D116 F82:AD116">
     <cfRule type="expression" dxfId="2" priority="11">
       <formula>$O2="changed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2 O3:Q65 E4:E139 A5:D65 F5:N65 R5:AF65 AG5:AH139 A82:D139 F82:AF139">
+  <conditionalFormatting sqref="D2 O3:Q65 E4:E140 A5:D65 F5:N65 R5:AF65 AG5:AH140 A82:D140 F82:AF140">
     <cfRule type="expression" dxfId="3" priority="12">
       <formula>$O2="deprecated"</formula>
     </cfRule>
@@ -9447,57 +9511,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="40" t="s">
-        <v>990</v>
+        <v>993</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>992</v>
+        <v>995</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>993</v>
+        <v>996</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>994</v>
+        <v>997</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>995</v>
+        <v>998</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>996</v>
+        <v>999</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="50" t="s">
-        <v>997</v>
-      </c>
-      <c r="B2" s="51" t="s">
-        <v>998</v>
+      <c r="A2" s="51" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>1001</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>999</v>
-      </c>
-      <c r="D2" s="52"/>
+        <v>1002</v>
+      </c>
+      <c r="D2" s="53"/>
       <c r="E2" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="53" t="s">
-        <v>1000</v>
+      <c r="A3" s="54" t="s">
+        <v>1003</v>
       </c>
       <c r="B3" s="40" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D3" s="40" t="s">
         <v>1001</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>1002</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>998</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>85</v>
@@ -9506,24 +9570,24 @@
         <v>214</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>1004</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="53" t="s">
-        <v>1005</v>
+      <c r="A4" s="54" t="s">
+        <v>1008</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>1007</v>
+        <v>1010</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>85</v>
@@ -9532,21 +9596,21 @@
         <v>309</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="54" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D5" s="40" t="s">
         <v>1009</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>1010</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>1011</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>1006</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>85</v>
@@ -9555,24 +9619,24 @@
         <v>85</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>1012</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="54" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D6" s="40" t="s">
         <v>1013</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>1014</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>1015</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>1010</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>85</v>
@@ -9581,47 +9645,47 @@
         <v>85</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>1016</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="53" t="s">
-        <v>1017</v>
+      <c r="A7" s="54" t="s">
+        <v>1020</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>311</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>1018</v>
+        <v>1021</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>85</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>1019</v>
+        <v>1022</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="53" t="s">
-        <v>1020</v>
+      <c r="A8" s="54" t="s">
+        <v>1023</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>81</v>
@@ -9630,24 +9694,24 @@
         <v>475</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="53" t="s">
-        <v>1023</v>
+      <c r="A9" s="54" t="s">
+        <v>1026</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>513</v>
       </c>
       <c r="C9" s="40" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D9" s="40" t="s">
         <v>1024</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>1021</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>81</v>
@@ -9656,47 +9720,47 @@
         <v>81</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>1025</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="53" t="s">
-        <v>1026</v>
+      <c r="A10" s="54" t="s">
+        <v>1029</v>
       </c>
       <c r="B10" s="40" t="s">
         <v>473</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>1027</v>
+        <v>1030</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>81</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>1028</v>
+        <v>1031</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="53" t="s">
-        <v>1029</v>
+      <c r="A11" s="54" t="s">
+        <v>1032</v>
       </c>
       <c r="B11" s="40" t="s">
         <v>517</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>1030</v>
+        <v>1033</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>81</v>
@@ -9705,24 +9769,24 @@
         <v>81</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>1031</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="53" t="s">
-        <v>1032</v>
+      <c r="A12" s="54" t="s">
+        <v>1035</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>1033</v>
+        <v>1036</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>1034</v>
+        <v>1037</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>81</v>
@@ -9731,24 +9795,24 @@
         <v>81</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>1035</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="53" t="s">
-        <v>1036</v>
+      <c r="A13" s="54" t="s">
+        <v>1039</v>
       </c>
       <c r="B13" s="40" t="s">
         <v>434</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>1037</v>
+        <v>1040</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>81</v>
@@ -9757,21 +9821,21 @@
         <v>425</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>1038</v>
+        <v>1041</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>1039</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="53" t="s">
-        <v>1040</v>
+      <c r="A14" s="54" t="s">
+        <v>1043</v>
       </c>
       <c r="B14" s="40" t="s">
         <v>437</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>1041</v>
+        <v>1044</v>
       </c>
       <c r="D14" s="40" t="s">
         <v>434</v>
@@ -9783,21 +9847,21 @@
         <v>81</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>1042</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="53" t="s">
-        <v>1043</v>
+      <c r="A15" s="54" t="s">
+        <v>1046</v>
       </c>
       <c r="B15" s="40" t="s">
         <v>407</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>1044</v>
+        <v>1047</v>
       </c>
       <c r="D15" s="40" t="s">
         <v>434</v>
@@ -9809,12 +9873,12 @@
         <v>425</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="53" t="s">
-        <v>1045</v>
+      <c r="A16" s="54" t="s">
+        <v>1048</v>
       </c>
       <c r="B16" s="40" t="s">
         <v>427</v>
@@ -9829,21 +9893,21 @@
         <v>81</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>1046</v>
+        <v>1049</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>1038</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="53" t="s">
-        <v>1047</v>
+      <c r="A17" s="54" t="s">
+        <v>1050</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>1048</v>
+        <v>1051</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>1049</v>
+        <v>1052</v>
       </c>
       <c r="D17" s="40" t="s">
         <v>407</v>
@@ -9852,21 +9916,21 @@
         <v>81</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>1050</v>
+        <v>1053</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="53" t="s">
-        <v>1051</v>
+      <c r="A18" s="54" t="s">
+        <v>1054</v>
       </c>
       <c r="B18" s="40" t="s">
         <v>430</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>1052</v>
+        <v>1055</v>
       </c>
       <c r="D18" s="40" t="s">
         <v>407</v>
@@ -9875,21 +9939,21 @@
         <v>81</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>1053</v>
+        <v>1056</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="53" t="s">
-        <v>1054</v>
+      <c r="A19" s="54" t="s">
+        <v>1057</v>
       </c>
       <c r="B19" s="40" t="s">
         <v>441</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>1055</v>
+        <v>1058</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>407</v>
@@ -9901,21 +9965,21 @@
         <v>81</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>1056</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="53" t="s">
-        <v>1057</v>
+      <c r="A20" s="54" t="s">
+        <v>1060</v>
       </c>
       <c r="B20" s="40" t="s">
         <v>444</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>1058</v>
+        <v>1061</v>
       </c>
       <c r="D20" s="40" t="s">
         <v>407</v>
@@ -9924,21 +9988,21 @@
         <v>81</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>1046</v>
+        <v>1049</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="53" t="s">
-        <v>1059</v>
+      <c r="A21" s="54" t="s">
+        <v>1062</v>
       </c>
       <c r="B21" s="40" t="s">
         <v>447</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
       <c r="D21" s="40" t="s">
         <v>407</v>
@@ -9950,21 +10014,21 @@
         <v>81</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>1061</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="53" t="s">
-        <v>1062</v>
+      <c r="A22" s="54" t="s">
+        <v>1065</v>
       </c>
       <c r="B22" s="40" t="s">
         <v>450</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>1063</v>
+        <v>1066</v>
       </c>
       <c r="D22" s="40" t="s">
         <v>407</v>
@@ -9973,27 +10037,27 @@
         <v>81</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>1053</v>
+        <v>1056</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>1038</v>
+        <v>1041</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>1064</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="53" t="s">
-        <v>1065</v>
+      <c r="A23" s="54" t="s">
+        <v>1068</v>
       </c>
       <c r="B23" s="40" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>1066</v>
+        <v>1069</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>81</v>
@@ -10002,21 +10066,21 @@
         <v>81</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>1067</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="53" t="s">
-        <v>1068</v>
+      <c r="A24" s="54" t="s">
+        <v>1071</v>
       </c>
       <c r="B24" s="40" t="s">
         <v>162</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
       <c r="D24" s="40" t="s">
         <v>47</v>
@@ -10028,15 +10092,15 @@
         <v>72</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="53" t="s">
-        <v>1071</v>
+      <c r="A25" s="54" t="s">
+        <v>1074</v>
       </c>
       <c r="B25" s="40" t="s">
         <v>404</v>
@@ -10054,35 +10118,35 @@
         <v>357</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>1072</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="50" t="s">
-        <v>1073</v>
-      </c>
-      <c r="B27" s="51" t="s">
+      <c r="A27" s="51" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B27" s="52" t="s">
         <v>208</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>1074</v>
+        <v>1077</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="53" t="s">
-        <v>1075</v>
+      <c r="A28" s="54" t="s">
+        <v>1078</v>
       </c>
       <c r="B28" s="40" t="s">
         <v>218</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>1076</v>
+        <v>1079</v>
       </c>
       <c r="D28" s="40" t="s">
         <v>208</v>
@@ -10094,18 +10158,18 @@
         <v>223</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="53" t="s">
-        <v>1077</v>
+      <c r="A29" s="54" t="s">
+        <v>1080</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>1078</v>
+        <v>1081</v>
       </c>
       <c r="C29" s="40" t="s">
-        <v>1079</v>
+        <v>1082</v>
       </c>
       <c r="D29" s="40" t="s">
         <v>218</v>
@@ -10117,18 +10181,18 @@
         <v>261</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>1080</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="53" t="s">
-        <v>1081</v>
+      <c r="A30" s="54" t="s">
+        <v>1084</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>1082</v>
+        <v>1085</v>
       </c>
       <c r="C30" s="40" t="s">
         <v>222</v>
@@ -10143,21 +10207,21 @@
         <v>223</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="53" t="s">
-        <v>1084</v>
+      <c r="A31" s="54" t="s">
+        <v>1087</v>
       </c>
       <c r="B31" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C31" s="40" t="s">
-        <v>1085</v>
+        <v>1088</v>
       </c>
       <c r="D31" s="40" t="s">
         <v>208</v>
@@ -10166,18 +10230,18 @@
         <v>85</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>1086</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="53" t="s">
-        <v>1087</v>
+      <c r="A32" s="54" t="s">
+        <v>1090</v>
       </c>
       <c r="B32" s="40" t="s">
-        <v>1088</v>
+        <v>1091</v>
       </c>
       <c r="C32" s="40" t="s">
-        <v>1089</v>
+        <v>1092</v>
       </c>
       <c r="D32" s="40" t="s">
         <v>233</v>
@@ -10186,18 +10250,18 @@
         <v>85</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>1090</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="53" t="s">
-        <v>1091</v>
+      <c r="A33" s="54" t="s">
+        <v>1094</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>1093</v>
+        <v>1096</v>
       </c>
       <c r="D33" s="40" t="s">
         <v>233</v>
@@ -10206,18 +10270,18 @@
         <v>85</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>1094</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="53" t="s">
-        <v>1095</v>
+      <c r="A34" s="54" t="s">
+        <v>1098</v>
       </c>
       <c r="B34" s="40" t="s">
         <v>236</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>1096</v>
+        <v>1099</v>
       </c>
       <c r="D34" s="40" t="s">
         <v>208</v>
@@ -10226,18 +10290,18 @@
         <v>85</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>1097</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="53" t="s">
-        <v>1098</v>
+      <c r="A35" s="54" t="s">
+        <v>1101</v>
       </c>
       <c r="B35" s="40" t="s">
-        <v>1099</v>
+        <v>1102</v>
       </c>
       <c r="C35" s="40" t="s">
-        <v>1100</v>
+        <v>1103</v>
       </c>
       <c r="D35" s="40" t="s">
         <v>208</v>
@@ -10246,21 +10310,21 @@
         <v>85</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>1101</v>
+        <v>1104</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>1038</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="53" t="s">
-        <v>1102</v>
+      <c r="A36" s="54" t="s">
+        <v>1105</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>1103</v>
+        <v>1106</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
       <c r="D36" s="40" t="s">
         <v>208</v>
@@ -10272,21 +10336,21 @@
         <v>214</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="53" t="s">
-        <v>1106</v>
+      <c r="A37" s="54" t="s">
+        <v>1109</v>
       </c>
       <c r="B37" s="40" t="s">
         <v>225</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
       <c r="D37" s="40" t="s">
         <v>208</v>
@@ -10295,36 +10359,36 @@
         <v>85</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>1108</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="50" t="s">
-        <v>1109</v>
-      </c>
-      <c r="B39" s="51" t="s">
-        <v>1110</v>
+      <c r="A39" s="51" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B39" s="52" t="s">
+        <v>1113</v>
       </c>
       <c r="C39" s="40" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D39" s="52"/>
+        <v>1114</v>
+      </c>
+      <c r="D39" s="53"/>
       <c r="E39" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="53" t="s">
-        <v>1112</v>
+      <c r="A40" s="54" t="s">
+        <v>1115</v>
       </c>
       <c r="B40" s="40" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C40" s="40" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D40" s="40" t="s">
         <v>1113</v>
-      </c>
-      <c r="C40" s="40" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D40" s="40" t="s">
-        <v>1110</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>67</v>
@@ -10333,24 +10397,24 @@
         <v>67</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>1115</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="53" t="s">
-        <v>1116</v>
+      <c r="A41" s="54" t="s">
+        <v>1119</v>
       </c>
       <c r="B41" s="40" t="s">
         <v>133</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>1117</v>
+        <v>1120</v>
       </c>
       <c r="D41" s="40" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>67</v>
@@ -10359,50 +10423,50 @@
         <v>67</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>1118</v>
+        <v>1121</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>1119</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="53" t="s">
-        <v>1120</v>
+      <c r="A42" s="54" t="s">
+        <v>1123</v>
       </c>
       <c r="B42" s="40" t="s">
         <v>100</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>1121</v>
+        <v>1124</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>67</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>1122</v>
+        <v>1125</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="53" t="s">
-        <v>1123</v>
+      <c r="A43" s="54" t="s">
+        <v>1126</v>
       </c>
       <c r="B43" s="40" t="s">
         <v>136</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>1124</v>
+        <v>1127</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>67</v>
@@ -10411,24 +10475,24 @@
         <v>67</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>1125</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="53" t="s">
-        <v>1126</v>
+      <c r="A44" s="54" t="s">
+        <v>1129</v>
       </c>
       <c r="B44" s="40" t="s">
         <v>138</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>1127</v>
+        <v>1130</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>67</v>
@@ -10437,24 +10501,24 @@
         <v>117</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>1128</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="53" t="s">
-        <v>1129</v>
+      <c r="A45" s="54" t="s">
+        <v>1132</v>
       </c>
       <c r="B45" s="40" t="s">
         <v>141</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>1130</v>
+        <v>1133</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>67</v>
@@ -10463,24 +10527,24 @@
         <v>67</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>1118</v>
+        <v>1121</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>1131</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="53" t="s">
-        <v>1132</v>
+      <c r="A46" s="54" t="s">
+        <v>1135</v>
       </c>
       <c r="B46" s="40" t="s">
         <v>144</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>1133</v>
+        <v>1136</v>
       </c>
       <c r="D46" s="40" t="s">
         <v>138</v>
@@ -10492,34 +10556,34 @@
         <v>67</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="s">
-        <v>1135</v>
-      </c>
-      <c r="B48" s="54" t="s">
-        <v>1136</v>
+        <v>1138</v>
+      </c>
+      <c r="B48" s="55" t="s">
+        <v>1139</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="6" t="s">
-        <v>1137</v>
-      </c>
-      <c r="B49" s="54" t="s">
-        <v>1138</v>
+        <v>1140</v>
+      </c>
+      <c r="B49" s="55" t="s">
+        <v>1141</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="40" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B50" s="53" t="s">
-        <v>1140</v>
+        <v>1142</v>
+      </c>
+      <c r="B50" s="54" t="s">
+        <v>1143</v>
       </c>
       <c r="C50" s="40"/>
       <c r="D50" s="40"/>
@@ -10532,215 +10596,215 @@
     </row>
     <row r="52">
       <c r="A52" s="40" t="s">
-        <v>1141</v>
+        <v>1144</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
       <c r="C52" s="40"/>
       <c r="D52" s="40" t="s">
-        <v>993</v>
+        <v>996</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>992</v>
+        <v>995</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="53" t="s">
-        <v>997</v>
+      <c r="A53" s="54" t="s">
+        <v>1000</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>998</v>
-      </c>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
+        <v>1001</v>
+      </c>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
       <c r="E53" s="40" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="53" t="s">
-        <v>1000</v>
+      <c r="A54" s="54" t="s">
+        <v>1003</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c r="C54" s="40"/>
       <c r="D54" s="40" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="E54" s="40" t="s">
-        <v>1002</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="53" t="s">
-        <v>1005</v>
+      <c r="A55" s="54" t="s">
+        <v>1008</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="C55" s="40"/>
       <c r="D55" s="40" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="E55" s="40" t="s">
-        <v>1007</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="53" t="s">
-        <v>1009</v>
+      <c r="A56" s="54" t="s">
+        <v>1012</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>1010</v>
+        <v>1013</v>
       </c>
       <c r="C56" s="40"/>
       <c r="D56" s="40" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="E56" s="40" t="s">
-        <v>1011</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="53" t="s">
-        <v>1013</v>
+      <c r="A57" s="54" t="s">
+        <v>1016</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>1014</v>
+        <v>1017</v>
       </c>
       <c r="C57" s="40"/>
       <c r="D57" s="40" t="s">
-        <v>1010</v>
+        <v>1013</v>
       </c>
       <c r="E57" s="40" t="s">
-        <v>1015</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="53" t="s">
-        <v>1017</v>
+      <c r="A58" s="54" t="s">
+        <v>1020</v>
       </c>
       <c r="B58" s="40" t="s">
         <v>311</v>
       </c>
       <c r="C58" s="40"/>
       <c r="D58" s="40" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="E58" s="40" t="s">
-        <v>1018</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="53" t="s">
-        <v>1020</v>
+      <c r="A59" s="54" t="s">
+        <v>1023</v>
       </c>
       <c r="B59" s="40" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="C59" s="40"/>
       <c r="D59" s="40" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="E59" s="40" t="s">
-        <v>1022</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="53" t="s">
-        <v>1023</v>
+      <c r="A60" s="54" t="s">
+        <v>1026</v>
       </c>
       <c r="B60" s="40" t="s">
         <v>513</v>
       </c>
       <c r="C60" s="40"/>
       <c r="D60" s="40" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="E60" s="40" t="s">
-        <v>1024</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="53" t="s">
-        <v>1026</v>
+      <c r="A61" s="54" t="s">
+        <v>1029</v>
       </c>
       <c r="B61" s="40" t="s">
         <v>473</v>
       </c>
       <c r="C61" s="40"/>
       <c r="D61" s="40" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="E61" s="40" t="s">
-        <v>1027</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="53" t="s">
-        <v>1029</v>
+      <c r="A62" s="54" t="s">
+        <v>1032</v>
       </c>
       <c r="B62" s="40" t="s">
         <v>517</v>
       </c>
       <c r="C62" s="40"/>
       <c r="D62" s="40" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="E62" s="40" t="s">
-        <v>1030</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="53" t="s">
-        <v>1032</v>
+      <c r="A63" s="54" t="s">
+        <v>1035</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>1033</v>
+        <v>1036</v>
       </c>
       <c r="C63" s="40"/>
       <c r="D63" s="40" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="E63" s="40" t="s">
-        <v>1034</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="53" t="s">
-        <v>1036</v>
+      <c r="A64" s="54" t="s">
+        <v>1039</v>
       </c>
       <c r="B64" s="40" t="s">
         <v>434</v>
       </c>
       <c r="C64" s="40"/>
       <c r="D64" s="40" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="E64" s="40" t="s">
-        <v>1037</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="53" t="s">
-        <v>1040</v>
+      <c r="A65" s="54" t="s">
+        <v>1043</v>
       </c>
       <c r="B65" s="40" t="s">
-        <v>1142</v>
+        <v>1145</v>
       </c>
       <c r="C65" s="40"/>
       <c r="D65" s="40" t="s">
         <v>434</v>
       </c>
       <c r="E65" s="40" t="s">
-        <v>1041</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="53" t="s">
-        <v>1043</v>
+      <c r="A66" s="54" t="s">
+        <v>1046</v>
       </c>
       <c r="B66" s="40" t="s">
         <v>407</v>
@@ -10750,12 +10814,12 @@
         <v>434</v>
       </c>
       <c r="E66" s="40" t="s">
-        <v>1044</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="53" t="s">
-        <v>1045</v>
+      <c r="A67" s="54" t="s">
+        <v>1048</v>
       </c>
       <c r="B67" s="40" t="s">
         <v>427</v>
@@ -10769,23 +10833,23 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="53" t="s">
-        <v>1047</v>
+      <c r="A68" s="54" t="s">
+        <v>1050</v>
       </c>
       <c r="B68" s="40" t="s">
-        <v>1048</v>
+        <v>1051</v>
       </c>
       <c r="C68" s="40"/>
       <c r="D68" s="40" t="s">
         <v>407</v>
       </c>
       <c r="E68" s="40" t="s">
-        <v>1049</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="53" t="s">
-        <v>1051</v>
+      <c r="A69" s="54" t="s">
+        <v>1054</v>
       </c>
       <c r="B69" s="40" t="s">
         <v>430</v>
@@ -10795,12 +10859,12 @@
         <v>407</v>
       </c>
       <c r="E69" s="40" t="s">
-        <v>1052</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="53" t="s">
-        <v>1054</v>
+      <c r="A70" s="54" t="s">
+        <v>1057</v>
       </c>
       <c r="B70" s="40" t="s">
         <v>441</v>
@@ -10810,12 +10874,12 @@
         <v>407</v>
       </c>
       <c r="E70" s="40" t="s">
-        <v>1055</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="53" t="s">
-        <v>1057</v>
+      <c r="A71" s="54" t="s">
+        <v>1060</v>
       </c>
       <c r="B71" s="40" t="s">
         <v>444</v>
@@ -10825,12 +10889,12 @@
         <v>407</v>
       </c>
       <c r="E71" s="40" t="s">
-        <v>1058</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="53" t="s">
-        <v>1059</v>
+      <c r="A72" s="54" t="s">
+        <v>1062</v>
       </c>
       <c r="B72" s="40" t="s">
         <v>447</v>
@@ -10840,12 +10904,12 @@
         <v>407</v>
       </c>
       <c r="E72" s="40" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="53" t="s">
-        <v>1062</v>
+      <c r="A73" s="54" t="s">
+        <v>1065</v>
       </c>
       <c r="B73" s="40" t="s">
         <v>450</v>
@@ -10855,42 +10919,42 @@
         <v>407</v>
       </c>
       <c r="E73" s="40" t="s">
-        <v>1063</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="53" t="s">
-        <v>1065</v>
+      <c r="A74" s="54" t="s">
+        <v>1068</v>
       </c>
       <c r="B74" s="40" t="s">
         <v>47</v>
       </c>
       <c r="C74" s="40"/>
       <c r="D74" s="40" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="E74" s="40" t="s">
-        <v>1066</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="53" t="s">
-        <v>1068</v>
+      <c r="A75" s="54" t="s">
+        <v>1071</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>1143</v>
+        <v>1146</v>
       </c>
       <c r="C75" s="40"/>
       <c r="D75" s="40" t="s">
         <v>47</v>
       </c>
       <c r="E75" s="40" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="53" t="s">
-        <v>1071</v>
+      <c r="A76" s="54" t="s">
+        <v>1074</v>
       </c>
       <c r="B76" s="40" t="s">
         <v>404</v>
@@ -10904,21 +10968,21 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="53" t="s">
-        <v>1073</v>
+      <c r="A77" s="54" t="s">
+        <v>1076</v>
       </c>
       <c r="B77" s="40" t="s">
         <v>208</v>
       </c>
-      <c r="C77" s="52"/>
-      <c r="D77" s="52"/>
+      <c r="C77" s="53"/>
+      <c r="D77" s="53"/>
       <c r="E77" s="40" t="s">
-        <v>1074</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="53" t="s">
-        <v>1075</v>
+      <c r="A78" s="54" t="s">
+        <v>1078</v>
       </c>
       <c r="B78" s="40" t="s">
         <v>218</v>
@@ -10928,30 +10992,30 @@
         <v>208</v>
       </c>
       <c r="E78" s="40" t="s">
-        <v>1076</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="53" t="s">
-        <v>1077</v>
+      <c r="A79" s="54" t="s">
+        <v>1080</v>
       </c>
       <c r="B79" s="40" t="s">
-        <v>1144</v>
+        <v>1147</v>
       </c>
       <c r="C79" s="40"/>
       <c r="D79" s="40" t="s">
         <v>218</v>
       </c>
       <c r="E79" s="40" t="s">
-        <v>1079</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="53" t="s">
-        <v>1081</v>
+      <c r="A80" s="54" t="s">
+        <v>1084</v>
       </c>
       <c r="B80" s="40" t="s">
-        <v>1082</v>
+        <v>1085</v>
       </c>
       <c r="C80" s="40"/>
       <c r="D80" s="40" t="s">
@@ -10962,8 +11026,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="53" t="s">
-        <v>1084</v>
+      <c r="A81" s="54" t="s">
+        <v>1087</v>
       </c>
       <c r="B81" s="40" t="s">
         <v>233</v>
@@ -10973,42 +11037,42 @@
         <v>208</v>
       </c>
       <c r="E81" s="40" t="s">
-        <v>1085</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="53" t="s">
-        <v>1087</v>
+      <c r="A82" s="54" t="s">
+        <v>1090</v>
       </c>
       <c r="B82" s="40" t="s">
-        <v>1088</v>
+        <v>1091</v>
       </c>
       <c r="C82" s="40"/>
       <c r="D82" s="40" t="s">
         <v>233</v>
       </c>
       <c r="E82" s="40" t="s">
-        <v>1089</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="53" t="s">
-        <v>1091</v>
+      <c r="A83" s="54" t="s">
+        <v>1094</v>
       </c>
       <c r="B83" s="40" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
       <c r="C83" s="40"/>
       <c r="D83" s="40" t="s">
         <v>233</v>
       </c>
       <c r="E83" s="40" t="s">
-        <v>1093</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="53" t="s">
-        <v>1095</v>
+      <c r="A84" s="54" t="s">
+        <v>1098</v>
       </c>
       <c r="B84" s="40" t="s">
         <v>236</v>
@@ -11018,42 +11082,42 @@
         <v>208</v>
       </c>
       <c r="E84" s="40" t="s">
-        <v>1096</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="53" t="s">
-        <v>1098</v>
+      <c r="A85" s="54" t="s">
+        <v>1101</v>
       </c>
       <c r="B85" s="40" t="s">
-        <v>1099</v>
+        <v>1102</v>
       </c>
       <c r="C85" s="40"/>
       <c r="D85" s="40" t="s">
         <v>208</v>
       </c>
       <c r="E85" s="40" t="s">
-        <v>1100</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="53" t="s">
-        <v>1102</v>
+      <c r="A86" s="54" t="s">
+        <v>1105</v>
       </c>
       <c r="B86" s="40" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="C86" s="40"/>
       <c r="D86" s="40" t="s">
         <v>208</v>
       </c>
       <c r="E86" s="40" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="53" t="s">
-        <v>1106</v>
+      <c r="A87" s="54" t="s">
+        <v>1109</v>
       </c>
       <c r="B87" s="40" t="s">
         <v>225</v>
@@ -11063,115 +11127,115 @@
         <v>208</v>
       </c>
       <c r="E87" s="40" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="53" t="s">
-        <v>1109</v>
+      <c r="A88" s="54" t="s">
+        <v>1112</v>
       </c>
       <c r="B88" s="40" t="s">
-        <v>1110</v>
-      </c>
-      <c r="C88" s="52"/>
-      <c r="D88" s="52"/>
+        <v>1113</v>
+      </c>
+      <c r="C88" s="53"/>
+      <c r="D88" s="53"/>
       <c r="E88" s="40" t="s">
-        <v>1111</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="53" t="s">
-        <v>1112</v>
+      <c r="A89" s="54" t="s">
+        <v>1115</v>
       </c>
       <c r="B89" s="40" t="s">
-        <v>1113</v>
+        <v>1116</v>
       </c>
       <c r="C89" s="40"/>
       <c r="D89" s="40" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="E89" s="40" t="s">
-        <v>1114</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="53" t="s">
-        <v>1116</v>
+      <c r="A90" s="54" t="s">
+        <v>1119</v>
       </c>
       <c r="B90" s="40" t="s">
         <v>133</v>
       </c>
       <c r="C90" s="40"/>
       <c r="D90" s="40" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="E90" s="40" t="s">
-        <v>1117</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="53" t="s">
-        <v>1120</v>
+      <c r="A91" s="54" t="s">
+        <v>1123</v>
       </c>
       <c r="B91" s="40" t="s">
         <v>100</v>
       </c>
       <c r="C91" s="40"/>
       <c r="D91" s="40" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="E91" s="40" t="s">
-        <v>1121</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="53" t="s">
-        <v>1123</v>
+      <c r="A92" s="54" t="s">
+        <v>1126</v>
       </c>
       <c r="B92" s="40" t="s">
         <v>136</v>
       </c>
       <c r="C92" s="40"/>
       <c r="D92" s="40" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="E92" s="40" t="s">
-        <v>1124</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="53" t="s">
-        <v>1126</v>
+      <c r="A93" s="54" t="s">
+        <v>1129</v>
       </c>
       <c r="B93" s="40" t="s">
         <v>138</v>
       </c>
       <c r="C93" s="40"/>
       <c r="D93" s="40" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="E93" s="40" t="s">
-        <v>1127</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="53" t="s">
-        <v>1129</v>
+      <c r="A94" s="54" t="s">
+        <v>1132</v>
       </c>
       <c r="B94" s="40" t="s">
         <v>141</v>
       </c>
       <c r="C94" s="40"/>
       <c r="D94" s="40" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="E94" s="40" t="s">
-        <v>1130</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="53" t="s">
-        <v>1132</v>
+      <c r="A95" s="54" t="s">
+        <v>1135</v>
       </c>
       <c r="B95" s="40" t="s">
         <v>144</v>
@@ -11181,7 +11245,7 @@
         <v>138</v>
       </c>
       <c r="E95" s="40" t="s">
-        <v>1133</v>
+        <v>1136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>